<commit_message>
added base Poker project
</commit_message>
<xml_diff>
--- a/Prezenta.xlsx
+++ b/Prezenta.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\AlgoritmiFundamentali_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B3D5B6-4289-4A49-8097-046D5D44ADFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3006962-40A6-4AC9-892E-2539089D5FCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Nume Prenume</t>
   </si>
@@ -118,15 +118,6 @@
   </si>
   <si>
     <t>Priala Emil</t>
-  </si>
-  <si>
-    <t>joc</t>
-  </si>
-  <si>
-    <t>FE</t>
-  </si>
-  <si>
-    <t>Votes:</t>
   </si>
 </sst>
 </file>
@@ -309,7 +300,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -326,7 +317,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -622,21 +612,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:S19"/>
+  <dimension ref="B2:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.6640625" customWidth="1"/>
     <col min="2" max="2" width="20.88671875" customWidth="1"/>
-    <col min="18" max="18" width="6.21875" customWidth="1"/>
-    <col min="19" max="19" width="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -685,14 +673,8 @@
       <c r="Q2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="2:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B3" s="10" t="s">
         <v>22</v>
       </c>
@@ -713,15 +695,11 @@
       <c r="O3" s="3"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="11">
-        <f>C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
-        <v>1</v>
-      </c>
-      <c r="R3" s="2"/>
-      <c r="S3" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.3">
+        <f t="shared" ref="Q3:Q17" si="0">C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B4" s="10" t="s">
         <v>21</v>
       </c>
@@ -730,15 +708,11 @@
       </c>
       <c r="P4" s="6"/>
       <c r="Q4" s="11">
-        <f>C4+D4+E4+F4+G4+H4+I4+J4+K4+L4+M4+N4+O4+P4</f>
-        <v>1</v>
-      </c>
-      <c r="R4" s="5"/>
-      <c r="S4" s="6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B5" s="10" t="s">
         <v>16</v>
       </c>
@@ -747,46 +721,24 @@
       </c>
       <c r="P5" s="6"/>
       <c r="Q5" s="11">
-        <f>C5+D5+E5+F5+G5+H5+I5+J5+K5+L5+M5+N5+O5+P5</f>
-        <v>1</v>
-      </c>
-      <c r="R5" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="S5" s="6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B6" s="10" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
       <c r="P6" s="6"/>
       <c r="Q6" s="11">
-        <f>C6+D6+E6+F6+G6+H6+I6+J6+K6+L6+M6+N6+O6+P6</f>
-        <v>1</v>
-      </c>
-      <c r="R6" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="S6" s="6"/>
-    </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B7" s="10" t="s">
         <v>26</v>
       </c>
@@ -795,17 +747,11 @@
       </c>
       <c r="P7" s="6"/>
       <c r="Q7" s="11">
-        <f>C7+D7+E7+F7+G7+H7+I7+J7+K7+L7+M7+N7+O7+P7</f>
-        <v>1</v>
-      </c>
-      <c r="R7" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="S7" s="6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B8" s="10" t="s">
         <v>29</v>
       </c>
@@ -814,15 +760,11 @@
       </c>
       <c r="P8" s="6"/>
       <c r="Q8" s="11">
-        <f>C8+D8+E8+F8+G8+H8+I8+J8+K8+L8+M8+N8+O8+P8</f>
-        <v>1</v>
-      </c>
-      <c r="R8" s="5"/>
-      <c r="S8" s="6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
         <v>27</v>
       </c>
@@ -831,15 +773,11 @@
       </c>
       <c r="P9" s="6"/>
       <c r="Q9" s="11">
-        <f>C9+D9+E9+F9+G9+H9+I9+J9+K9+L9+M9+N9+O9+P9</f>
-        <v>1</v>
-      </c>
-      <c r="R9" s="5"/>
-      <c r="S9" s="6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B10" s="10" t="s">
         <v>25</v>
       </c>
@@ -848,15 +786,11 @@
       </c>
       <c r="P10" s="6"/>
       <c r="Q10" s="11">
-        <f>C10+D10+E10+F10+G10+H10+I10+J10+K10+L10+M10+N10+O10+P10</f>
-        <v>1</v>
-      </c>
-      <c r="R10" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="S10" s="6"/>
-    </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B11" s="10" t="s">
         <v>24</v>
       </c>
@@ -865,15 +799,11 @@
       </c>
       <c r="P11" s="6"/>
       <c r="Q11" s="11">
-        <f>C11+D11+E11+F11+G11+H11+I11+J11+K11+L11+M11+N11+O11+P11</f>
-        <v>1</v>
-      </c>
-      <c r="R11" s="5"/>
-      <c r="S11" s="6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B12" s="10" t="s">
         <v>20</v>
       </c>
@@ -882,15 +812,11 @@
       </c>
       <c r="P12" s="6"/>
       <c r="Q12" s="11">
-        <f>C12+D12+E12+F12+G12+H12+I12+J12+K12+L12+M12+N12+O12+P12</f>
-        <v>1</v>
-      </c>
-      <c r="R12" s="5"/>
-      <c r="S12" s="6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B13" s="10" t="s">
         <v>19</v>
       </c>
@@ -899,48 +825,24 @@
       </c>
       <c r="P13" s="6"/>
       <c r="Q13" s="11">
-        <f>C13+D13+E13+F13+G13+H13+I13+J13+K13+L13+M13+N13+O13+P13</f>
-        <v>1</v>
-      </c>
-      <c r="R13" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="S13" s="6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B14" s="10" t="s">
         <v>30</v>
       </c>
       <c r="C14" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
-      <c r="O14" s="12"/>
       <c r="P14" s="6"/>
       <c r="Q14" s="11">
-        <f>C14+D14+E14+F14+G14+H14+I14+J14+K14+L14+M14+N14+O14+P14</f>
-        <v>1</v>
-      </c>
-      <c r="R14" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="S14" s="6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B15" s="10" t="s">
         <v>18</v>
       </c>
@@ -949,17 +851,11 @@
       </c>
       <c r="P15" s="6"/>
       <c r="Q15" s="11">
-        <f>C15+D15+E15+F15+G15+H15+I15+J15+K15+L15+M15+N15+O15+P15</f>
-        <v>1</v>
-      </c>
-      <c r="R15" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="S15" s="6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B16" s="10" t="s">
         <v>28</v>
       </c>
@@ -968,15 +864,11 @@
       </c>
       <c r="P16" s="6"/>
       <c r="Q16" s="11">
-        <f>C16+D16+E16+F16+G16+H16+I16+J16+K16+L16+M16+N16+O16+P16</f>
-        <v>1</v>
-      </c>
-      <c r="R16" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="S16" s="6"/>
-    </row>
-    <row r="17" spans="2:19" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B17" s="10" t="s">
         <v>23</v>
       </c>
@@ -997,31 +889,12 @@
       <c r="O17" s="8"/>
       <c r="P17" s="9"/>
       <c r="Q17" s="11">
-        <f>C17+D17+E17+F17+G17+H17+I17+J17+K17+L17+M17+N17+O17+P17</f>
-        <v>1</v>
-      </c>
-      <c r="R17" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="S17" s="9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="Q19" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="R19" s="11">
-        <f>R3+R4+R5+R6+R7+R8+R9+R10+R11+R12+R13+R14+R15+R16+R17+R18</f>
-        <v>9</v>
-      </c>
-      <c r="S19" s="11">
-        <f>S3+S4+S5+S6+S7+S8+S9+S10+S11+S12+S13+S14+S15+S16+S17+S18</f>
-        <v>12</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:S17">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:Q17">
     <sortCondition ref="B3:B17"/>
   </sortState>
   <conditionalFormatting sqref="Q3:Q17">
@@ -1029,11 +902,6 @@
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R19:S19">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
-      <formula>4</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Laborator 07.03.2023 - Jocul X si O
</commit_message>
<xml_diff>
--- a/Prezenta.xlsx
+++ b/Prezenta.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\AlgoritmiFundamentali_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3006962-40A6-4AC9-892E-2539089D5FCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BAC79EE-4D5D-4CA5-AD40-5A572BF039C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>Nume Prenume</t>
   </si>
@@ -118,6 +118,54 @@
   </si>
   <si>
     <t>Priala Emil</t>
+  </si>
+  <si>
+    <t>Turani Narcis</t>
+  </si>
+  <si>
+    <t>Szarkozi Alex</t>
+  </si>
+  <si>
+    <t>Taichis Vasile</t>
+  </si>
+  <si>
+    <t>Porumb Ionut</t>
+  </si>
+  <si>
+    <t>Rulea Bogdan</t>
+  </si>
+  <si>
+    <t>Covaci Raul</t>
+  </si>
+  <si>
+    <t>Juhasz Szebastian</t>
+  </si>
+  <si>
+    <t>Vereabcean Nicoleta</t>
+  </si>
+  <si>
+    <t>Uzum Mara</t>
+  </si>
+  <si>
+    <t>Toie Patricia</t>
+  </si>
+  <si>
+    <t>Luca Alin</t>
+  </si>
+  <si>
+    <t>Vaida David</t>
+  </si>
+  <si>
+    <t>Sule Zsolt</t>
+  </si>
+  <si>
+    <t>Mura Mihai</t>
+  </si>
+  <si>
+    <t>Stroiescu Raul</t>
+  </si>
+  <si>
+    <t>Lucuta Stefan</t>
   </si>
 </sst>
 </file>
@@ -300,7 +348,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -317,18 +365,15 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -612,10 +657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:Q17"/>
+  <dimension ref="B2:Q33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T32" sqref="T32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -676,12 +721,12 @@
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B3" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D3" s="3"/>
+        <v>36</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -695,15 +740,16 @@
       <c r="O3" s="3"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="11">
-        <f t="shared" ref="Q3:Q17" si="0">C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
+        <f t="shared" ref="Q3:Q33" si="0">C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B4" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="5" t="b">
+        <v>37</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" t="b">
         <v>1</v>
       </c>
       <c r="P4" s="6"/>
@@ -714,9 +760,10 @@
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B5" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="5" t="b">
+        <v>41</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" t="b">
         <v>1</v>
       </c>
       <c r="P5" s="6"/>
@@ -727,9 +774,10 @@
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B6" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="5" t="b">
+        <v>46</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" t="b">
         <v>1</v>
       </c>
       <c r="P6" s="6"/>
@@ -740,9 +788,10 @@
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B7" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="5" t="b">
+        <v>44</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" t="b">
         <v>1</v>
       </c>
       <c r="P7" s="6"/>
@@ -753,72 +802,87 @@
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B8" s="10" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C8" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D8" t="b">
         <v>1</v>
       </c>
       <c r="P8" s="6"/>
       <c r="Q8" s="11">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C9" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" t="b">
         <v>1</v>
       </c>
       <c r="P9" s="6"/>
       <c r="Q9" s="11">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B10" s="10" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C10" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10" t="b">
         <v>1</v>
       </c>
       <c r="P10" s="6"/>
       <c r="Q10" s="11">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B11" s="10" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C11" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D11" t="b">
         <v>1</v>
       </c>
       <c r="P11" s="6"/>
       <c r="Q11" s="11">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B12" s="10" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C12" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" t="b">
         <v>1</v>
       </c>
       <c r="P12" s="6"/>
       <c r="Q12" s="11">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B13" s="10" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C13" s="5" t="b">
         <v>1</v>
@@ -831,7 +895,7 @@
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B14" s="10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C14" s="5" t="b">
         <v>1</v>
@@ -844,61 +908,297 @@
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B15" s="10" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C15" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D15" t="b">
         <v>1</v>
       </c>
       <c r="P15" s="6"/>
       <c r="Q15" s="11">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B16" s="10" t="s">
-        <v>28</v>
+      <c r="B16" s="12" t="s">
+        <v>24</v>
       </c>
       <c r="C16" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D16" t="b">
         <v>1</v>
       </c>
       <c r="P16" s="6"/>
       <c r="Q16" s="11">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B18" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D18" t="b">
+        <v>1</v>
+      </c>
+      <c r="P18" s="6"/>
+      <c r="Q18" s="13">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B19" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" t="b">
+        <v>1</v>
+      </c>
+      <c r="P19" s="6"/>
+      <c r="Q19" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B20" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D20" t="b">
+        <v>1</v>
+      </c>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="13">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B21" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B22" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D22" t="b">
+        <v>1</v>
+      </c>
+      <c r="P22" s="6"/>
+      <c r="Q22" s="13">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B23" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="8"/>
-      <c r="O17" s="8"/>
-      <c r="P17" s="9"/>
-      <c r="Q17" s="11">
+      <c r="C23" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23" t="b">
+        <v>1</v>
+      </c>
+      <c r="P23" s="6"/>
+      <c r="Q23" s="13">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B24" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" t="b">
+        <v>1</v>
+      </c>
+      <c r="P24" s="6"/>
+      <c r="Q24" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B25" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="5"/>
+      <c r="D25" t="b">
+        <v>1</v>
+      </c>
+      <c r="P25" s="6"/>
+      <c r="Q25" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B26" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="5"/>
+      <c r="D26" t="b">
+        <v>1</v>
+      </c>
+      <c r="P26" s="6"/>
+      <c r="Q26" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B27" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" s="5"/>
+      <c r="D27" t="b">
+        <v>1</v>
+      </c>
+      <c r="P27" s="6"/>
+      <c r="Q27" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B28" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="5"/>
+      <c r="D28" t="b">
+        <v>1</v>
+      </c>
+      <c r="P28" s="6"/>
+      <c r="Q28" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B29" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="5"/>
+      <c r="D29" t="b">
+        <v>1</v>
+      </c>
+      <c r="P29" s="6"/>
+      <c r="Q29" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B30" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" s="5"/>
+      <c r="D30" t="b">
+        <v>1</v>
+      </c>
+      <c r="P30" s="6"/>
+      <c r="Q30" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B31" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" s="5"/>
+      <c r="D31" t="b">
+        <v>1</v>
+      </c>
+      <c r="P31" s="6"/>
+      <c r="Q31" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B32" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" s="5"/>
+      <c r="D32" t="b">
+        <v>1</v>
+      </c>
+      <c r="P32" s="6"/>
+      <c r="Q32" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B33" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" s="7"/>
+      <c r="D33" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
+      <c r="K33" s="8"/>
+      <c r="L33" s="8"/>
+      <c r="M33" s="8"/>
+      <c r="N33" s="8"/>
+      <c r="O33" s="8"/>
+      <c r="P33" s="9"/>
+      <c r="Q33" s="13">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:Q17">
-    <sortCondition ref="B3:B17"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:Q33">
+    <sortCondition ref="B3:B33"/>
   </sortState>
-  <conditionalFormatting sqref="Q3:Q17">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+  <conditionalFormatting sqref="Q3:Q33">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Laborator 09.03.2023 - am inceput verificarea mainilor jucatorilor conform regulilor din poker
</commit_message>
<xml_diff>
--- a/Prezenta.xlsx
+++ b/Prezenta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\AlgoritmiFundamentali_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BAC79EE-4D5D-4CA5-AD40-5A572BF039C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E9321F-CAD6-4D7E-A9DA-D18B0DA52C5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>Nume Prenume</t>
   </si>
@@ -96,9 +96,6 @@
     <t>Olah Antoniu</t>
   </si>
   <si>
-    <t>Riabuokon Karolina</t>
-  </si>
-  <si>
     <t>Pintilie Robert</t>
   </si>
   <si>
@@ -166,6 +163,21 @@
   </si>
   <si>
     <t>Lucuta Stefan</t>
+  </si>
+  <si>
+    <t>Tirtea Gabriel</t>
+  </si>
+  <si>
+    <t>Farc Denisa</t>
+  </si>
+  <si>
+    <t>Tigan Andreea</t>
+  </si>
+  <si>
+    <t>Beschiu Valentin</t>
+  </si>
+  <si>
+    <t>Riabokon Karolina</t>
   </si>
 </sst>
 </file>
@@ -215,7 +227,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -344,11 +356,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -367,6 +390,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -657,10 +685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:Q33"/>
+  <dimension ref="B2:Q37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T32" sqref="T32"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -721,7 +749,7 @@
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B3" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="3" t="b">
@@ -740,13 +768,13 @@
       <c r="O3" s="3"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="11">
-        <f t="shared" ref="Q3:Q33" si="0">C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
+        <f t="shared" ref="Q3:Q37" si="0">C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B4" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" t="b">
@@ -760,7 +788,7 @@
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B5" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" t="b">
@@ -774,7 +802,7 @@
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B6" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" t="b">
@@ -788,7 +816,7 @@
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B7" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" t="b">
@@ -866,7 +894,7 @@
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B12" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" s="5" t="b">
         <v>1</v>
@@ -882,20 +910,23 @@
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B13" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D13" t="b">
         <v>1</v>
       </c>
       <c r="P13" s="6"/>
       <c r="Q13" s="11">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B14" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C14" s="5" t="b">
         <v>1</v>
@@ -908,7 +939,7 @@
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B15" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" s="5" t="b">
         <v>1</v>
@@ -924,7 +955,7 @@
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B16" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C16" s="5" t="b">
         <v>1</v>
@@ -969,7 +1000,7 @@
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B19" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" t="b">
@@ -983,7 +1014,7 @@
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B20" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C20" s="5" t="b">
         <v>1</v>
@@ -1012,7 +1043,7 @@
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B22" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C22" s="5" t="b">
         <v>1</v>
@@ -1028,7 +1059,7 @@
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B23" s="12" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="C23" s="5" t="b">
         <v>1</v>
@@ -1044,7 +1075,7 @@
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B24" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" t="b">
@@ -1058,7 +1089,7 @@
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B25" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" t="b">
@@ -1072,7 +1103,7 @@
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B26" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" t="b">
@@ -1086,7 +1117,7 @@
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B27" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" t="b">
@@ -1100,7 +1131,7 @@
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B28" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" t="b">
@@ -1114,7 +1145,7 @@
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B29" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" t="b">
@@ -1128,7 +1159,7 @@
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B30" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" t="b">
@@ -1142,7 +1173,7 @@
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B31" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" t="b">
@@ -1156,7 +1187,7 @@
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B32" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" t="b">
@@ -1170,7 +1201,7 @@
     </row>
     <row r="33" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B33" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C33" s="7"/>
       <c r="D33" s="8" t="b">
@@ -1193,11 +1224,59 @@
         <v>1</v>
       </c>
     </row>
+    <row r="34" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B34" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D34" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q34" s="16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B35" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D35" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q35" s="16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B36" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D36" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q36" s="16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B37" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D37" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q37" s="16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:Q33">
     <sortCondition ref="B3:B33"/>
   </sortState>
-  <conditionalFormatting sqref="Q3:Q33">
+  <conditionalFormatting sqref="Q3:Q37">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
       <formula>4</formula>
     </cfRule>

</xml_diff>

<commit_message>
Pregatire pentru urmatorul laborator de algoritmi - baza la Rainbow Sort
</commit_message>
<xml_diff>
--- a/Prezenta.xlsx
+++ b/Prezenta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\AlgoritmiFundamentali_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E9321F-CAD6-4D7E-A9DA-D18B0DA52C5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70B469C6-A601-4C93-888C-7974887AAF86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -363,7 +363,9 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -371,7 +373,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -388,13 +390,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -688,7 +688,7 @@
   <dimension ref="B2:Q37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="V27" sqref="V27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -701,46 +701,46 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="O2" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="P2" s="14" t="s">
         <v>14</v>
       </c>
       <c r="Q2" s="1" t="s">
@@ -749,7 +749,7 @@
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B3" s="10" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="3" t="b">
@@ -768,513 +768,887 @@
       <c r="O3" s="3"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="11">
-        <f t="shared" ref="Q3:Q37" si="0">C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
+        <f>C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B4" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" s="5"/>
-      <c r="D4" t="b">
-        <v>1</v>
-      </c>
+      <c r="D4" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
       <c r="P4" s="6"/>
       <c r="Q4" s="11">
-        <f t="shared" si="0"/>
+        <f>C4+D4+E4+F4+G4+H4+I4+J4+K4+L4+M4+N4+O4+P4</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B5" s="10" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C5" s="5"/>
-      <c r="D5" t="b">
-        <v>1</v>
-      </c>
+      <c r="D5" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
       <c r="P5" s="6"/>
       <c r="Q5" s="11">
-        <f t="shared" si="0"/>
+        <f>C5+D5+E5+F5+G5+H5+I5+J5+K5+L5+M5+N5+O5+P5</f>
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B6" s="10" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C6" s="5"/>
-      <c r="D6" t="b">
-        <v>1</v>
-      </c>
+      <c r="D6" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
       <c r="P6" s="6"/>
       <c r="Q6" s="11">
-        <f t="shared" si="0"/>
+        <f>C6+D6+E6+F6+G6+H6+I6+J6+K6+L6+M6+N6+O6+P6</f>
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B7" s="10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C7" s="5"/>
-      <c r="D7" t="b">
-        <v>1</v>
-      </c>
+      <c r="D7" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
       <c r="P7" s="6"/>
       <c r="Q7" s="11">
-        <f t="shared" si="0"/>
+        <f>C7+D7+E7+F7+G7+H7+I7+J7+K7+L7+M7+N7+O7+P7</f>
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B8" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D8" t="b">
-        <v>1</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
       <c r="P8" s="6"/>
       <c r="Q8" s="11">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C8+D8+E8+F8+G8+H8+I8+J8+K8+L8+M8+N8+O8+P8</f>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D9" t="b">
-        <v>1</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
       <c r="P9" s="6"/>
       <c r="Q9" s="11">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C9+D9+E9+F9+G9+H9+I9+J9+K9+L9+M9+N9+O9+P9</f>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B10" s="10" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C10" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D10" t="b">
-        <v>1</v>
-      </c>
+      <c r="D10" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
       <c r="P10" s="6"/>
       <c r="Q10" s="11">
-        <f t="shared" si="0"/>
+        <f>C10+D10+E10+F10+G10+H10+I10+J10+K10+L10+M10+N10+O10+P10</f>
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B11" s="10" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C11" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D11" t="b">
-        <v>1</v>
-      </c>
+      <c r="D11" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
       <c r="P11" s="6"/>
       <c r="Q11" s="11">
-        <f t="shared" si="0"/>
+        <f>C11+D11+E11+F11+G11+H11+I11+J11+K11+L11+M11+N11+O11+P11</f>
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B12" s="10" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C12" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D12" t="b">
-        <v>1</v>
-      </c>
+      <c r="D12" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
       <c r="P12" s="6"/>
       <c r="Q12" s="11">
-        <f t="shared" si="0"/>
+        <f>C12+D12+E12+F12+G12+H12+I12+J12+K12+L12+M12+N12+O12+P12</f>
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B13" s="10" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="C13" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D13" t="b">
-        <v>1</v>
-      </c>
+      <c r="D13" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
       <c r="P13" s="6"/>
       <c r="Q13" s="11">
-        <f t="shared" si="0"/>
+        <f>C13+D13+E13+F13+G13+H13+I13+J13+K13+L13+M13+N13+O13+P13</f>
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B14" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" s="5" t="b">
         <v>1</v>
       </c>
+      <c r="D14" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
       <c r="P14" s="6"/>
       <c r="Q14" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>C14+D14+E14+F14+G14+H14+I14+J14+K14+L14+M14+N14+O14+P14</f>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B15" s="10" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C15" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D15" t="b">
-        <v>1</v>
-      </c>
+      <c r="D15" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
       <c r="P15" s="6"/>
       <c r="Q15" s="11">
-        <f t="shared" si="0"/>
+        <f>C15+D15+E15+F15+G15+H15+I15+J15+K15+L15+M15+N15+O15+P15</f>
         <v>2</v>
       </c>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B16" s="12" t="s">
-        <v>23</v>
+      <c r="B16" s="10" t="s">
+        <v>26</v>
       </c>
       <c r="C16" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D16" t="b">
-        <v>1</v>
-      </c>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
+      <c r="O16" s="13"/>
       <c r="P16" s="6"/>
       <c r="Q16" s="11">
-        <f t="shared" si="0"/>
+        <f>C16+D16+E16+F16+G16+H16+I16+J16+K16+L16+M16+N16+O16+P16</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B17" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="13"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="11">
+        <f>C17+D17+E17+F17+G17+H17+I17+J17+K17+L17+M17+N17+O17+P17</f>
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B17" s="12" t="s">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B18" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D18" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="13"/>
+      <c r="O18" s="13"/>
+      <c r="P18" s="6"/>
+      <c r="Q18" s="11">
+        <f>C18+D18+E18+F18+G18+H18+I18+J18+K18+L18+M18+N18+O18+P18</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B19" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="P17" s="6"/>
-      <c r="Q17" s="13">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B18" s="12" t="s">
+      <c r="C19" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="13"/>
+      <c r="P19" s="6"/>
+      <c r="Q19" s="11">
+        <f>C19+D19+E19+F19+G19+H19+I19+J19+K19+L19+M19+N19+O19+P19</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B20" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D18" t="b">
-        <v>1</v>
-      </c>
-      <c r="P18" s="6"/>
-      <c r="Q18" s="13">
-        <f t="shared" si="0"/>
+      <c r="C20" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D20" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="11">
+        <f>C20+D20+E20+F20+G20+H20+I20+J20+K20+L20+M20+N20+O20+P20</f>
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B19" s="12" t="s">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B21" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="5"/>
-      <c r="D19" t="b">
-        <v>1</v>
-      </c>
-      <c r="P19" s="6"/>
-      <c r="Q19" s="13">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B20" s="12" t="s">
+      <c r="C21" s="5"/>
+      <c r="D21" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="11">
+        <f>C21+D21+E21+F21+G21+H21+I21+J21+K21+L21+M21+N21+O21+P21</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B22" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D20" t="b">
-        <v>1</v>
-      </c>
-      <c r="P20" s="6"/>
-      <c r="Q20" s="13">
-        <f t="shared" si="0"/>
+      <c r="C22" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D22" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="13"/>
+      <c r="P22" s="6"/>
+      <c r="Q22" s="11">
+        <f>C22+D22+E22+F22+G22+H22+I22+J22+K22+L22+M22+N22+O22+P22</f>
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B21" s="12" t="s">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B23" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="P21" s="6"/>
-      <c r="Q21" s="13">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B22" s="12" t="s">
+      <c r="C23" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="13"/>
+      <c r="P23" s="6"/>
+      <c r="Q23" s="11">
+        <f>C23+D23+E23+F23+G23+H23+I23+J23+K23+L23+M23+N23+O23+P23</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B24" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D22" t="b">
-        <v>1</v>
-      </c>
-      <c r="P22" s="6"/>
-      <c r="Q22" s="13">
-        <f t="shared" si="0"/>
+      <c r="C24" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D24" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="13"/>
+      <c r="N24" s="13"/>
+      <c r="O24" s="13"/>
+      <c r="P24" s="6"/>
+      <c r="Q24" s="11">
+        <f>C24+D24+E24+F24+G24+H24+I24+J24+K24+L24+M24+N24+O24+P24</f>
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B23" s="12" t="s">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B25" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D23" t="b">
-        <v>1</v>
-      </c>
-      <c r="P23" s="6"/>
-      <c r="Q23" s="13">
-        <f t="shared" si="0"/>
+      <c r="C25" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D25" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="13"/>
+      <c r="N25" s="13"/>
+      <c r="O25" s="13"/>
+      <c r="P25" s="6"/>
+      <c r="Q25" s="11">
+        <f>C25+D25+E25+F25+G25+H25+I25+J25+K25+L25+M25+N25+O25+P25</f>
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B24" s="12" t="s">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B26" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C24" s="5"/>
-      <c r="D24" t="b">
-        <v>1</v>
-      </c>
-      <c r="P24" s="6"/>
-      <c r="Q24" s="13">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B25" s="12" t="s">
+      <c r="C26" s="5"/>
+      <c r="D26" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="13"/>
+      <c r="N26" s="13"/>
+      <c r="O26" s="13"/>
+      <c r="P26" s="6"/>
+      <c r="Q26" s="11">
+        <f>C26+D26+E26+F26+G26+H26+I26+J26+K26+L26+M26+N26+O26+P26</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B27" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C25" s="5"/>
-      <c r="D25" t="b">
-        <v>1</v>
-      </c>
-      <c r="P25" s="6"/>
-      <c r="Q25" s="13">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B26" s="12" t="s">
+      <c r="C27" s="5"/>
+      <c r="D27" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="13"/>
+      <c r="O27" s="13"/>
+      <c r="P27" s="6"/>
+      <c r="Q27" s="11">
+        <f>C27+D27+E27+F27+G27+H27+I27+J27+K27+L27+M27+N27+O27+P27</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B28" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="5"/>
-      <c r="D26" t="b">
-        <v>1</v>
-      </c>
-      <c r="P26" s="6"/>
-      <c r="Q26" s="13">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B27" s="12" t="s">
+      <c r="C28" s="5"/>
+      <c r="D28" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="13"/>
+      <c r="N28" s="13"/>
+      <c r="O28" s="13"/>
+      <c r="P28" s="6"/>
+      <c r="Q28" s="11">
+        <f>C28+D28+E28+F28+G28+H28+I28+J28+K28+L28+M28+N28+O28+P28</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B29" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="5"/>
-      <c r="D27" t="b">
-        <v>1</v>
-      </c>
-      <c r="P27" s="6"/>
-      <c r="Q27" s="13">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B28" s="12" t="s">
+      <c r="C29" s="5"/>
+      <c r="D29" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13"/>
+      <c r="M29" s="13"/>
+      <c r="N29" s="13"/>
+      <c r="O29" s="13"/>
+      <c r="P29" s="6"/>
+      <c r="Q29" s="11">
+        <f>C29+D29+E29+F29+G29+H29+I29+J29+K29+L29+M29+N29+O29+P29</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B30" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C28" s="5"/>
-      <c r="D28" t="b">
-        <v>1</v>
-      </c>
-      <c r="P28" s="6"/>
-      <c r="Q28" s="13">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B29" s="12" t="s">
+      <c r="C30" s="5"/>
+      <c r="D30" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="13"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13"/>
+      <c r="M30" s="13"/>
+      <c r="N30" s="13"/>
+      <c r="O30" s="13"/>
+      <c r="P30" s="6"/>
+      <c r="Q30" s="11">
+        <f>C30+D30+E30+F30+G30+H30+I30+J30+K30+L30+M30+N30+O30+P30</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B31" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C31" s="5"/>
+      <c r="D31" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
+      <c r="M31" s="13"/>
+      <c r="N31" s="13"/>
+      <c r="O31" s="13"/>
+      <c r="P31" s="6"/>
+      <c r="Q31" s="11">
+        <f>C31+D31+E31+F31+G31+H31+I31+J31+K31+L31+M31+N31+O31+P31</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B32" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" s="5"/>
+      <c r="D32" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="13"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="13"/>
+      <c r="N32" s="13"/>
+      <c r="O32" s="13"/>
+      <c r="P32" s="6"/>
+      <c r="Q32" s="11">
+        <f>C32+D32+E32+F32+G32+H32+I32+J32+K32+L32+M32+N32+O32+P32</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B33" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C29" s="5"/>
-      <c r="D29" t="b">
-        <v>1</v>
-      </c>
-      <c r="P29" s="6"/>
-      <c r="Q29" s="13">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B30" s="12" t="s">
+      <c r="C33" s="5"/>
+      <c r="D33" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="13"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="13"/>
+      <c r="M33" s="13"/>
+      <c r="N33" s="13"/>
+      <c r="O33" s="13"/>
+      <c r="P33" s="6"/>
+      <c r="Q33" s="11">
+        <f>C33+D33+E33+F33+G33+H33+I33+J33+K33+L33+M33+N33+O33+P33</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B34" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="5"/>
-      <c r="D30" t="b">
-        <v>1</v>
-      </c>
-      <c r="P30" s="6"/>
-      <c r="Q30" s="13">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B31" s="12" t="s">
+      <c r="C34" s="5"/>
+      <c r="D34" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="13"/>
+      <c r="M34" s="13"/>
+      <c r="N34" s="13"/>
+      <c r="O34" s="13"/>
+      <c r="P34" s="6"/>
+      <c r="Q34" s="12">
+        <f>C34+D34+E34+F34+G34+H34+I34+J34+K34+L34+M34+N34+O34+P34</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B35" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C31" s="5"/>
-      <c r="D31" t="b">
-        <v>1</v>
-      </c>
-      <c r="P31" s="6"/>
-      <c r="Q31" s="13">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B32" s="12" t="s">
+      <c r="C35" s="5"/>
+      <c r="D35" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="13"/>
+      <c r="K35" s="13"/>
+      <c r="L35" s="13"/>
+      <c r="M35" s="13"/>
+      <c r="N35" s="13"/>
+      <c r="O35" s="13"/>
+      <c r="P35" s="6"/>
+      <c r="Q35" s="12">
+        <f>C35+D35+E35+F35+G35+H35+I35+J35+K35+L35+M35+N35+O35+P35</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B36" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C32" s="5"/>
-      <c r="D32" t="b">
-        <v>1</v>
-      </c>
-      <c r="P32" s="6"/>
-      <c r="Q32" s="13">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B33" s="12" t="s">
+      <c r="C36" s="5"/>
+      <c r="D36" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="13"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
+      <c r="M36" s="13"/>
+      <c r="N36" s="13"/>
+      <c r="O36" s="13"/>
+      <c r="P36" s="6"/>
+      <c r="Q36" s="12">
+        <f>C36+D36+E36+F36+G36+H36+I36+J36+K36+L36+M36+N36+O36+P36</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B37" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C33" s="7"/>
-      <c r="D33" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
-      <c r="M33" s="8"/>
-      <c r="N33" s="8"/>
-      <c r="O33" s="8"/>
-      <c r="P33" s="9"/>
-      <c r="Q33" s="13">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B34" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="D34" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q34" s="16">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B35" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D35" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q35" s="16">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B36" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="D36" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q36" s="16">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B37" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="D37" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q37" s="16">
-        <f t="shared" si="0"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+      <c r="L37" s="8"/>
+      <c r="M37" s="8"/>
+      <c r="N37" s="8"/>
+      <c r="O37" s="8"/>
+      <c r="P37" s="9"/>
+      <c r="Q37" s="12">
+        <f>C37+D37+E37+F37+G37+H37+I37+J37+K37+L37+M37+N37+O37+P37</f>
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:Q33">
-    <sortCondition ref="B3:B33"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:Q37">
+    <sortCondition ref="B3:B37"/>
   </sortState>
   <conditionalFormatting sqref="Q3:Q37">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">

</xml_diff>

<commit_message>
Laborator 14.03.2023 - Generarea matricei jocului Minesweeper
</commit_message>
<xml_diff>
--- a/Prezenta.xlsx
+++ b/Prezenta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\AlgoritmiFundamentali_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70B469C6-A601-4C93-888C-7974887AAF86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C56F289-6FE8-4E0A-9FCF-82D44C512CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Nume Prenume</t>
   </si>
@@ -178,6 +178,12 @@
   </si>
   <si>
     <t>Riabokon Karolina</t>
+  </si>
+  <si>
+    <t>Vancea Claudiu</t>
+  </si>
+  <si>
+    <t>Dumitrache Luca</t>
   </si>
 </sst>
 </file>
@@ -373,7 +379,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -390,13 +396,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -685,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:Q37"/>
+  <dimension ref="B2:Q39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V27" sqref="V27"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -701,46 +704,46 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="14" t="s">
+      <c r="C2" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="J2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="K2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="14" t="s">
+      <c r="L2" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="14" t="s">
+      <c r="M2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="14" t="s">
+      <c r="N2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="14" t="s">
+      <c r="O2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="14" t="s">
+      <c r="P2" s="12" t="s">
         <v>14</v>
       </c>
       <c r="Q2" s="1" t="s">
@@ -755,7 +758,9 @@
       <c r="D3" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E3" s="3"/>
+      <c r="E3" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -769,7 +774,7 @@
       <c r="P3" s="4"/>
       <c r="Q3" s="11">
         <f>C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.3">
@@ -799,13 +804,13 @@
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B5" s="10" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C5" s="5"/>
-      <c r="D5" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13" t="b">
+        <v>1</v>
+      </c>
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
       <c r="H5" s="13"/>
@@ -824,7 +829,7 @@
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B6" s="10" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="13" t="b">
@@ -849,13 +854,15 @@
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B7" s="10" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="E7" s="13"/>
+      <c r="E7" s="13" t="b">
+        <v>1</v>
+      </c>
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
@@ -869,12 +876,12 @@
       <c r="P7" s="6"/>
       <c r="Q7" s="11">
         <f>C7+D7+E7+F7+G7+H7+I7+J7+K7+L7+M7+N7+O7+P7</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B8" s="10" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="13" t="b">
@@ -899,7 +906,7 @@
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="13" t="b">
@@ -924,15 +931,15 @@
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B10" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="5" t="b">
-        <v>1</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="C10" s="5"/>
       <c r="D10" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="E10" s="13"/>
+      <c r="E10" s="13" t="b">
+        <v>1</v>
+      </c>
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
@@ -951,7 +958,7 @@
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B11" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C11" s="5" t="b">
         <v>1</v>
@@ -959,7 +966,9 @@
       <c r="D11" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="E11" s="13"/>
+      <c r="E11" s="13" t="b">
+        <v>1</v>
+      </c>
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
@@ -973,12 +982,12 @@
       <c r="P11" s="6"/>
       <c r="Q11" s="11">
         <f>C11+D11+E11+F11+G11+H11+I11+J11+K11+L11+M11+N11+O11+P11</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B12" s="10" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C12" s="5" t="b">
         <v>1</v>
@@ -986,7 +995,9 @@
       <c r="D12" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="E12" s="13"/>
+      <c r="E12" s="13" t="b">
+        <v>1</v>
+      </c>
       <c r="F12" s="13"/>
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
@@ -1000,12 +1011,12 @@
       <c r="P12" s="6"/>
       <c r="Q12" s="11">
         <f>C12+D12+E12+F12+G12+H12+I12+J12+K12+L12+M12+N12+O12+P12</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B13" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" s="5" t="b">
         <v>1</v>
@@ -1032,7 +1043,7 @@
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B14" s="10" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C14" s="5" t="b">
         <v>1</v>
@@ -1040,7 +1051,9 @@
       <c r="D14" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="E14" s="13"/>
+      <c r="E14" s="13" t="b">
+        <v>1</v>
+      </c>
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
@@ -1054,12 +1067,12 @@
       <c r="P14" s="6"/>
       <c r="Q14" s="11">
         <f>C14+D14+E14+F14+G14+H14+I14+J14+K14+L14+M14+N14+O14+P14</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B15" s="10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C15" s="5" t="b">
         <v>1</v>
@@ -1067,7 +1080,9 @@
       <c r="D15" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="E15" s="13"/>
+      <c r="E15" s="13" t="b">
+        <v>1</v>
+      </c>
       <c r="F15" s="13"/>
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
@@ -1081,17 +1096,19 @@
       <c r="P15" s="6"/>
       <c r="Q15" s="11">
         <f>C15+D15+E15+F15+G15+H15+I15+J15+K15+L15+M15+N15+O15+P15</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B16" s="10" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C16" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D16" s="13"/>
+      <c r="D16" s="13" t="b">
+        <v>1</v>
+      </c>
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
@@ -1106,19 +1123,17 @@
       <c r="P16" s="6"/>
       <c r="Q16" s="11">
         <f>C16+D16+E16+F16+G16+H16+I16+J16+K16+L16+M16+N16+O16+P16</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B17" s="10" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C17" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D17" s="13" t="b">
-        <v>1</v>
-      </c>
+      <c r="D17" s="13"/>
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
       <c r="G17" s="13"/>
@@ -1133,12 +1148,12 @@
       <c r="P17" s="6"/>
       <c r="Q17" s="11">
         <f>C17+D17+E17+F17+G17+H17+I17+J17+K17+L17+M17+N17+O17+P17</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B18" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C18" s="5" t="b">
         <v>1</v>
@@ -1146,7 +1161,9 @@
       <c r="D18" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="E18" s="13"/>
+      <c r="E18" s="13" t="b">
+        <v>1</v>
+      </c>
       <c r="F18" s="13"/>
       <c r="G18" s="13"/>
       <c r="H18" s="13"/>
@@ -1160,17 +1177,19 @@
       <c r="P18" s="6"/>
       <c r="Q18" s="11">
         <f>C18+D18+E18+F18+G18+H18+I18+J18+K18+L18+M18+N18+O18+P18</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B19" s="10" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C19" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D19" s="13"/>
+      <c r="D19" s="13" t="b">
+        <v>1</v>
+      </c>
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
       <c r="G19" s="13"/>
@@ -1185,19 +1204,17 @@
       <c r="P19" s="6"/>
       <c r="Q19" s="11">
         <f>C19+D19+E19+F19+G19+H19+I19+J19+K19+L19+M19+N19+O19+P19</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B20" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C20" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D20" s="13" t="b">
-        <v>1</v>
-      </c>
+      <c r="D20" s="13"/>
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>
@@ -1212,18 +1229,22 @@
       <c r="P20" s="6"/>
       <c r="Q20" s="11">
         <f>C20+D20+E20+F20+G20+H20+I20+J20+K20+L20+M20+N20+O20+P20</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B21" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" s="5"/>
+        <v>19</v>
+      </c>
+      <c r="C21" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="D21" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="E21" s="13"/>
+      <c r="E21" s="13" t="b">
+        <v>1</v>
+      </c>
       <c r="F21" s="13"/>
       <c r="G21" s="13"/>
       <c r="H21" s="13"/>
@@ -1237,16 +1258,14 @@
       <c r="P21" s="6"/>
       <c r="Q21" s="11">
         <f>C21+D21+E21+F21+G21+H21+I21+J21+K21+L21+M21+N21+O21+P21</f>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B22" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="5" t="b">
-        <v>1</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="C22" s="5"/>
       <c r="D22" s="13" t="b">
         <v>1</v>
       </c>
@@ -1264,18 +1283,22 @@
       <c r="P22" s="6"/>
       <c r="Q22" s="11">
         <f>C22+D22+E22+F22+G22+H22+I22+J22+K22+L22+M22+N22+O22+P22</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B23" s="10" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="C23" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
+      <c r="D23" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E23" s="13" t="b">
+        <v>1</v>
+      </c>
       <c r="F23" s="13"/>
       <c r="G23" s="13"/>
       <c r="H23" s="13"/>
@@ -1289,19 +1312,17 @@
       <c r="P23" s="6"/>
       <c r="Q23" s="11">
         <f>C23+D23+E23+F23+G23+H23+I23+J23+K23+L23+M23+N23+O23+P23</f>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B24" s="10" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C24" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D24" s="13" t="b">
-        <v>1</v>
-      </c>
+      <c r="D24" s="13"/>
       <c r="E24" s="13"/>
       <c r="F24" s="13"/>
       <c r="G24" s="13"/>
@@ -1316,12 +1337,12 @@
       <c r="P24" s="6"/>
       <c r="Q24" s="11">
         <f>C24+D24+E24+F24+G24+H24+I24+J24+K24+L24+M24+N24+O24+P24</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B25" s="10" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="C25" s="5" t="b">
         <v>1</v>
@@ -1348,13 +1369,17 @@
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B26" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C26" s="5"/>
+        <v>50</v>
+      </c>
+      <c r="C26" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="D26" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="E26" s="13"/>
+      <c r="E26" s="13" t="b">
+        <v>1</v>
+      </c>
       <c r="F26" s="13"/>
       <c r="G26" s="13"/>
       <c r="H26" s="13"/>
@@ -1368,12 +1393,12 @@
       <c r="P26" s="6"/>
       <c r="Q26" s="11">
         <f>C26+D26+E26+F26+G26+H26+I26+J26+K26+L26+M26+N26+O26+P26</f>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B27" s="10" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="13" t="b">
@@ -1398,13 +1423,15 @@
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B28" s="10" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="E28" s="13"/>
+      <c r="E28" s="13" t="b">
+        <v>1</v>
+      </c>
       <c r="F28" s="13"/>
       <c r="G28" s="13"/>
       <c r="H28" s="13"/>
@@ -1418,12 +1445,12 @@
       <c r="P28" s="6"/>
       <c r="Q28" s="11">
         <f>C28+D28+E28+F28+G28+H28+I28+J28+K28+L28+M28+N28+O28+P28</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B29" s="10" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="13" t="b">
@@ -1448,7 +1475,7 @@
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B30" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="13" t="b">
@@ -1473,7 +1500,7 @@
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B31" s="10" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="13" t="b">
@@ -1498,7 +1525,7 @@
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B32" s="10" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="13" t="b">
@@ -1523,7 +1550,7 @@
     </row>
     <row r="33" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B33" s="10" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="13" t="b">
@@ -1548,13 +1575,15 @@
     </row>
     <row r="34" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B34" s="10" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="E34" s="13"/>
+      <c r="E34" s="13" t="b">
+        <v>1</v>
+      </c>
       <c r="F34" s="13"/>
       <c r="G34" s="13"/>
       <c r="H34" s="13"/>
@@ -1566,20 +1595,22 @@
       <c r="N34" s="13"/>
       <c r="O34" s="13"/>
       <c r="P34" s="6"/>
-      <c r="Q34" s="12">
+      <c r="Q34" s="11">
         <f>C34+D34+E34+F34+G34+H34+I34+J34+K34+L34+M34+N34+O34+P34</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B35" s="10" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="E35" s="13"/>
+      <c r="E35" s="13" t="b">
+        <v>1</v>
+      </c>
       <c r="F35" s="13"/>
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
@@ -1591,20 +1622,22 @@
       <c r="N35" s="13"/>
       <c r="O35" s="13"/>
       <c r="P35" s="6"/>
-      <c r="Q35" s="12">
+      <c r="Q35" s="11">
         <f>C35+D35+E35+F35+G35+H35+I35+J35+K35+L35+M35+N35+O35+P35</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B36" s="10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="E36" s="13"/>
+      <c r="E36" s="13" t="b">
+        <v>1</v>
+      </c>
       <c r="F36" s="13"/>
       <c r="G36" s="13"/>
       <c r="H36" s="13"/>
@@ -1616,41 +1649,93 @@
       <c r="N36" s="13"/>
       <c r="O36" s="13"/>
       <c r="P36" s="6"/>
-      <c r="Q36" s="12">
+      <c r="Q36" s="11">
         <f>C36+D36+E36+F36+G36+H36+I36+J36+K36+L36+M36+N36+O36+P36</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B37" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37" s="5"/>
+      <c r="D37" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E37" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13"/>
+      <c r="K37" s="13"/>
+      <c r="L37" s="13"/>
+      <c r="M37" s="13"/>
+      <c r="N37" s="13"/>
+      <c r="O37" s="13"/>
+      <c r="P37" s="6"/>
+      <c r="Q37" s="11">
+        <f>C37+D37+E37+F37+G37+H37+I37+J37+K37+L37+M37+N37+O37+P37</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B38" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C38" s="5"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="13"/>
+      <c r="J38" s="13"/>
+      <c r="K38" s="13"/>
+      <c r="L38" s="13"/>
+      <c r="M38" s="13"/>
+      <c r="N38" s="13"/>
+      <c r="O38" s="13"/>
+      <c r="P38" s="6"/>
+      <c r="Q38" s="11">
+        <f>C38+D38+E38+F38+G38+H38+I38+J38+K38+L38+M38+N38+O38+P38</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B39" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C37" s="7"/>
-      <c r="D37" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
-      <c r="J37" s="8"/>
-      <c r="K37" s="8"/>
-      <c r="L37" s="8"/>
-      <c r="M37" s="8"/>
-      <c r="N37" s="8"/>
-      <c r="O37" s="8"/>
-      <c r="P37" s="9"/>
-      <c r="Q37" s="12">
-        <f>C37+D37+E37+F37+G37+H37+I37+J37+K37+L37+M37+N37+O37+P37</f>
+      <c r="C39" s="7"/>
+      <c r="D39" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+      <c r="K39" s="8"/>
+      <c r="L39" s="8"/>
+      <c r="M39" s="8"/>
+      <c r="N39" s="8"/>
+      <c r="O39" s="8"/>
+      <c r="P39" s="9"/>
+      <c r="Q39" s="11">
+        <f>C39+D39+E39+F39+G39+H39+I39+J39+K39+L39+M39+N39+O39+P39</f>
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:Q37">
-    <sortCondition ref="B3:B37"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:Q39">
+    <sortCondition ref="B3:B39"/>
   </sortState>
-  <conditionalFormatting sqref="Q3:Q37">
+  <conditionalFormatting sqref="Q3:Q39">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
       <formula>4</formula>
     </cfRule>

</xml_diff>

<commit_message>
Laborator 16.03.2023 - Afisarea castigatorului la Poker si cele 3 sortari de baza puse in Rainbow Sort
</commit_message>
<xml_diff>
--- a/Prezenta.xlsx
+++ b/Prezenta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\AlgoritmiFundamentali_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C56F289-6FE8-4E0A-9FCF-82D44C512CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB7C88F-C586-4D3F-994C-46DF2DE0CBBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -379,7 +379,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -399,7 +399,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -690,8 +689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -773,7 +772,7 @@
       <c r="O3" s="3"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="11">
-        <f>C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
+        <f t="shared" ref="Q3:Q39" si="0">C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
         <v>2</v>
       </c>
     </row>
@@ -782,23 +781,12 @@
         <v>35</v>
       </c>
       <c r="C4" s="5"/>
-      <c r="D4" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
       <c r="P4" s="6"/>
       <c r="Q4" s="11">
-        <f>C4+D4+E4+F4+G4+H4+I4+J4+K4+L4+M4+N4+O4+P4</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -807,23 +795,12 @@
         <v>52</v>
       </c>
       <c r="C5" s="5"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
       <c r="P5" s="6"/>
       <c r="Q5" s="11">
-        <f>C5+D5+E5+F5+G5+H5+I5+J5+K5+L5+M5+N5+O5+P5</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -832,23 +809,12 @@
         <v>47</v>
       </c>
       <c r="C6" s="5"/>
-      <c r="D6" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
       <c r="P6" s="6"/>
       <c r="Q6" s="11">
-        <f>C6+D6+E6+F6+G6+H6+I6+J6+K6+L6+M6+N6+O6+P6</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -857,25 +823,15 @@
         <v>36</v>
       </c>
       <c r="C7" s="5"/>
-      <c r="D7" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E7" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
+      <c r="D7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
       <c r="P7" s="6"/>
       <c r="Q7" s="11">
-        <f>C7+D7+E7+F7+G7+H7+I7+J7+K7+L7+M7+N7+O7+P7</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -884,23 +840,12 @@
         <v>40</v>
       </c>
       <c r="C8" s="5"/>
-      <c r="D8" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13"/>
+      <c r="D8" t="b">
+        <v>1</v>
+      </c>
       <c r="P8" s="6"/>
       <c r="Q8" s="11">
-        <f>C8+D8+E8+F8+G8+H8+I8+J8+K8+L8+M8+N8+O8+P8</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -909,23 +854,12 @@
         <v>45</v>
       </c>
       <c r="C9" s="5"/>
-      <c r="D9" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="13"/>
+      <c r="D9" t="b">
+        <v>1</v>
+      </c>
       <c r="P9" s="6"/>
       <c r="Q9" s="11">
-        <f>C9+D9+E9+F9+G9+H9+I9+J9+K9+L9+M9+N9+O9+P9</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -934,25 +868,15 @@
         <v>43</v>
       </c>
       <c r="C10" s="5"/>
-      <c r="D10" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E10" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13"/>
+      <c r="D10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" t="b">
+        <v>1</v>
+      </c>
       <c r="P10" s="6"/>
       <c r="Q10" s="11">
-        <f>C10+D10+E10+F10+G10+H10+I10+J10+K10+L10+M10+N10+O10+P10</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -963,25 +887,15 @@
       <c r="C11" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D11" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E11" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="13"/>
+      <c r="D11" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" t="b">
+        <v>1</v>
+      </c>
       <c r="P11" s="6"/>
       <c r="Q11" s="11">
-        <f>C11+D11+E11+F11+G11+H11+I11+J11+K11+L11+M11+N11+O11+P11</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -992,25 +906,15 @@
       <c r="C12" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D12" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E12" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
-      <c r="N12" s="13"/>
-      <c r="O12" s="13"/>
+      <c r="D12" t="b">
+        <v>1</v>
+      </c>
+      <c r="E12" t="b">
+        <v>1</v>
+      </c>
       <c r="P12" s="6"/>
       <c r="Q12" s="11">
-        <f>C12+D12+E12+F12+G12+H12+I12+J12+K12+L12+M12+N12+O12+P12</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -1021,23 +925,12 @@
       <c r="C13" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D13" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
-      <c r="O13" s="13"/>
+      <c r="D13" t="b">
+        <v>1</v>
+      </c>
       <c r="P13" s="6"/>
       <c r="Q13" s="11">
-        <f>C13+D13+E13+F13+G13+H13+I13+J13+K13+L13+M13+N13+O13+P13</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -1048,25 +941,15 @@
       <c r="C14" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D14" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E14" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
-      <c r="N14" s="13"/>
-      <c r="O14" s="13"/>
+      <c r="D14" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14" t="b">
+        <v>1</v>
+      </c>
       <c r="P14" s="6"/>
       <c r="Q14" s="11">
-        <f>C14+D14+E14+F14+G14+H14+I14+J14+K14+L14+M14+N14+O14+P14</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -1077,25 +960,15 @@
       <c r="C15" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D15" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E15" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="13"/>
-      <c r="O15" s="13"/>
+      <c r="D15" t="b">
+        <v>1</v>
+      </c>
+      <c r="E15" t="b">
+        <v>1</v>
+      </c>
       <c r="P15" s="6"/>
       <c r="Q15" s="11">
-        <f>C15+D15+E15+F15+G15+H15+I15+J15+K15+L15+M15+N15+O15+P15</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -1106,24 +979,16 @@
       <c r="C16" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D16" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="13"/>
-      <c r="N16" s="13"/>
-      <c r="O16" s="13"/>
+      <c r="D16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E16" t="b">
+        <v>1</v>
+      </c>
       <c r="P16" s="6"/>
       <c r="Q16" s="11">
-        <f>C16+D16+E16+F16+G16+H16+I16+J16+K16+L16+M16+N16+O16+P16</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.3">
@@ -1133,21 +998,9 @@
       <c r="C17" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="13"/>
-      <c r="O17" s="13"/>
       <c r="P17" s="6"/>
       <c r="Q17" s="11">
-        <f>C17+D17+E17+F17+G17+H17+I17+J17+K17+L17+M17+N17+O17+P17</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1158,25 +1011,15 @@
       <c r="C18" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D18" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E18" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
-      <c r="N18" s="13"/>
-      <c r="O18" s="13"/>
+      <c r="D18" t="b">
+        <v>1</v>
+      </c>
+      <c r="E18" t="b">
+        <v>1</v>
+      </c>
       <c r="P18" s="6"/>
       <c r="Q18" s="11">
-        <f>C18+D18+E18+F18+G18+H18+I18+J18+K18+L18+M18+N18+O18+P18</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -1187,23 +1030,12 @@
       <c r="C19" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D19" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
-      <c r="N19" s="13"/>
-      <c r="O19" s="13"/>
+      <c r="D19" t="b">
+        <v>1</v>
+      </c>
       <c r="P19" s="6"/>
       <c r="Q19" s="11">
-        <f>C19+D19+E19+F19+G19+H19+I19+J19+K19+L19+M19+N19+O19+P19</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -1214,21 +1046,9 @@
       <c r="C20" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="13"/>
-      <c r="O20" s="13"/>
       <c r="P20" s="6"/>
       <c r="Q20" s="11">
-        <f>C20+D20+E20+F20+G20+H20+I20+J20+K20+L20+M20+N20+O20+P20</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1239,25 +1059,15 @@
       <c r="C21" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D21" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E21" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
-      <c r="N21" s="13"/>
-      <c r="O21" s="13"/>
+      <c r="D21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E21" t="b">
+        <v>1</v>
+      </c>
       <c r="P21" s="6"/>
       <c r="Q21" s="11">
-        <f>C21+D21+E21+F21+G21+H21+I21+J21+K21+L21+M21+N21+O21+P21</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -1266,23 +1076,12 @@
         <v>33</v>
       </c>
       <c r="C22" s="5"/>
-      <c r="D22" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
-      <c r="O22" s="13"/>
+      <c r="D22" t="b">
+        <v>1</v>
+      </c>
       <c r="P22" s="6"/>
       <c r="Q22" s="11">
-        <f>C22+D22+E22+F22+G22+H22+I22+J22+K22+L22+M22+N22+O22+P22</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1293,25 +1092,15 @@
       <c r="C23" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D23" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E23" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
-      <c r="O23" s="13"/>
+      <c r="D23" t="b">
+        <v>1</v>
+      </c>
+      <c r="E23" t="b">
+        <v>1</v>
+      </c>
       <c r="P23" s="6"/>
       <c r="Q23" s="11">
-        <f>C23+D23+E23+F23+G23+H23+I23+J23+K23+L23+M23+N23+O23+P23</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -1322,21 +1111,9 @@
       <c r="C24" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="13"/>
-      <c r="M24" s="13"/>
-      <c r="N24" s="13"/>
-      <c r="O24" s="13"/>
       <c r="P24" s="6"/>
       <c r="Q24" s="11">
-        <f>C24+D24+E24+F24+G24+H24+I24+J24+K24+L24+M24+N24+O24+P24</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1347,24 +1124,16 @@
       <c r="C25" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D25" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="13"/>
-      <c r="N25" s="13"/>
-      <c r="O25" s="13"/>
+      <c r="D25" t="b">
+        <v>1</v>
+      </c>
+      <c r="E25" t="b">
+        <v>1</v>
+      </c>
       <c r="P25" s="6"/>
       <c r="Q25" s="11">
-        <f>C25+D25+E25+F25+G25+H25+I25+J25+K25+L25+M25+N25+O25+P25</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.3">
@@ -1374,25 +1143,15 @@
       <c r="C26" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D26" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E26" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="13"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="13"/>
-      <c r="M26" s="13"/>
-      <c r="N26" s="13"/>
-      <c r="O26" s="13"/>
+      <c r="D26" t="b">
+        <v>1</v>
+      </c>
+      <c r="E26" t="b">
+        <v>1</v>
+      </c>
       <c r="P26" s="6"/>
       <c r="Q26" s="11">
-        <f>C26+D26+E26+F26+G26+H26+I26+J26+K26+L26+M26+N26+O26+P26</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -1401,24 +1160,16 @@
         <v>34</v>
       </c>
       <c r="C27" s="5"/>
-      <c r="D27" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="13"/>
-      <c r="K27" s="13"/>
-      <c r="L27" s="13"/>
-      <c r="M27" s="13"/>
-      <c r="N27" s="13"/>
-      <c r="O27" s="13"/>
+      <c r="D27" t="b">
+        <v>1</v>
+      </c>
+      <c r="E27" t="b">
+        <v>1</v>
+      </c>
       <c r="P27" s="6"/>
       <c r="Q27" s="11">
-        <f>C27+D27+E27+F27+G27+H27+I27+J27+K27+L27+M27+N27+O27+P27</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.3">
@@ -1426,25 +1177,15 @@
         <v>44</v>
       </c>
       <c r="C28" s="5"/>
-      <c r="D28" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E28" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="13"/>
-      <c r="K28" s="13"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="13"/>
-      <c r="N28" s="13"/>
-      <c r="O28" s="13"/>
+      <c r="D28" t="b">
+        <v>1</v>
+      </c>
+      <c r="E28" t="b">
+        <v>1</v>
+      </c>
       <c r="P28" s="6"/>
       <c r="Q28" s="11">
-        <f>C28+D28+E28+F28+G28+H28+I28+J28+K28+L28+M28+N28+O28+P28</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -1453,23 +1194,12 @@
         <v>42</v>
       </c>
       <c r="C29" s="5"/>
-      <c r="D29" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="13"/>
-      <c r="K29" s="13"/>
-      <c r="L29" s="13"/>
-      <c r="M29" s="13"/>
-      <c r="N29" s="13"/>
-      <c r="O29" s="13"/>
+      <c r="D29" t="b">
+        <v>1</v>
+      </c>
       <c r="P29" s="6"/>
       <c r="Q29" s="11">
-        <f>C29+D29+E29+F29+G29+H29+I29+J29+K29+L29+M29+N29+O29+P29</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1478,24 +1208,16 @@
         <v>31</v>
       </c>
       <c r="C30" s="5"/>
-      <c r="D30" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="13"/>
-      <c r="J30" s="13"/>
-      <c r="K30" s="13"/>
-      <c r="L30" s="13"/>
-      <c r="M30" s="13"/>
-      <c r="N30" s="13"/>
-      <c r="O30" s="13"/>
+      <c r="D30" t="b">
+        <v>1</v>
+      </c>
+      <c r="E30" t="b">
+        <v>1</v>
+      </c>
       <c r="P30" s="6"/>
       <c r="Q30" s="11">
-        <f>C30+D30+E30+F30+G30+H30+I30+J30+K30+L30+M30+N30+O30+P30</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.3">
@@ -1503,23 +1225,12 @@
         <v>32</v>
       </c>
       <c r="C31" s="5"/>
-      <c r="D31" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="13"/>
-      <c r="I31" s="13"/>
-      <c r="J31" s="13"/>
-      <c r="K31" s="13"/>
-      <c r="L31" s="13"/>
-      <c r="M31" s="13"/>
-      <c r="N31" s="13"/>
-      <c r="O31" s="13"/>
+      <c r="D31" t="b">
+        <v>1</v>
+      </c>
       <c r="P31" s="6"/>
       <c r="Q31" s="11">
-        <f>C31+D31+E31+F31+G31+H31+I31+J31+K31+L31+M31+N31+O31+P31</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1528,23 +1239,12 @@
         <v>48</v>
       </c>
       <c r="C32" s="5"/>
-      <c r="D32" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
-      <c r="I32" s="13"/>
-      <c r="J32" s="13"/>
-      <c r="K32" s="13"/>
-      <c r="L32" s="13"/>
-      <c r="M32" s="13"/>
-      <c r="N32" s="13"/>
-      <c r="O32" s="13"/>
+      <c r="D32" t="b">
+        <v>1</v>
+      </c>
       <c r="P32" s="6"/>
       <c r="Q32" s="11">
-        <f>C32+D32+E32+F32+G32+H32+I32+J32+K32+L32+M32+N32+O32+P32</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1553,23 +1253,12 @@
         <v>46</v>
       </c>
       <c r="C33" s="5"/>
-      <c r="D33" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="13"/>
-      <c r="I33" s="13"/>
-      <c r="J33" s="13"/>
-      <c r="K33" s="13"/>
-      <c r="L33" s="13"/>
-      <c r="M33" s="13"/>
-      <c r="N33" s="13"/>
-      <c r="O33" s="13"/>
+      <c r="D33" t="b">
+        <v>1</v>
+      </c>
       <c r="P33" s="6"/>
       <c r="Q33" s="11">
-        <f>C33+D33+E33+F33+G33+H33+I33+J33+K33+L33+M33+N33+O33+P33</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1578,25 +1267,15 @@
         <v>39</v>
       </c>
       <c r="C34" s="5"/>
-      <c r="D34" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E34" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
-      <c r="H34" s="13"/>
-      <c r="I34" s="13"/>
-      <c r="J34" s="13"/>
-      <c r="K34" s="13"/>
-      <c r="L34" s="13"/>
-      <c r="M34" s="13"/>
-      <c r="N34" s="13"/>
-      <c r="O34" s="13"/>
+      <c r="D34" t="b">
+        <v>1</v>
+      </c>
+      <c r="E34" t="b">
+        <v>1</v>
+      </c>
       <c r="P34" s="6"/>
       <c r="Q34" s="11">
-        <f>C34+D34+E34+F34+G34+H34+I34+J34+K34+L34+M34+N34+O34+P34</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -1605,25 +1284,15 @@
         <v>30</v>
       </c>
       <c r="C35" s="5"/>
-      <c r="D35" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E35" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="13"/>
-      <c r="J35" s="13"/>
-      <c r="K35" s="13"/>
-      <c r="L35" s="13"/>
-      <c r="M35" s="13"/>
-      <c r="N35" s="13"/>
-      <c r="O35" s="13"/>
+      <c r="D35" t="b">
+        <v>1</v>
+      </c>
+      <c r="E35" t="b">
+        <v>1</v>
+      </c>
       <c r="P35" s="6"/>
       <c r="Q35" s="11">
-        <f>C35+D35+E35+F35+G35+H35+I35+J35+K35+L35+M35+N35+O35+P35</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -1632,25 +1301,15 @@
         <v>38</v>
       </c>
       <c r="C36" s="5"/>
-      <c r="D36" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E36" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="13"/>
-      <c r="I36" s="13"/>
-      <c r="J36" s="13"/>
-      <c r="K36" s="13"/>
-      <c r="L36" s="13"/>
-      <c r="M36" s="13"/>
-      <c r="N36" s="13"/>
-      <c r="O36" s="13"/>
+      <c r="D36" t="b">
+        <v>1</v>
+      </c>
+      <c r="E36" t="b">
+        <v>1</v>
+      </c>
       <c r="P36" s="6"/>
       <c r="Q36" s="11">
-        <f>C36+D36+E36+F36+G36+H36+I36+J36+K36+L36+M36+N36+O36+P36</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -1659,25 +1318,15 @@
         <v>41</v>
       </c>
       <c r="C37" s="5"/>
-      <c r="D37" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E37" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="13"/>
-      <c r="I37" s="13"/>
-      <c r="J37" s="13"/>
-      <c r="K37" s="13"/>
-      <c r="L37" s="13"/>
-      <c r="M37" s="13"/>
-      <c r="N37" s="13"/>
-      <c r="O37" s="13"/>
+      <c r="D37" t="b">
+        <v>1</v>
+      </c>
+      <c r="E37" t="b">
+        <v>1</v>
+      </c>
       <c r="P37" s="6"/>
       <c r="Q37" s="11">
-        <f>C37+D37+E37+F37+G37+H37+I37+J37+K37+L37+M37+N37+O37+P37</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -1686,23 +1335,12 @@
         <v>51</v>
       </c>
       <c r="C38" s="5"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="13"/>
-      <c r="I38" s="13"/>
-      <c r="J38" s="13"/>
-      <c r="K38" s="13"/>
-      <c r="L38" s="13"/>
-      <c r="M38" s="13"/>
-      <c r="N38" s="13"/>
-      <c r="O38" s="13"/>
+      <c r="E38" t="b">
+        <v>1</v>
+      </c>
       <c r="P38" s="6"/>
       <c r="Q38" s="11">
-        <f>C38+D38+E38+F38+G38+H38+I38+J38+K38+L38+M38+N38+O38+P38</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1727,7 +1365,7 @@
       <c r="O39" s="8"/>
       <c r="P39" s="9"/>
       <c r="Q39" s="11">
-        <f>C39+D39+E39+F39+G39+H39+I39+J39+K39+L39+M39+N39+O39+P39</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Laborator 21.03.2023 - am terminat jocul Minesweeper
</commit_message>
<xml_diff>
--- a/Prezenta.xlsx
+++ b/Prezenta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\AlgoritmiFundamentali_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB7C88F-C586-4D3F-994C-46DF2DE0CBBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{947B8B82-B356-487E-80A5-58AF10354CC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>Nume Prenume</t>
   </si>
@@ -184,6 +184,9 @@
   </si>
   <si>
     <t>Dumitrache Luca</t>
+  </si>
+  <si>
+    <t>Potcdan Ioana</t>
   </si>
 </sst>
 </file>
@@ -379,7 +382,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -399,6 +402,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -687,10 +691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:Q39"/>
+  <dimension ref="B2:Q40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U24" sqref="U24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -760,7 +764,9 @@
       <c r="E3" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="F3" s="3"/>
+      <c r="F3" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
@@ -772,8 +778,8 @@
       <c r="O3" s="3"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="11">
-        <f t="shared" ref="Q3:Q39" si="0">C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
-        <v>2</v>
+        <f>C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.3">
@@ -786,7 +792,7 @@
       </c>
       <c r="P4" s="6"/>
       <c r="Q4" s="11">
-        <f t="shared" si="0"/>
+        <f>C4+D4+E4+F4+G4+H4+I4+J4+K4+L4+M4+N4+O4+P4</f>
         <v>1</v>
       </c>
     </row>
@@ -798,10 +804,13 @@
       <c r="E5" t="b">
         <v>1</v>
       </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
       <c r="P5" s="6"/>
       <c r="Q5" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>C5+D5+E5+F5+G5+H5+I5+J5+K5+L5+M5+N5+O5+P5</f>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.3">
@@ -814,7 +823,7 @@
       </c>
       <c r="P6" s="6"/>
       <c r="Q6" s="11">
-        <f t="shared" si="0"/>
+        <f>C6+D6+E6+F6+G6+H6+I6+J6+K6+L6+M6+N6+O6+P6</f>
         <v>1</v>
       </c>
     </row>
@@ -829,10 +838,13 @@
       <c r="E7" t="b">
         <v>1</v>
       </c>
+      <c r="F7" t="b">
+        <v>1</v>
+      </c>
       <c r="P7" s="6"/>
       <c r="Q7" s="11">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C7+D7+E7+F7+G7+H7+I7+J7+K7+L7+M7+N7+O7+P7</f>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.3">
@@ -845,7 +857,7 @@
       </c>
       <c r="P8" s="6"/>
       <c r="Q8" s="11">
-        <f t="shared" si="0"/>
+        <f>C8+D8+E8+F8+G8+H8+I8+J8+K8+L8+M8+N8+O8+P8</f>
         <v>1</v>
       </c>
     </row>
@@ -859,7 +871,7 @@
       </c>
       <c r="P9" s="6"/>
       <c r="Q9" s="11">
-        <f t="shared" si="0"/>
+        <f>C9+D9+E9+F9+G9+H9+I9+J9+K9+L9+M9+N9+O9+P9</f>
         <v>1</v>
       </c>
     </row>
@@ -874,10 +886,13 @@
       <c r="E10" t="b">
         <v>1</v>
       </c>
+      <c r="F10" t="b">
+        <v>1</v>
+      </c>
       <c r="P10" s="6"/>
       <c r="Q10" s="11">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C10+D10+E10+F10+G10+H10+I10+J10+K10+L10+M10+N10+O10+P10</f>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.3">
@@ -895,7 +910,7 @@
       </c>
       <c r="P11" s="6"/>
       <c r="Q11" s="11">
-        <f t="shared" si="0"/>
+        <f>C11+D11+E11+F11+G11+H11+I11+J11+K11+L11+M11+N11+O11+P11</f>
         <v>3</v>
       </c>
     </row>
@@ -912,10 +927,13 @@
       <c r="E12" t="b">
         <v>1</v>
       </c>
+      <c r="F12" t="b">
+        <v>1</v>
+      </c>
       <c r="P12" s="6"/>
       <c r="Q12" s="11">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>C12+D12+E12+F12+G12+H12+I12+J12+K12+L12+M12+N12+O12+P12</f>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.3">
@@ -928,10 +946,13 @@
       <c r="D13" t="b">
         <v>1</v>
       </c>
+      <c r="F13" t="b">
+        <v>1</v>
+      </c>
       <c r="P13" s="6"/>
       <c r="Q13" s="11">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C13+D13+E13+F13+G13+H13+I13+J13+K13+L13+M13+N13+O13+P13</f>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.3">
@@ -947,10 +968,13 @@
       <c r="E14" t="b">
         <v>1</v>
       </c>
+      <c r="F14" t="b">
+        <v>1</v>
+      </c>
       <c r="P14" s="6"/>
       <c r="Q14" s="11">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>C14+D14+E14+F14+G14+H14+I14+J14+K14+L14+M14+N14+O14+P14</f>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.3">
@@ -966,10 +990,13 @@
       <c r="E15" t="b">
         <v>1</v>
       </c>
+      <c r="F15" t="b">
+        <v>1</v>
+      </c>
       <c r="P15" s="6"/>
       <c r="Q15" s="11">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>C15+D15+E15+F15+G15+H15+I15+J15+K15+L15+M15+N15+O15+P15</f>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.3">
@@ -987,7 +1014,7 @@
       </c>
       <c r="P16" s="6"/>
       <c r="Q16" s="11">
-        <f t="shared" si="0"/>
+        <f>C16+D16+E16+F16+G16+H16+I16+J16+K16+L16+M16+N16+O16+P16</f>
         <v>3</v>
       </c>
     </row>
@@ -998,10 +1025,13 @@
       <c r="C17" s="5" t="b">
         <v>1</v>
       </c>
+      <c r="F17" t="b">
+        <v>1</v>
+      </c>
       <c r="P17" s="6"/>
       <c r="Q17" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>C17+D17+E17+F17+G17+H17+I17+J17+K17+L17+M17+N17+O17+P17</f>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.3">
@@ -1017,10 +1047,13 @@
       <c r="E18" t="b">
         <v>1</v>
       </c>
+      <c r="F18" t="b">
+        <v>1</v>
+      </c>
       <c r="P18" s="6"/>
       <c r="Q18" s="11">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>C18+D18+E18+F18+G18+H18+I18+J18+K18+L18+M18+N18+O18+P18</f>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.3">
@@ -1033,10 +1066,13 @@
       <c r="D19" t="b">
         <v>1</v>
       </c>
+      <c r="F19" t="b">
+        <v>1</v>
+      </c>
       <c r="P19" s="6"/>
       <c r="Q19" s="11">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C19+D19+E19+F19+G19+H19+I19+J19+K19+L19+M19+N19+O19+P19</f>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.3">
@@ -1048,7 +1084,7 @@
       </c>
       <c r="P20" s="6"/>
       <c r="Q20" s="11">
-        <f t="shared" si="0"/>
+        <f>C20+D20+E20+F20+G20+H20+I20+J20+K20+L20+M20+N20+O20+P20</f>
         <v>1</v>
       </c>
     </row>
@@ -1065,10 +1101,13 @@
       <c r="E21" t="b">
         <v>1</v>
       </c>
+      <c r="F21" t="b">
+        <v>1</v>
+      </c>
       <c r="P21" s="6"/>
       <c r="Q21" s="11">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>C21+D21+E21+F21+G21+H21+I21+J21+K21+L21+M21+N21+O21+P21</f>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.3">
@@ -1081,64 +1120,73 @@
       </c>
       <c r="P22" s="6"/>
       <c r="Q22" s="11">
-        <f t="shared" si="0"/>
+        <f>C22+D22+E22+F22+G22+H22+I22+J22+K22+L22+M22+N22+O22+P22</f>
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B23" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E23" t="b">
-        <v>1</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="13"/>
       <c r="P23" s="6"/>
       <c r="Q23" s="11">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>C23+D23+E23+F23+G23+H23+I23+J23+K23+L23+M23+N23+O23+P23</f>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B24" s="10" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="C24" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D24" t="b">
+        <v>1</v>
+      </c>
+      <c r="E24" t="b">
+        <v>1</v>
+      </c>
+      <c r="F24" t="b">
         <v>1</v>
       </c>
       <c r="P24" s="6"/>
       <c r="Q24" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>C24+D24+E24+F24+G24+H24+I24+J24+K24+L24+M24+N24+O24+P24</f>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B25" s="10" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C25" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D25" t="b">
-        <v>1</v>
-      </c>
-      <c r="E25" t="b">
         <v>1</v>
       </c>
       <c r="P25" s="6"/>
       <c r="Q25" s="11">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>C25+D25+E25+F25+G25+H25+I25+J25+K25+L25+M25+N25+O25+P25</f>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B26" s="10" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="C26" s="5" t="b">
         <v>1</v>
@@ -1151,30 +1199,35 @@
       </c>
       <c r="P26" s="6"/>
       <c r="Q26" s="11">
-        <f t="shared" si="0"/>
+        <f>C26+D26+E26+F26+G26+H26+I26+J26+K26+L26+M26+N26+O26+P26</f>
         <v>3</v>
       </c>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B27" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C27" s="5"/>
+        <v>50</v>
+      </c>
+      <c r="C27" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="D27" t="b">
         <v>1</v>
       </c>
       <c r="E27" t="b">
+        <v>1</v>
+      </c>
+      <c r="F27" t="b">
         <v>1</v>
       </c>
       <c r="P27" s="6"/>
       <c r="Q27" s="11">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C27+D27+E27+F27+G27+H27+I27+J27+K27+L27+M27+N27+O27+P27</f>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B28" s="10" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" t="b">
@@ -1185,58 +1238,64 @@
       </c>
       <c r="P28" s="6"/>
       <c r="Q28" s="11">
-        <f t="shared" si="0"/>
+        <f>C28+D28+E28+F28+G28+H28+I28+J28+K28+L28+M28+N28+O28+P28</f>
         <v>2</v>
       </c>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B29" s="10" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" t="b">
         <v>1</v>
       </c>
+      <c r="E29" t="b">
+        <v>1</v>
+      </c>
+      <c r="F29" t="b">
+        <v>1</v>
+      </c>
       <c r="P29" s="6"/>
       <c r="Q29" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>C29+D29+E29+F29+G29+H29+I29+J29+K29+L29+M29+N29+O29+P29</f>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B30" s="10" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" t="b">
         <v>1</v>
       </c>
-      <c r="E30" t="b">
-        <v>1</v>
-      </c>
       <c r="P30" s="6"/>
       <c r="Q30" s="11">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C30+D30+E30+F30+G30+H30+I30+J30+K30+L30+M30+N30+O30+P30</f>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B31" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" t="b">
         <v>1</v>
       </c>
+      <c r="E31" t="b">
+        <v>1</v>
+      </c>
       <c r="P31" s="6"/>
       <c r="Q31" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>C31+D31+E31+F31+G31+H31+I31+J31+K31+L31+M31+N31+O31+P31</f>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B32" s="10" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" t="b">
@@ -1244,13 +1303,13 @@
       </c>
       <c r="P32" s="6"/>
       <c r="Q32" s="11">
-        <f t="shared" si="0"/>
+        <f>C32+D32+E32+F32+G32+H32+I32+J32+K32+L32+M32+N32+O32+P32</f>
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B33" s="10" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" t="b">
@@ -1258,30 +1317,27 @@
       </c>
       <c r="P33" s="6"/>
       <c r="Q33" s="11">
-        <f t="shared" si="0"/>
+        <f>C33+D33+E33+F33+G33+H33+I33+J33+K33+L33+M33+N33+O33+P33</f>
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B34" s="10" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" t="b">
         <v>1</v>
       </c>
-      <c r="E34" t="b">
-        <v>1</v>
-      </c>
       <c r="P34" s="6"/>
       <c r="Q34" s="11">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C34+D34+E34+F34+G34+H34+I34+J34+K34+L34+M34+N34+O34+P34</f>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B35" s="10" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" t="b">
@@ -1290,15 +1346,18 @@
       <c r="E35" t="b">
         <v>1</v>
       </c>
+      <c r="F35" t="b">
+        <v>1</v>
+      </c>
       <c r="P35" s="6"/>
       <c r="Q35" s="11">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C35+D35+E35+F35+G35+H35+I35+J35+K35+L35+M35+N35+O35+P35</f>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B36" s="10" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" t="b">
@@ -1307,15 +1366,18 @@
       <c r="E36" t="b">
         <v>1</v>
       </c>
+      <c r="F36" t="b">
+        <v>1</v>
+      </c>
       <c r="P36" s="6"/>
       <c r="Q36" s="11">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C36+D36+E36+F36+G36+H36+I36+J36+K36+L36+M36+N36+O36+P36</f>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B37" s="10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" t="b">
@@ -1324,56 +1386,76 @@
       <c r="E37" t="b">
         <v>1</v>
       </c>
+      <c r="F37" t="b">
+        <v>1</v>
+      </c>
       <c r="P37" s="6"/>
       <c r="Q37" s="11">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C37+D37+E37+F37+G37+H37+I37+J37+K37+L37+M37+N37+O37+P37</f>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B38" s="10" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C38" s="5"/>
+      <c r="D38" t="b">
+        <v>1</v>
+      </c>
       <c r="E38" t="b">
         <v>1</v>
       </c>
       <c r="P38" s="6"/>
       <c r="Q38" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>C38+D38+E38+F38+G38+H38+I38+J38+K38+L38+M38+N38+O38+P38</f>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B39" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C39" s="5"/>
+      <c r="E39" t="b">
+        <v>1</v>
+      </c>
+      <c r="P39" s="6"/>
+      <c r="Q39" s="11">
+        <f>C39+D39+E39+F39+G39+H39+I39+J39+K39+L39+M39+N39+O39+P39</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B40" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C39" s="7"/>
-      <c r="D39" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="8"/>
-      <c r="I39" s="8"/>
-      <c r="J39" s="8"/>
-      <c r="K39" s="8"/>
-      <c r="L39" s="8"/>
-      <c r="M39" s="8"/>
-      <c r="N39" s="8"/>
-      <c r="O39" s="8"/>
-      <c r="P39" s="9"/>
-      <c r="Q39" s="11">
-        <f t="shared" si="0"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="8"/>
+      <c r="J40" s="8"/>
+      <c r="K40" s="8"/>
+      <c r="L40" s="8"/>
+      <c r="M40" s="8"/>
+      <c r="N40" s="8"/>
+      <c r="O40" s="8"/>
+      <c r="P40" s="9"/>
+      <c r="Q40" s="11">
+        <f>C40+D40+E40+F40+G40+H40+I40+J40+K40+L40+M40+N40+O40+P40</f>
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:Q39">
-    <sortCondition ref="B3:B39"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:Q40">
+    <sortCondition ref="B40"/>
   </sortState>
-  <conditionalFormatting sqref="Q3:Q39">
+  <conditionalFormatting sqref="Q3:Q40">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
       <formula>4</formula>
     </cfRule>

</xml_diff>

<commit_message>
Laborator 23.03.2023 - Am discutat pe algoritmii deja existenti si pe unul nou - aflarea varfului maxim dintr-o lista de numere
</commit_message>
<xml_diff>
--- a/Prezenta.xlsx
+++ b/Prezenta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\AlgoritmiFundamentali_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{947B8B82-B356-487E-80A5-58AF10354CC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5243910B-DF60-4AAF-94EA-6AC9BCA48601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -382,7 +382,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -402,7 +402,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -693,8 +692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U24" sqref="U24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -778,7 +777,7 @@
       <c r="O3" s="3"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="11">
-        <f>C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
+        <f t="shared" ref="Q3:Q40" si="0">C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
         <v>3</v>
       </c>
     </row>
@@ -792,7 +791,7 @@
       </c>
       <c r="P4" s="6"/>
       <c r="Q4" s="11">
-        <f>C4+D4+E4+F4+G4+H4+I4+J4+K4+L4+M4+N4+O4+P4</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -809,7 +808,7 @@
       </c>
       <c r="P5" s="6"/>
       <c r="Q5" s="11">
-        <f>C5+D5+E5+F5+G5+H5+I5+J5+K5+L5+M5+N5+O5+P5</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -823,7 +822,7 @@
       </c>
       <c r="P6" s="6"/>
       <c r="Q6" s="11">
-        <f>C6+D6+E6+F6+G6+H6+I6+J6+K6+L6+M6+N6+O6+P6</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -843,7 +842,7 @@
       </c>
       <c r="P7" s="6"/>
       <c r="Q7" s="11">
-        <f>C7+D7+E7+F7+G7+H7+I7+J7+K7+L7+M7+N7+O7+P7</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -857,7 +856,7 @@
       </c>
       <c r="P8" s="6"/>
       <c r="Q8" s="11">
-        <f>C8+D8+E8+F8+G8+H8+I8+J8+K8+L8+M8+N8+O8+P8</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -871,7 +870,7 @@
       </c>
       <c r="P9" s="6"/>
       <c r="Q9" s="11">
-        <f>C9+D9+E9+F9+G9+H9+I9+J9+K9+L9+M9+N9+O9+P9</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -891,7 +890,7 @@
       </c>
       <c r="P10" s="6"/>
       <c r="Q10" s="11">
-        <f>C10+D10+E10+F10+G10+H10+I10+J10+K10+L10+M10+N10+O10+P10</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -908,10 +907,13 @@
       <c r="E11" t="b">
         <v>1</v>
       </c>
+      <c r="F11" t="b">
+        <v>1</v>
+      </c>
       <c r="P11" s="6"/>
       <c r="Q11" s="11">
-        <f>C11+D11+E11+F11+G11+H11+I11+J11+K11+L11+M11+N11+O11+P11</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.3">
@@ -932,7 +934,7 @@
       </c>
       <c r="P12" s="6"/>
       <c r="Q12" s="11">
-        <f>C12+D12+E12+F12+G12+H12+I12+J12+K12+L12+M12+N12+O12+P12</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -951,7 +953,7 @@
       </c>
       <c r="P13" s="6"/>
       <c r="Q13" s="11">
-        <f>C13+D13+E13+F13+G13+H13+I13+J13+K13+L13+M13+N13+O13+P13</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -973,7 +975,7 @@
       </c>
       <c r="P14" s="6"/>
       <c r="Q14" s="11">
-        <f>C14+D14+E14+F14+G14+H14+I14+J14+K14+L14+M14+N14+O14+P14</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -995,7 +997,7 @@
       </c>
       <c r="P15" s="6"/>
       <c r="Q15" s="11">
-        <f>C15+D15+E15+F15+G15+H15+I15+J15+K15+L15+M15+N15+O15+P15</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -1012,10 +1014,13 @@
       <c r="E16" t="b">
         <v>1</v>
       </c>
+      <c r="F16" t="b">
+        <v>1</v>
+      </c>
       <c r="P16" s="6"/>
       <c r="Q16" s="11">
-        <f>C16+D16+E16+F16+G16+H16+I16+J16+K16+L16+M16+N16+O16+P16</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.3">
@@ -1030,7 +1035,7 @@
       </c>
       <c r="P17" s="6"/>
       <c r="Q17" s="11">
-        <f>C17+D17+E17+F17+G17+H17+I17+J17+K17+L17+M17+N17+O17+P17</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -1052,7 +1057,7 @@
       </c>
       <c r="P18" s="6"/>
       <c r="Q18" s="11">
-        <f>C18+D18+E18+F18+G18+H18+I18+J18+K18+L18+M18+N18+O18+P18</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -1071,7 +1076,7 @@
       </c>
       <c r="P19" s="6"/>
       <c r="Q19" s="11">
-        <f>C19+D19+E19+F19+G19+H19+I19+J19+K19+L19+M19+N19+O19+P19</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -1084,7 +1089,7 @@
       </c>
       <c r="P20" s="6"/>
       <c r="Q20" s="11">
-        <f>C20+D20+E20+F20+G20+H20+I20+J20+K20+L20+M20+N20+O20+P20</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1106,7 +1111,7 @@
       </c>
       <c r="P21" s="6"/>
       <c r="Q21" s="11">
-        <f>C21+D21+E21+F21+G21+H21+I21+J21+K21+L21+M21+N21+O21+P21</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -1120,7 +1125,7 @@
       </c>
       <c r="P22" s="6"/>
       <c r="Q22" s="11">
-        <f>C22+D22+E22+F22+G22+H22+I22+J22+K22+L22+M22+N22+O22+P22</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1129,23 +1134,12 @@
         <v>53</v>
       </c>
       <c r="C23" s="5"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
-      <c r="O23" s="13"/>
+      <c r="F23" t="b">
+        <v>1</v>
+      </c>
       <c r="P23" s="6"/>
       <c r="Q23" s="11">
-        <f>C23+D23+E23+F23+G23+H23+I23+J23+K23+L23+M23+N23+O23+P23</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1167,7 +1161,7 @@
       </c>
       <c r="P24" s="6"/>
       <c r="Q24" s="11">
-        <f>C24+D24+E24+F24+G24+H24+I24+J24+K24+L24+M24+N24+O24+P24</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -1180,7 +1174,7 @@
       </c>
       <c r="P25" s="6"/>
       <c r="Q25" s="11">
-        <f>C25+D25+E25+F25+G25+H25+I25+J25+K25+L25+M25+N25+O25+P25</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1199,7 +1193,7 @@
       </c>
       <c r="P26" s="6"/>
       <c r="Q26" s="11">
-        <f>C26+D26+E26+F26+G26+H26+I26+J26+K26+L26+M26+N26+O26+P26</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -1221,7 +1215,7 @@
       </c>
       <c r="P27" s="6"/>
       <c r="Q27" s="11">
-        <f>C27+D27+E27+F27+G27+H27+I27+J27+K27+L27+M27+N27+O27+P27</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -1238,7 +1232,7 @@
       </c>
       <c r="P28" s="6"/>
       <c r="Q28" s="11">
-        <f>C28+D28+E28+F28+G28+H28+I28+J28+K28+L28+M28+N28+O28+P28</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -1258,7 +1252,7 @@
       </c>
       <c r="P29" s="6"/>
       <c r="Q29" s="11">
-        <f>C29+D29+E29+F29+G29+H29+I29+J29+K29+L29+M29+N29+O29+P29</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -1272,7 +1266,7 @@
       </c>
       <c r="P30" s="6"/>
       <c r="Q30" s="11">
-        <f>C30+D30+E30+F30+G30+H30+I30+J30+K30+L30+M30+N30+O30+P30</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1289,7 +1283,7 @@
       </c>
       <c r="P31" s="6"/>
       <c r="Q31" s="11">
-        <f>C31+D31+E31+F31+G31+H31+I31+J31+K31+L31+M31+N31+O31+P31</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -1303,7 +1297,7 @@
       </c>
       <c r="P32" s="6"/>
       <c r="Q32" s="11">
-        <f>C32+D32+E32+F32+G32+H32+I32+J32+K32+L32+M32+N32+O32+P32</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1317,7 +1311,7 @@
       </c>
       <c r="P33" s="6"/>
       <c r="Q33" s="11">
-        <f>C33+D33+E33+F33+G33+H33+I33+J33+K33+L33+M33+N33+O33+P33</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1331,7 +1325,7 @@
       </c>
       <c r="P34" s="6"/>
       <c r="Q34" s="11">
-        <f>C34+D34+E34+F34+G34+H34+I34+J34+K34+L34+M34+N34+O34+P34</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1351,7 +1345,7 @@
       </c>
       <c r="P35" s="6"/>
       <c r="Q35" s="11">
-        <f>C35+D35+E35+F35+G35+H35+I35+J35+K35+L35+M35+N35+O35+P35</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -1371,7 +1365,7 @@
       </c>
       <c r="P36" s="6"/>
       <c r="Q36" s="11">
-        <f>C36+D36+E36+F36+G36+H36+I36+J36+K36+L36+M36+N36+O36+P36</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -1391,7 +1385,7 @@
       </c>
       <c r="P37" s="6"/>
       <c r="Q37" s="11">
-        <f>C37+D37+E37+F37+G37+H37+I37+J37+K37+L37+M37+N37+O37+P37</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -1408,7 +1402,7 @@
       </c>
       <c r="P38" s="6"/>
       <c r="Q38" s="11">
-        <f>C38+D38+E38+F38+G38+H38+I38+J38+K38+L38+M38+N38+O38+P38</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -1422,7 +1416,7 @@
       </c>
       <c r="P39" s="6"/>
       <c r="Q39" s="11">
-        <f>C39+D39+E39+F39+G39+H39+I39+J39+K39+L39+M39+N39+O39+P39</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1447,7 +1441,7 @@
       <c r="O40" s="8"/>
       <c r="P40" s="9"/>
       <c r="Q40" s="11">
-        <f>C40+D40+E40+F40+G40+H40+I40+J40+K40+L40+M40+N40+O40+P40</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Laborator 28.03.2023 - Am creat jocul Shooter, in care apar niste inamici, ii putem impusca, si daca ies din ecran, am pierdut
</commit_message>
<xml_diff>
--- a/Prezenta.xlsx
+++ b/Prezenta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\AlgoritmiFundamentali_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5243910B-DF60-4AAF-94EA-6AC9BCA48601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C5241C0-9208-4954-A76D-4B41723512DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -692,8 +692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L36" sqref="L36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -766,7 +766,9 @@
       <c r="F3" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="G3" s="3"/>
+      <c r="G3" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
@@ -778,7 +780,7 @@
       <c r="P3" s="4"/>
       <c r="Q3" s="11">
         <f t="shared" ref="Q3:Q40" si="0">C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.3">
@@ -806,10 +808,13 @@
       <c r="F5" t="b">
         <v>1</v>
       </c>
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
       <c r="P5" s="6"/>
       <c r="Q5" s="11">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.3">
@@ -840,10 +845,13 @@
       <c r="F7" t="b">
         <v>1</v>
       </c>
+      <c r="G7" t="b">
+        <v>1</v>
+      </c>
       <c r="P7" s="6"/>
       <c r="Q7" s="11">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.3">
@@ -973,10 +981,13 @@
       <c r="F14" t="b">
         <v>1</v>
       </c>
+      <c r="G14" t="b">
+        <v>1</v>
+      </c>
       <c r="P14" s="6"/>
       <c r="Q14" s="11">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.3">
@@ -995,10 +1006,13 @@
       <c r="F15" t="b">
         <v>1</v>
       </c>
+      <c r="G15" t="b">
+        <v>1</v>
+      </c>
       <c r="P15" s="6"/>
       <c r="Q15" s="11">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.3">
@@ -1055,10 +1069,13 @@
       <c r="F18" t="b">
         <v>1</v>
       </c>
+      <c r="G18" t="b">
+        <v>1</v>
+      </c>
       <c r="P18" s="6"/>
       <c r="Q18" s="11">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.3">
@@ -1109,10 +1126,13 @@
       <c r="F21" t="b">
         <v>1</v>
       </c>
+      <c r="G21" t="b">
+        <v>1</v>
+      </c>
       <c r="P21" s="6"/>
       <c r="Q21" s="11">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.3">
@@ -1137,10 +1157,13 @@
       <c r="F23" t="b">
         <v>1</v>
       </c>
+      <c r="G23" t="b">
+        <v>1</v>
+      </c>
       <c r="P23" s="6"/>
       <c r="Q23" s="11">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.3">
@@ -1159,10 +1182,13 @@
       <c r="F24" t="b">
         <v>1</v>
       </c>
+      <c r="G24" t="b">
+        <v>1</v>
+      </c>
       <c r="P24" s="6"/>
       <c r="Q24" s="11">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.3">
@@ -1191,10 +1217,13 @@
       <c r="E26" t="b">
         <v>1</v>
       </c>
+      <c r="G26" t="b">
+        <v>1</v>
+      </c>
       <c r="P26" s="6"/>
       <c r="Q26" s="11">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.3">
@@ -1264,10 +1293,13 @@
       <c r="D30" t="b">
         <v>1</v>
       </c>
+      <c r="G30" t="b">
+        <v>1</v>
+      </c>
       <c r="P30" s="6"/>
       <c r="Q30" s="11">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.3">
@@ -1363,10 +1395,13 @@
       <c r="F36" t="b">
         <v>1</v>
       </c>
+      <c r="G36" t="b">
+        <v>1</v>
+      </c>
       <c r="P36" s="6"/>
       <c r="Q36" s="11">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="2:17" x14ac:dyDescent="0.3">
@@ -1383,10 +1418,13 @@
       <c r="F37" t="b">
         <v>1</v>
       </c>
+      <c r="G37" t="b">
+        <v>1</v>
+      </c>
       <c r="P37" s="6"/>
       <c r="Q37" s="11">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="2:17" x14ac:dyDescent="0.3">
@@ -1400,10 +1438,13 @@
       <c r="E38" t="b">
         <v>1</v>
       </c>
+      <c r="G38" t="b">
+        <v>1</v>
+      </c>
       <c r="P38" s="6"/>
       <c r="Q38" s="11">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="2:17" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Laborator 04.04.2023 - am terminat jocul shooter
</commit_message>
<xml_diff>
--- a/Prezenta.xlsx
+++ b/Prezenta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\AlgoritmiFundamentali_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C5241C0-9208-4954-A76D-4B41723512DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B765E102-0010-4288-9AB4-24A11BF66C7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -692,8 +692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L36" sqref="L36"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -769,7 +769,9 @@
       <c r="G3" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="H3" s="3"/>
+      <c r="H3" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
@@ -780,7 +782,7 @@
       <c r="P3" s="4"/>
       <c r="Q3" s="11">
         <f t="shared" ref="Q3:Q40" si="0">C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.3">
@@ -811,10 +813,13 @@
       <c r="G5" t="b">
         <v>1</v>
       </c>
+      <c r="H5" t="b">
+        <v>1</v>
+      </c>
       <c r="P5" s="6"/>
       <c r="Q5" s="11">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.3">
@@ -896,10 +901,13 @@
       <c r="F10" t="b">
         <v>1</v>
       </c>
+      <c r="H10" t="b">
+        <v>1</v>
+      </c>
       <c r="P10" s="6"/>
       <c r="Q10" s="11">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.3">
@@ -959,10 +967,13 @@
       <c r="F13" t="b">
         <v>1</v>
       </c>
+      <c r="H13" t="b">
+        <v>1</v>
+      </c>
       <c r="P13" s="6"/>
       <c r="Q13" s="11">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.3">
@@ -984,10 +995,13 @@
       <c r="G14" t="b">
         <v>1</v>
       </c>
+      <c r="H14" t="b">
+        <v>1</v>
+      </c>
       <c r="P14" s="6"/>
       <c r="Q14" s="11">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.3">
@@ -1009,10 +1023,13 @@
       <c r="G15" t="b">
         <v>1</v>
       </c>
+      <c r="H15" t="b">
+        <v>1</v>
+      </c>
       <c r="P15" s="6"/>
       <c r="Q15" s="11">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.3">
@@ -1047,10 +1064,13 @@
       <c r="F17" t="b">
         <v>1</v>
       </c>
+      <c r="H17" t="b">
+        <v>1</v>
+      </c>
       <c r="P17" s="6"/>
       <c r="Q17" s="11">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.3">
@@ -1072,10 +1092,13 @@
       <c r="G18" t="b">
         <v>1</v>
       </c>
+      <c r="H18" t="b">
+        <v>1</v>
+      </c>
       <c r="P18" s="6"/>
       <c r="Q18" s="11">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.3">
@@ -1129,10 +1152,13 @@
       <c r="G21" t="b">
         <v>1</v>
       </c>
+      <c r="H21" t="b">
+        <v>1</v>
+      </c>
       <c r="P21" s="6"/>
       <c r="Q21" s="11">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.3">
@@ -1185,10 +1211,13 @@
       <c r="G24" t="b">
         <v>1</v>
       </c>
+      <c r="H24" t="b">
+        <v>1</v>
+      </c>
       <c r="P24" s="6"/>
       <c r="Q24" s="11">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.3">
@@ -1220,10 +1249,13 @@
       <c r="G26" t="b">
         <v>1</v>
       </c>
+      <c r="H26" t="b">
+        <v>1</v>
+      </c>
       <c r="P26" s="6"/>
       <c r="Q26" s="11">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.3">
@@ -1242,10 +1274,16 @@
       <c r="F27" t="b">
         <v>1</v>
       </c>
+      <c r="G27" t="b">
+        <v>1</v>
+      </c>
+      <c r="H27" t="b">
+        <v>1</v>
+      </c>
       <c r="P27" s="6"/>
       <c r="Q27" s="11">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.3">
@@ -1259,10 +1297,13 @@
       <c r="E28" t="b">
         <v>1</v>
       </c>
+      <c r="H28" t="b">
+        <v>1</v>
+      </c>
       <c r="P28" s="6"/>
       <c r="Q28" s="11">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.3">
@@ -1279,10 +1320,13 @@
       <c r="F29" t="b">
         <v>1</v>
       </c>
+      <c r="H29" t="b">
+        <v>1</v>
+      </c>
       <c r="P29" s="6"/>
       <c r="Q29" s="11">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.3">
@@ -1296,10 +1340,13 @@
       <c r="G30" t="b">
         <v>1</v>
       </c>
+      <c r="H30" t="b">
+        <v>1</v>
+      </c>
       <c r="P30" s="6"/>
       <c r="Q30" s="11">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.3">
@@ -1398,10 +1445,13 @@
       <c r="G36" t="b">
         <v>1</v>
       </c>
+      <c r="H36" t="b">
+        <v>1</v>
+      </c>
       <c r="P36" s="6"/>
       <c r="Q36" s="11">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="2:17" x14ac:dyDescent="0.3">
@@ -1421,10 +1471,13 @@
       <c r="G37" t="b">
         <v>1</v>
       </c>
+      <c r="H37" t="b">
+        <v>1</v>
+      </c>
       <c r="P37" s="6"/>
       <c r="Q37" s="11">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="2:17" x14ac:dyDescent="0.3">
@@ -1441,10 +1494,13 @@
       <c r="G38" t="b">
         <v>1</v>
       </c>
+      <c r="H38" t="b">
+        <v>1</v>
+      </c>
       <c r="P38" s="6"/>
       <c r="Q38" s="11">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="2:17" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Laborator 11.04.2023 - HTML CSS
</commit_message>
<xml_diff>
--- a/Prezenta.xlsx
+++ b/Prezenta.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\AlgoritmiFundamentali_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B86380-54C6-4E46-8E53-84AA3DC17C73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBED17D7-38F2-4748-808A-9B7424F968E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>Nume Prenume</t>
   </si>
@@ -159,9 +159,6 @@
     <t>Mura Mihai</t>
   </si>
   <si>
-    <t>Stroiescu Raul</t>
-  </si>
-  <si>
     <t>Lucuta Stefan</t>
   </si>
   <si>
@@ -187,6 +184,15 @@
   </si>
   <si>
     <t>Potcdan Ioana</t>
+  </si>
+  <si>
+    <t>Bumb Tudor</t>
+  </si>
+  <si>
+    <t>Stroescu Raul</t>
+  </si>
+  <si>
+    <t>Bucsa Andrei</t>
   </si>
 </sst>
 </file>
@@ -382,7 +388,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -402,6 +408,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -690,10 +699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:Q40"/>
+  <dimension ref="B2:Q42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -754,7 +763,7 @@
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B3" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="3" t="b">
@@ -772,7 +781,9 @@
       <c r="H3" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="I3" s="3"/>
+      <c r="I3" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -781,787 +792,1184 @@
       <c r="O3" s="3"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="11">
-        <f t="shared" ref="Q3:Q40" si="0">C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
-        <v>5</v>
+        <f>C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B4" s="10" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="C4" s="5"/>
-      <c r="D4" t="b">
-        <v>1</v>
-      </c>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
       <c r="P4" s="6"/>
       <c r="Q4" s="11">
-        <f t="shared" si="0"/>
+        <f>C4+D4+E4+F4+G4+H4+I4+J4+K4+L4+M4+N4+O4+P4</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B5" s="10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C5" s="5"/>
-      <c r="E5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F5" t="b">
-        <v>1</v>
-      </c>
-      <c r="G5" t="b">
-        <v>1</v>
-      </c>
-      <c r="H5" t="b">
-        <v>1</v>
-      </c>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
       <c r="P5" s="6"/>
       <c r="Q5" s="11">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f>C5+D5+E5+F5+G5+H5+I5+J5+K5+L5+M5+N5+O5+P5</f>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B6" s="10" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="C6" s="5"/>
-      <c r="D6" t="b">
-        <v>1</v>
-      </c>
+      <c r="D6" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
       <c r="P6" s="6"/>
       <c r="Q6" s="11">
-        <f t="shared" si="0"/>
+        <f>C6+D6+E6+F6+G6+H6+I6+J6+K6+L6+M6+N6+O6+P6</f>
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B7" s="10" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="C7" s="5"/>
-      <c r="D7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G7" t="b">
-        <v>1</v>
-      </c>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I7" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
       <c r="P7" s="6"/>
       <c r="Q7" s="11">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f>C7+D7+E7+F7+G7+H7+I7+J7+K7+L7+M7+N7+O7+P7</f>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B8" s="10" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C8" s="5"/>
-      <c r="D8" t="b">
-        <v>1</v>
-      </c>
+      <c r="D8" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
       <c r="P8" s="6"/>
       <c r="Q8" s="11">
-        <f t="shared" si="0"/>
+        <f>C8+D8+E8+F8+G8+H8+I8+J8+K8+L8+M8+N8+O8+P8</f>
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C9" s="5"/>
-      <c r="D9" t="b">
-        <v>1</v>
-      </c>
+      <c r="D9" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" s="13"/>
+      <c r="I9" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
       <c r="P9" s="6"/>
       <c r="Q9" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>C9+D9+E9+F9+G9+H9+I9+J9+K9+L9+M9+N9+O9+P9</f>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B10" s="10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C10" s="5"/>
-      <c r="D10" t="b">
-        <v>1</v>
-      </c>
-      <c r="E10" t="b">
-        <v>1</v>
-      </c>
-      <c r="F10" t="b">
-        <v>1</v>
-      </c>
-      <c r="H10" t="b">
-        <v>1</v>
-      </c>
+      <c r="D10" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
       <c r="P10" s="6"/>
       <c r="Q10" s="11">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f>C10+D10+E10+F10+G10+H10+I10+J10+K10+L10+M10+N10+O10+P10</f>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B11" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D11" t="b">
-        <v>1</v>
-      </c>
-      <c r="E11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F11" t="b">
-        <v>1</v>
-      </c>
-      <c r="G11" t="b">
-        <v>1</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
       <c r="P11" s="6"/>
       <c r="Q11" s="11">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f>C11+D11+E11+F11+G11+H11+I11+J11+K11+L11+M11+N11+O11+P11</f>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B12" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D12" t="b">
-        <v>1</v>
-      </c>
-      <c r="E12" t="b">
-        <v>1</v>
-      </c>
-      <c r="F12" t="b">
-        <v>1</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E12" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F12" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I12" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
       <c r="P12" s="6"/>
       <c r="Q12" s="11">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f>C12+D12+E12+F12+G12+H12+I12+J12+K12+L12+M12+N12+O12+P12</f>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B13" s="10" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C13" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H13" t="b">
-        <v>1</v>
-      </c>
+      <c r="D13" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
       <c r="P13" s="6"/>
       <c r="Q13" s="11">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f>C13+D13+E13+F13+G13+H13+I13+J13+K13+L13+M13+N13+O13+P13</f>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B14" s="10" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C14" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D14" t="b">
-        <v>1</v>
-      </c>
-      <c r="E14" t="b">
-        <v>1</v>
-      </c>
-      <c r="F14" t="b">
-        <v>1</v>
-      </c>
-      <c r="G14" t="b">
-        <v>1</v>
-      </c>
-      <c r="H14" t="b">
-        <v>1</v>
-      </c>
+      <c r="D14" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F14" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
       <c r="P14" s="6"/>
       <c r="Q14" s="11">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f>C14+D14+E14+F14+G14+H14+I14+J14+K14+L14+M14+N14+O14+P14</f>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B15" s="10" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C15" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D15" t="b">
-        <v>1</v>
-      </c>
-      <c r="E15" t="b">
-        <v>1</v>
-      </c>
-      <c r="F15" t="b">
-        <v>1</v>
-      </c>
-      <c r="G15" t="b">
-        <v>1</v>
-      </c>
-      <c r="H15" t="b">
-        <v>1</v>
-      </c>
+      <c r="D15" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
       <c r="P15" s="6"/>
       <c r="Q15" s="11">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f>C15+D15+E15+F15+G15+H15+I15+J15+K15+L15+M15+N15+O15+P15</f>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B16" s="10" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="C16" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D16" t="b">
-        <v>1</v>
-      </c>
-      <c r="E16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F16" t="b">
-        <v>1</v>
-      </c>
-      <c r="G16" t="b">
-        <v>1</v>
-      </c>
+      <c r="D16" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E16" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F16" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G16" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
+      <c r="O16" s="13"/>
       <c r="P16" s="6"/>
       <c r="Q16" s="11">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f>C16+D16+E16+F16+G16+H16+I16+J16+K16+L16+M16+N16+O16+P16</f>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B17" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="F17" t="b">
-        <v>1</v>
-      </c>
-      <c r="H17" t="b">
-        <v>1</v>
-      </c>
+      <c r="D17" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F17" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G17" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H17" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I17" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="13"/>
       <c r="P17" s="6"/>
       <c r="Q17" s="11">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>C17+D17+E17+F17+G17+H17+I17+J17+K17+L17+M17+N17+O17+P17</f>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B18" s="10" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C18" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D18" t="b">
-        <v>1</v>
-      </c>
-      <c r="E18" t="b">
-        <v>1</v>
-      </c>
-      <c r="F18" t="b">
-        <v>1</v>
-      </c>
-      <c r="G18" t="b">
-        <v>1</v>
-      </c>
-      <c r="H18" t="b">
-        <v>1</v>
-      </c>
+      <c r="D18" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E18" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F18" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G18" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="13"/>
+      <c r="O18" s="13"/>
       <c r="P18" s="6"/>
       <c r="Q18" s="11">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f>C18+D18+E18+F18+G18+H18+I18+J18+K18+L18+M18+N18+O18+P18</f>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B19" s="10" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C19" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D19" t="b">
-        <v>1</v>
-      </c>
-      <c r="F19" t="b">
-        <v>1</v>
-      </c>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="13"/>
       <c r="P19" s="6"/>
       <c r="Q19" s="11">
-        <f t="shared" si="0"/>
+        <f>C19+D19+E19+F19+G19+H19+I19+J19+K19+L19+M19+N19+O19+P19</f>
         <v>3</v>
       </c>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B20" s="10" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C20" s="5" t="b">
         <v>1</v>
       </c>
+      <c r="D20" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E20" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F20" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G20" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
       <c r="P20" s="6"/>
       <c r="Q20" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>C20+D20+E20+F20+G20+H20+I20+J20+K20+L20+M20+N20+O20+P20</f>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B21" s="10" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C21" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D21" t="b">
-        <v>1</v>
-      </c>
-      <c r="E21" t="b">
-        <v>1</v>
-      </c>
-      <c r="F21" t="b">
-        <v>1</v>
-      </c>
-      <c r="G21" t="b">
-        <v>1</v>
-      </c>
-      <c r="H21" t="b">
-        <v>1</v>
-      </c>
+      <c r="D21" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13"/>
       <c r="P21" s="6"/>
       <c r="Q21" s="11">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f>C21+D21+E21+F21+G21+H21+I21+J21+K21+L21+M21+N21+O21+P21</f>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B22" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" s="5"/>
-      <c r="D22" t="b">
-        <v>1</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="C22" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="13"/>
       <c r="P22" s="6"/>
       <c r="Q22" s="11">
-        <f t="shared" si="0"/>
+        <f>C22+D22+E22+F22+G22+H22+I22+J22+K22+L22+M22+N22+O22+P22</f>
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B23" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C23" s="5"/>
-      <c r="F23" t="b">
-        <v>1</v>
-      </c>
-      <c r="G23" t="b">
-        <v>1</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="C23" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E23" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F23" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G23" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H23" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I23" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="13"/>
       <c r="P23" s="6"/>
       <c r="Q23" s="11">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C23+D23+E23+F23+G23+H23+I23+J23+K23+L23+M23+N23+O23+P23</f>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B24" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D24" t="b">
-        <v>1</v>
-      </c>
-      <c r="E24" t="b">
-        <v>1</v>
-      </c>
-      <c r="F24" t="b">
-        <v>1</v>
-      </c>
-      <c r="G24" t="b">
-        <v>1</v>
-      </c>
-      <c r="H24" t="b">
-        <v>1</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="13"/>
+      <c r="N24" s="13"/>
+      <c r="O24" s="13"/>
       <c r="P24" s="6"/>
       <c r="Q24" s="11">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f>C24+D24+E24+F24+G24+H24+I24+J24+K24+L24+M24+N24+O24+P24</f>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B25" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C25" s="5" t="b">
-        <v>1</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="C25" s="5"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G25" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="13"/>
+      <c r="N25" s="13"/>
+      <c r="O25" s="13"/>
       <c r="P25" s="6"/>
       <c r="Q25" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>C25+D25+E25+F25+G25+H25+I25+J25+K25+L25+M25+N25+O25+P25</f>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B26" s="10" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C26" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D26" t="b">
-        <v>1</v>
-      </c>
-      <c r="E26" t="b">
-        <v>1</v>
-      </c>
-      <c r="G26" t="b">
-        <v>1</v>
-      </c>
-      <c r="H26" t="b">
-        <v>1</v>
-      </c>
+      <c r="D26" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E26" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F26" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G26" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H26" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I26" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="13"/>
+      <c r="N26" s="13"/>
+      <c r="O26" s="13"/>
       <c r="P26" s="6"/>
       <c r="Q26" s="11">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f>C26+D26+E26+F26+G26+H26+I26+J26+K26+L26+M26+N26+O26+P26</f>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B27" s="10" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="C27" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D27" t="b">
-        <v>1</v>
-      </c>
-      <c r="E27" t="b">
-        <v>1</v>
-      </c>
-      <c r="F27" t="b">
-        <v>1</v>
-      </c>
-      <c r="G27" t="b">
-        <v>1</v>
-      </c>
-      <c r="H27" t="b">
-        <v>1</v>
-      </c>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="13"/>
+      <c r="O27" s="13"/>
       <c r="P27" s="6"/>
       <c r="Q27" s="11">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f>C27+D27+E27+F27+G27+H27+I27+J27+K27+L27+M27+N27+O27+P27</f>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B28" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C28" s="5"/>
-      <c r="D28" t="b">
-        <v>1</v>
-      </c>
-      <c r="E28" t="b">
-        <v>1</v>
-      </c>
-      <c r="G28" t="b">
-        <v>1</v>
-      </c>
-      <c r="H28" t="b">
-        <v>1</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="C28" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D28" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E28" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H28" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="13"/>
+      <c r="N28" s="13"/>
+      <c r="O28" s="13"/>
       <c r="P28" s="6"/>
       <c r="Q28" s="11">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f>C28+D28+E28+F28+G28+H28+I28+J28+K28+L28+M28+N28+O28+P28</f>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B29" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C29" s="5"/>
-      <c r="D29" t="b">
-        <v>1</v>
-      </c>
-      <c r="E29" t="b">
-        <v>1</v>
-      </c>
-      <c r="F29" t="b">
-        <v>1</v>
-      </c>
-      <c r="H29" t="b">
-        <v>1</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="C29" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D29" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E29" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F29" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G29" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H29" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13"/>
+      <c r="M29" s="13"/>
+      <c r="N29" s="13"/>
+      <c r="O29" s="13"/>
       <c r="P29" s="6"/>
       <c r="Q29" s="11">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f>C29+D29+E29+F29+G29+H29+I29+J29+K29+L29+M29+N29+O29+P29</f>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B30" s="10" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C30" s="5"/>
-      <c r="D30" t="b">
-        <v>1</v>
-      </c>
-      <c r="G30" t="b">
-        <v>1</v>
-      </c>
-      <c r="H30" t="b">
-        <v>1</v>
-      </c>
+      <c r="D30" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E30" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H30" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I30" s="13"/>
+      <c r="J30" s="13"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13"/>
+      <c r="M30" s="13"/>
+      <c r="N30" s="13"/>
+      <c r="O30" s="13"/>
       <c r="P30" s="6"/>
       <c r="Q30" s="11">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>C30+D30+E30+F30+G30+H30+I30+J30+K30+L30+M30+N30+O30+P30</f>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B31" s="10" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="C31" s="5"/>
-      <c r="D31" t="b">
-        <v>1</v>
-      </c>
-      <c r="E31" t="b">
-        <v>1</v>
-      </c>
-      <c r="G31" t="b">
-        <v>1</v>
-      </c>
+      <c r="D31" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E31" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F31" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I31" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
+      <c r="M31" s="13"/>
+      <c r="N31" s="13"/>
+      <c r="O31" s="13"/>
       <c r="P31" s="6"/>
       <c r="Q31" s="11">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>C31+D31+E31+F31+G31+H31+I31+J31+K31+L31+M31+N31+O31+P31</f>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B32" s="10" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="C32" s="5"/>
-      <c r="D32" t="b">
-        <v>1</v>
-      </c>
+      <c r="D32" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H32" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I32" s="13"/>
+      <c r="J32" s="13"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="13"/>
+      <c r="N32" s="13"/>
+      <c r="O32" s="13"/>
       <c r="P32" s="6"/>
       <c r="Q32" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>C32+D32+E32+F32+G32+H32+I32+J32+K32+L32+M32+N32+O32+P32</f>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B33" s="10" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="C33" s="5"/>
-      <c r="D33" t="b">
-        <v>1</v>
-      </c>
+      <c r="D33" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E33" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="13"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="13"/>
+      <c r="M33" s="13"/>
+      <c r="N33" s="13"/>
+      <c r="O33" s="13"/>
       <c r="P33" s="6"/>
       <c r="Q33" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>C33+D33+E33+F33+G33+H33+I33+J33+K33+L33+M33+N33+O33+P33</f>
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B34" s="10" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="C34" s="5"/>
-      <c r="D34" t="b">
-        <v>1</v>
-      </c>
+      <c r="D34" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="13"/>
+      <c r="M34" s="13"/>
+      <c r="N34" s="13"/>
+      <c r="O34" s="13"/>
       <c r="P34" s="6"/>
       <c r="Q34" s="11">
-        <f t="shared" si="0"/>
+        <f>C34+D34+E34+F34+G34+H34+I34+J34+K34+L34+M34+N34+O34+P34</f>
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B35" s="10" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C35" s="5"/>
-      <c r="D35" t="b">
-        <v>1</v>
-      </c>
-      <c r="E35" t="b">
-        <v>1</v>
-      </c>
-      <c r="F35" t="b">
-        <v>1</v>
-      </c>
-      <c r="G35" t="b">
-        <v>1</v>
-      </c>
+      <c r="D35" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="13"/>
+      <c r="K35" s="13"/>
+      <c r="L35" s="13"/>
+      <c r="M35" s="13"/>
+      <c r="N35" s="13"/>
+      <c r="O35" s="13"/>
       <c r="P35" s="6"/>
       <c r="Q35" s="11">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f>C35+D35+E35+F35+G35+H35+I35+J35+K35+L35+M35+N35+O35+P35</f>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B36" s="10" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="C36" s="5"/>
-      <c r="D36" t="b">
-        <v>1</v>
-      </c>
-      <c r="E36" t="b">
-        <v>1</v>
-      </c>
-      <c r="F36" t="b">
-        <v>1</v>
-      </c>
-      <c r="G36" t="b">
-        <v>1</v>
-      </c>
-      <c r="H36" t="b">
-        <v>1</v>
-      </c>
+      <c r="D36" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="13"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
+      <c r="M36" s="13"/>
+      <c r="N36" s="13"/>
+      <c r="O36" s="13"/>
       <c r="P36" s="6"/>
       <c r="Q36" s="11">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f>C36+D36+E36+F36+G36+H36+I36+J36+K36+L36+M36+N36+O36+P36</f>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B37" s="10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C37" s="5"/>
-      <c r="D37" t="b">
-        <v>1</v>
-      </c>
-      <c r="E37" t="b">
-        <v>1</v>
-      </c>
-      <c r="F37" t="b">
-        <v>1</v>
-      </c>
-      <c r="G37" t="b">
-        <v>1</v>
-      </c>
-      <c r="H37" t="b">
-        <v>1</v>
-      </c>
+      <c r="D37" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E37" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F37" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G37" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H37" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I37" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="J37" s="13"/>
+      <c r="K37" s="13"/>
+      <c r="L37" s="13"/>
+      <c r="M37" s="13"/>
+      <c r="N37" s="13"/>
+      <c r="O37" s="13"/>
       <c r="P37" s="6"/>
       <c r="Q37" s="11">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f>C37+D37+E37+F37+G37+H37+I37+J37+K37+L37+M37+N37+O37+P37</f>
+        <v>6</v>
       </c>
     </row>
     <row r="38" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B38" s="10" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="C38" s="5"/>
-      <c r="D38" t="b">
-        <v>1</v>
-      </c>
-      <c r="E38" t="b">
-        <v>1</v>
-      </c>
-      <c r="G38" t="b">
-        <v>1</v>
-      </c>
-      <c r="H38" t="b">
-        <v>1</v>
-      </c>
+      <c r="D38" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E38" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F38" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G38" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H38" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I38" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="J38" s="13"/>
+      <c r="K38" s="13"/>
+      <c r="L38" s="13"/>
+      <c r="M38" s="13"/>
+      <c r="N38" s="13"/>
+      <c r="O38" s="13"/>
       <c r="P38" s="6"/>
       <c r="Q38" s="11">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f>C38+D38+E38+F38+G38+H38+I38+J38+K38+L38+M38+N38+O38+P38</f>
+        <v>6</v>
       </c>
     </row>
     <row r="39" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B39" s="10" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="C39" s="5"/>
-      <c r="E39" t="b">
-        <v>1</v>
-      </c>
+      <c r="D39" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E39" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F39" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G39" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H39" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I39" s="13"/>
+      <c r="J39" s="13"/>
+      <c r="K39" s="13"/>
+      <c r="L39" s="13"/>
+      <c r="M39" s="13"/>
+      <c r="N39" s="13"/>
+      <c r="O39" s="13"/>
       <c r="P39" s="6"/>
       <c r="Q39" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>C39+D39+E39+F39+G39+H39+I39+J39+K39+L39+M39+N39+O39+P39</f>
+        <v>5</v>
       </c>
     </row>
     <row r="40" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B40" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C40" s="5"/>
+      <c r="D40" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E40" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H40" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I40" s="13"/>
+      <c r="J40" s="13"/>
+      <c r="K40" s="13"/>
+      <c r="L40" s="13"/>
+      <c r="M40" s="13"/>
+      <c r="N40" s="13"/>
+      <c r="O40" s="13"/>
+      <c r="P40" s="6"/>
+      <c r="Q40" s="11">
+        <f>C40+D40+E40+F40+G40+H40+I40+J40+K40+L40+M40+N40+O40+P40</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B41" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C41" s="5"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="13"/>
+      <c r="I41" s="13"/>
+      <c r="J41" s="13"/>
+      <c r="K41" s="13"/>
+      <c r="L41" s="13"/>
+      <c r="M41" s="13"/>
+      <c r="N41" s="13"/>
+      <c r="O41" s="13"/>
+      <c r="P41" s="6"/>
+      <c r="Q41" s="11">
+        <f>C41+D41+E41+F41+G41+H41+I41+J41+K41+L41+M41+N41+O41+P41</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B42" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C40" s="7"/>
-      <c r="D40" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
-      <c r="I40" s="8"/>
-      <c r="J40" s="8"/>
-      <c r="K40" s="8"/>
-      <c r="L40" s="8"/>
-      <c r="M40" s="8"/>
-      <c r="N40" s="8"/>
-      <c r="O40" s="8"/>
-      <c r="P40" s="9"/>
-      <c r="Q40" s="11">
-        <f t="shared" si="0"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
+      <c r="J42" s="8"/>
+      <c r="K42" s="8"/>
+      <c r="L42" s="8"/>
+      <c r="M42" s="8"/>
+      <c r="N42" s="8"/>
+      <c r="O42" s="8"/>
+      <c r="P42" s="9"/>
+      <c r="Q42" s="11">
+        <f>C42+D42+E42+F42+G42+H42+I42+J42+K42+L42+M42+N42+O42+P42</f>
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:Q40">
-    <sortCondition ref="B40"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:Q42">
+    <sortCondition ref="B3:B42"/>
   </sortState>
-  <conditionalFormatting sqref="Q3:Q40">
+  <conditionalFormatting sqref="Q3:Q42">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
       <formula>4</formula>
     </cfRule>

</xml_diff>

<commit_message>
Laborator 13.04.2023 - mai multe modele de matrici
</commit_message>
<xml_diff>
--- a/Prezenta.xlsx
+++ b/Prezenta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\AlgoritmiFundamentali_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBED17D7-38F2-4748-808A-9B7424F968E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECCD8CC8-1B51-4E57-9448-3166C9A995B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -388,7 +388,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -408,9 +408,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -702,7 +700,7 @@
   <dimension ref="B2:Q42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -792,7 +790,7 @@
       <c r="O3" s="3"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="11">
-        <f>C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
+        <f t="shared" ref="Q3:Q42" si="0">C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
         <v>6</v>
       </c>
     </row>
@@ -801,23 +799,12 @@
         <v>55</v>
       </c>
       <c r="C4" s="5"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
+      <c r="I4" t="b">
+        <v>1</v>
+      </c>
       <c r="P4" s="6"/>
       <c r="Q4" s="11">
-        <f>C4+D4+E4+F4+G4+H4+I4+J4+K4+L4+M4+N4+O4+P4</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -826,23 +813,12 @@
         <v>53</v>
       </c>
       <c r="C5" s="5"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
+      <c r="I5" t="b">
+        <v>1</v>
+      </c>
       <c r="P5" s="6"/>
       <c r="Q5" s="11">
-        <f>C5+D5+E5+F5+G5+H5+I5+J5+K5+L5+M5+N5+O5+P5</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -851,23 +827,12 @@
         <v>35</v>
       </c>
       <c r="C6" s="5"/>
-      <c r="D6" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
       <c r="P6" s="6"/>
       <c r="Q6" s="11">
-        <f>C6+D6+E6+F6+G6+H6+I6+J6+K6+L6+M6+N6+O6+P6</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -876,31 +841,24 @@
         <v>51</v>
       </c>
       <c r="C7" s="5"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F7" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G7" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H7" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I7" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" t="b">
+        <v>1</v>
+      </c>
+      <c r="I7" t="b">
+        <v>1</v>
+      </c>
       <c r="P7" s="6"/>
       <c r="Q7" s="11">
-        <f>C7+D7+E7+F7+G7+H7+I7+J7+K7+L7+M7+N7+O7+P7</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -909,23 +867,12 @@
         <v>46</v>
       </c>
       <c r="C8" s="5"/>
-      <c r="D8" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13"/>
+      <c r="D8" t="b">
+        <v>1</v>
+      </c>
       <c r="P8" s="6"/>
       <c r="Q8" s="11">
-        <f>C8+D8+E8+F8+G8+H8+I8+J8+K8+L8+M8+N8+O8+P8</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -934,31 +881,24 @@
         <v>36</v>
       </c>
       <c r="C9" s="5"/>
-      <c r="D9" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E9" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F9" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G9" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H9" s="13"/>
-      <c r="I9" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="13"/>
+      <c r="D9" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9" t="b">
+        <v>1</v>
+      </c>
+      <c r="I9" t="b">
+        <v>1</v>
+      </c>
       <c r="P9" s="6"/>
       <c r="Q9" s="11">
-        <f>C9+D9+E9+F9+G9+H9+I9+J9+K9+L9+M9+N9+O9+P9</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -967,23 +907,12 @@
         <v>40</v>
       </c>
       <c r="C10" s="5"/>
-      <c r="D10" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13"/>
+      <c r="D10" t="b">
+        <v>1</v>
+      </c>
       <c r="P10" s="6"/>
       <c r="Q10" s="11">
-        <f>C10+D10+E10+F10+G10+H10+I10+J10+K10+L10+M10+N10+O10+P10</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -992,23 +921,12 @@
         <v>44</v>
       </c>
       <c r="C11" s="5"/>
-      <c r="D11" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="13"/>
+      <c r="D11" t="b">
+        <v>1</v>
+      </c>
       <c r="P11" s="6"/>
       <c r="Q11" s="11">
-        <f>C11+D11+E11+F11+G11+H11+I11+J11+K11+L11+M11+N11+O11+P11</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1017,31 +935,24 @@
         <v>43</v>
       </c>
       <c r="C12" s="5"/>
-      <c r="D12" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E12" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F12" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I12" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
-      <c r="N12" s="13"/>
-      <c r="O12" s="13"/>
+      <c r="D12" t="b">
+        <v>1</v>
+      </c>
+      <c r="E12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I12" t="b">
+        <v>1</v>
+      </c>
       <c r="P12" s="6"/>
       <c r="Q12" s="11">
-        <f>C12+D12+E12+F12+G12+H12+I12+J12+K12+L12+M12+N12+O12+P12</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -1052,29 +963,21 @@
       <c r="C13" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D13" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E13" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F13" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G13" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
-      <c r="O13" s="13"/>
+      <c r="D13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13" t="b">
+        <v>1</v>
+      </c>
       <c r="P13" s="6"/>
       <c r="Q13" s="11">
-        <f>C13+D13+E13+F13+G13+H13+I13+J13+K13+L13+M13+N13+O13+P13</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -1085,29 +988,21 @@
       <c r="C14" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D14" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E14" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F14" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
-      <c r="N14" s="13"/>
-      <c r="O14" s="13"/>
+      <c r="D14" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14" t="b">
+        <v>1</v>
+      </c>
+      <c r="F14" t="b">
+        <v>1</v>
+      </c>
+      <c r="I14" t="b">
+        <v>1</v>
+      </c>
       <c r="P14" s="6"/>
       <c r="Q14" s="11">
-        <f>C14+D14+E14+F14+G14+H14+I14+J14+K14+L14+M14+N14+O14+P14</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -1118,27 +1013,18 @@
       <c r="C15" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D15" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="13"/>
-      <c r="O15" s="13"/>
+      <c r="D15" t="b">
+        <v>1</v>
+      </c>
+      <c r="F15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H15" t="b">
+        <v>1</v>
+      </c>
       <c r="P15" s="6"/>
       <c r="Q15" s="11">
-        <f>C15+D15+E15+F15+G15+H15+I15+J15+K15+L15+M15+N15+O15+P15</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -1149,31 +1035,24 @@
       <c r="C16" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D16" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E16" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F16" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G16" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H16" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="13"/>
-      <c r="N16" s="13"/>
-      <c r="O16" s="13"/>
+      <c r="D16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16" t="b">
+        <v>1</v>
+      </c>
       <c r="P16" s="6"/>
       <c r="Q16" s="11">
-        <f>C16+D16+E16+F16+G16+H16+I16+J16+K16+L16+M16+N16+O16+P16</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
@@ -1184,33 +1063,27 @@
       <c r="C17" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D17" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E17" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F17" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G17" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H17" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I17" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="13"/>
-      <c r="O17" s="13"/>
+      <c r="D17" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17" t="b">
+        <v>1</v>
+      </c>
+      <c r="F17" t="b">
+        <v>1</v>
+      </c>
+      <c r="G17" t="b">
+        <v>1</v>
+      </c>
+      <c r="H17" t="b">
+        <v>1</v>
+      </c>
+      <c r="I17" t="b">
+        <v>1</v>
+      </c>
       <c r="P17" s="6"/>
       <c r="Q17" s="11">
-        <f>C17+D17+E17+F17+G17+H17+I17+J17+K17+L17+M17+N17+O17+P17</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
@@ -1221,29 +1094,21 @@
       <c r="C18" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D18" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E18" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F18" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G18" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
-      <c r="N18" s="13"/>
-      <c r="O18" s="13"/>
+      <c r="D18" t="b">
+        <v>1</v>
+      </c>
+      <c r="E18" t="b">
+        <v>1</v>
+      </c>
+      <c r="F18" t="b">
+        <v>1</v>
+      </c>
+      <c r="G18" t="b">
+        <v>1</v>
+      </c>
       <c r="P18" s="6"/>
       <c r="Q18" s="11">
-        <f>C18+D18+E18+F18+G18+H18+I18+J18+K18+L18+M18+N18+O18+P18</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -1254,25 +1119,15 @@
       <c r="C19" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
-      <c r="N19" s="13"/>
-      <c r="O19" s="13"/>
+      <c r="F19" t="b">
+        <v>1</v>
+      </c>
+      <c r="H19" t="b">
+        <v>1</v>
+      </c>
       <c r="P19" s="6"/>
       <c r="Q19" s="11">
-        <f>C19+D19+E19+F19+G19+H19+I19+J19+K19+L19+M19+N19+O19+P19</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -1283,31 +1138,24 @@
       <c r="C20" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D20" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E20" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F20" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G20" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H20" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="13"/>
-      <c r="O20" s="13"/>
+      <c r="D20" t="b">
+        <v>1</v>
+      </c>
+      <c r="E20" t="b">
+        <v>1</v>
+      </c>
+      <c r="F20" t="b">
+        <v>1</v>
+      </c>
+      <c r="G20" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20" t="b">
+        <v>1</v>
+      </c>
       <c r="P20" s="6"/>
       <c r="Q20" s="11">
-        <f>C20+D20+E20+F20+G20+H20+I20+J20+K20+L20+M20+N20+O20+P20</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
@@ -1318,25 +1166,15 @@
       <c r="C21" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D21" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
-      <c r="N21" s="13"/>
-      <c r="O21" s="13"/>
+      <c r="D21" t="b">
+        <v>1</v>
+      </c>
+      <c r="F21" t="b">
+        <v>1</v>
+      </c>
       <c r="P21" s="6"/>
       <c r="Q21" s="11">
-        <f>C21+D21+E21+F21+G21+H21+I21+J21+K21+L21+M21+N21+O21+P21</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -1347,21 +1185,9 @@
       <c r="C22" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
-      <c r="O22" s="13"/>
       <c r="P22" s="6"/>
       <c r="Q22" s="11">
-        <f>C22+D22+E22+F22+G22+H22+I22+J22+K22+L22+M22+N22+O22+P22</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1372,33 +1198,27 @@
       <c r="C23" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D23" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E23" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F23" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G23" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H23" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I23" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
-      <c r="O23" s="13"/>
+      <c r="D23" t="b">
+        <v>1</v>
+      </c>
+      <c r="E23" t="b">
+        <v>1</v>
+      </c>
+      <c r="F23" t="b">
+        <v>1</v>
+      </c>
+      <c r="G23" t="b">
+        <v>1</v>
+      </c>
+      <c r="H23" t="b">
+        <v>1</v>
+      </c>
+      <c r="I23" t="b">
+        <v>1</v>
+      </c>
       <c r="P23" s="6"/>
       <c r="Q23" s="11">
-        <f>C23+D23+E23+F23+G23+H23+I23+J23+K23+L23+M23+N23+O23+P23</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
@@ -1407,23 +1227,12 @@
         <v>33</v>
       </c>
       <c r="C24" s="5"/>
-      <c r="D24" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="13"/>
-      <c r="M24" s="13"/>
-      <c r="N24" s="13"/>
-      <c r="O24" s="13"/>
+      <c r="D24" t="b">
+        <v>1</v>
+      </c>
       <c r="P24" s="6"/>
       <c r="Q24" s="11">
-        <f>C24+D24+E24+F24+G24+H24+I24+J24+K24+L24+M24+N24+O24+P24</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1432,25 +1241,15 @@
         <v>52</v>
       </c>
       <c r="C25" s="5"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G25" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="13"/>
-      <c r="N25" s="13"/>
-      <c r="O25" s="13"/>
+      <c r="F25" t="b">
+        <v>1</v>
+      </c>
+      <c r="G25" t="b">
+        <v>1</v>
+      </c>
       <c r="P25" s="6"/>
       <c r="Q25" s="11">
-        <f>C25+D25+E25+F25+G25+H25+I25+J25+K25+L25+M25+N25+O25+P25</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -1461,33 +1260,27 @@
       <c r="C26" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D26" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E26" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F26" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G26" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H26" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I26" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="J26" s="13"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="13"/>
-      <c r="M26" s="13"/>
-      <c r="N26" s="13"/>
-      <c r="O26" s="13"/>
+      <c r="D26" t="b">
+        <v>1</v>
+      </c>
+      <c r="E26" t="b">
+        <v>1</v>
+      </c>
+      <c r="F26" t="b">
+        <v>1</v>
+      </c>
+      <c r="G26" t="b">
+        <v>1</v>
+      </c>
+      <c r="H26" t="b">
+        <v>1</v>
+      </c>
+      <c r="I26" t="b">
+        <v>1</v>
+      </c>
       <c r="P26" s="6"/>
       <c r="Q26" s="11">
-        <f>C26+D26+E26+F26+G26+H26+I26+J26+K26+L26+M26+N26+O26+P26</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
@@ -1498,21 +1291,9 @@
       <c r="C27" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="13"/>
-      <c r="K27" s="13"/>
-      <c r="L27" s="13"/>
-      <c r="M27" s="13"/>
-      <c r="N27" s="13"/>
-      <c r="O27" s="13"/>
       <c r="P27" s="6"/>
       <c r="Q27" s="11">
-        <f>C27+D27+E27+F27+G27+H27+I27+J27+K27+L27+M27+N27+O27+P27</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1523,29 +1304,21 @@
       <c r="C28" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D28" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E28" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H28" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I28" s="13"/>
-      <c r="J28" s="13"/>
-      <c r="K28" s="13"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="13"/>
-      <c r="N28" s="13"/>
-      <c r="O28" s="13"/>
+      <c r="D28" t="b">
+        <v>1</v>
+      </c>
+      <c r="E28" t="b">
+        <v>1</v>
+      </c>
+      <c r="G28" t="b">
+        <v>1</v>
+      </c>
+      <c r="H28" t="b">
+        <v>1</v>
+      </c>
       <c r="P28" s="6"/>
       <c r="Q28" s="11">
-        <f>C28+D28+E28+F28+G28+H28+I28+J28+K28+L28+M28+N28+O28+P28</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -1556,31 +1329,24 @@
       <c r="C29" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D29" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E29" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F29" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G29" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H29" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I29" s="13"/>
-      <c r="J29" s="13"/>
-      <c r="K29" s="13"/>
-      <c r="L29" s="13"/>
-      <c r="M29" s="13"/>
-      <c r="N29" s="13"/>
-      <c r="O29" s="13"/>
+      <c r="D29" t="b">
+        <v>1</v>
+      </c>
+      <c r="E29" t="b">
+        <v>1</v>
+      </c>
+      <c r="F29" t="b">
+        <v>1</v>
+      </c>
+      <c r="G29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H29" t="b">
+        <v>1</v>
+      </c>
       <c r="P29" s="6"/>
       <c r="Q29" s="11">
-        <f>C29+D29+E29+F29+G29+H29+I29+J29+K29+L29+M29+N29+O29+P29</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
@@ -1589,30 +1355,25 @@
         <v>34</v>
       </c>
       <c r="C30" s="5"/>
-      <c r="D30" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E30" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H30" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I30" s="13"/>
-      <c r="J30" s="13"/>
-      <c r="K30" s="13"/>
-      <c r="L30" s="13"/>
-      <c r="M30" s="13"/>
-      <c r="N30" s="13"/>
-      <c r="O30" s="13"/>
+      <c r="D30" t="b">
+        <v>1</v>
+      </c>
+      <c r="E30" t="b">
+        <v>1</v>
+      </c>
+      <c r="G30" t="b">
+        <v>1</v>
+      </c>
+      <c r="H30" t="b">
+        <v>1</v>
+      </c>
+      <c r="I30" t="b">
+        <v>1</v>
+      </c>
       <c r="P30" s="6"/>
       <c r="Q30" s="11">
-        <f>C30+D30+E30+F30+G30+H30+I30+J30+K30+L30+M30+N30+O30+P30</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.3">
@@ -1620,31 +1381,24 @@
         <v>54</v>
       </c>
       <c r="C31" s="5"/>
-      <c r="D31" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E31" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F31" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G31" s="13"/>
-      <c r="H31" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I31" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="J31" s="13"/>
-      <c r="K31" s="13"/>
-      <c r="L31" s="13"/>
-      <c r="M31" s="13"/>
-      <c r="N31" s="13"/>
-      <c r="O31" s="13"/>
+      <c r="D31" t="b">
+        <v>1</v>
+      </c>
+      <c r="E31" t="b">
+        <v>1</v>
+      </c>
+      <c r="F31" t="b">
+        <v>1</v>
+      </c>
+      <c r="H31" t="b">
+        <v>1</v>
+      </c>
+      <c r="I31" t="b">
+        <v>1</v>
+      </c>
       <c r="P31" s="6"/>
       <c r="Q31" s="11">
-        <f>C31+D31+E31+F31+G31+H31+I31+J31+K31+L31+M31+N31+O31+P31</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -1653,27 +1407,18 @@
         <v>42</v>
       </c>
       <c r="C32" s="5"/>
-      <c r="D32" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H32" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I32" s="13"/>
-      <c r="J32" s="13"/>
-      <c r="K32" s="13"/>
-      <c r="L32" s="13"/>
-      <c r="M32" s="13"/>
-      <c r="N32" s="13"/>
-      <c r="O32" s="13"/>
+      <c r="D32" t="b">
+        <v>1</v>
+      </c>
+      <c r="G32" t="b">
+        <v>1</v>
+      </c>
+      <c r="H32" t="b">
+        <v>1</v>
+      </c>
       <c r="P32" s="6"/>
       <c r="Q32" s="11">
-        <f>C32+D32+E32+F32+G32+H32+I32+J32+K32+L32+M32+N32+O32+P32</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -1682,27 +1427,18 @@
         <v>31</v>
       </c>
       <c r="C33" s="5"/>
-      <c r="D33" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E33" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H33" s="13"/>
-      <c r="I33" s="13"/>
-      <c r="J33" s="13"/>
-      <c r="K33" s="13"/>
-      <c r="L33" s="13"/>
-      <c r="M33" s="13"/>
-      <c r="N33" s="13"/>
-      <c r="O33" s="13"/>
+      <c r="D33" t="b">
+        <v>1</v>
+      </c>
+      <c r="E33" t="b">
+        <v>1</v>
+      </c>
+      <c r="G33" t="b">
+        <v>1</v>
+      </c>
       <c r="P33" s="6"/>
       <c r="Q33" s="11">
-        <f>C33+D33+E33+F33+G33+H33+I33+J33+K33+L33+M33+N33+O33+P33</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -1711,23 +1447,12 @@
         <v>32</v>
       </c>
       <c r="C34" s="5"/>
-      <c r="D34" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
-      <c r="H34" s="13"/>
-      <c r="I34" s="13"/>
-      <c r="J34" s="13"/>
-      <c r="K34" s="13"/>
-      <c r="L34" s="13"/>
-      <c r="M34" s="13"/>
-      <c r="N34" s="13"/>
-      <c r="O34" s="13"/>
+      <c r="D34" t="b">
+        <v>1</v>
+      </c>
       <c r="P34" s="6"/>
       <c r="Q34" s="11">
-        <f>C34+D34+E34+F34+G34+H34+I34+J34+K34+L34+M34+N34+O34+P34</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1736,23 +1461,12 @@
         <v>47</v>
       </c>
       <c r="C35" s="5"/>
-      <c r="D35" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="13"/>
-      <c r="J35" s="13"/>
-      <c r="K35" s="13"/>
-      <c r="L35" s="13"/>
-      <c r="M35" s="13"/>
-      <c r="N35" s="13"/>
-      <c r="O35" s="13"/>
+      <c r="D35" t="b">
+        <v>1</v>
+      </c>
       <c r="P35" s="6"/>
       <c r="Q35" s="11">
-        <f>C35+D35+E35+F35+G35+H35+I35+J35+K35+L35+M35+N35+O35+P35</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1761,23 +1475,12 @@
         <v>45</v>
       </c>
       <c r="C36" s="5"/>
-      <c r="D36" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="13"/>
-      <c r="I36" s="13"/>
-      <c r="J36" s="13"/>
-      <c r="K36" s="13"/>
-      <c r="L36" s="13"/>
-      <c r="M36" s="13"/>
-      <c r="N36" s="13"/>
-      <c r="O36" s="13"/>
+      <c r="D36" t="b">
+        <v>1</v>
+      </c>
       <c r="P36" s="6"/>
       <c r="Q36" s="11">
-        <f>C36+D36+E36+F36+G36+H36+I36+J36+K36+L36+M36+N36+O36+P36</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1786,33 +1489,27 @@
         <v>39</v>
       </c>
       <c r="C37" s="5"/>
-      <c r="D37" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E37" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F37" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G37" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H37" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I37" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="J37" s="13"/>
-      <c r="K37" s="13"/>
-      <c r="L37" s="13"/>
-      <c r="M37" s="13"/>
-      <c r="N37" s="13"/>
-      <c r="O37" s="13"/>
+      <c r="D37" t="b">
+        <v>1</v>
+      </c>
+      <c r="E37" t="b">
+        <v>1</v>
+      </c>
+      <c r="F37" t="b">
+        <v>1</v>
+      </c>
+      <c r="G37" t="b">
+        <v>1</v>
+      </c>
+      <c r="H37" t="b">
+        <v>1</v>
+      </c>
+      <c r="I37" t="b">
+        <v>1</v>
+      </c>
       <c r="P37" s="6"/>
       <c r="Q37" s="11">
-        <f>C37+D37+E37+F37+G37+H37+I37+J37+K37+L37+M37+N37+O37+P37</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
@@ -1821,33 +1518,27 @@
         <v>30</v>
       </c>
       <c r="C38" s="5"/>
-      <c r="D38" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E38" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F38" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G38" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H38" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I38" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="J38" s="13"/>
-      <c r="K38" s="13"/>
-      <c r="L38" s="13"/>
-      <c r="M38" s="13"/>
-      <c r="N38" s="13"/>
-      <c r="O38" s="13"/>
+      <c r="D38" t="b">
+        <v>1</v>
+      </c>
+      <c r="E38" t="b">
+        <v>1</v>
+      </c>
+      <c r="F38" t="b">
+        <v>1</v>
+      </c>
+      <c r="G38" t="b">
+        <v>1</v>
+      </c>
+      <c r="H38" t="b">
+        <v>1</v>
+      </c>
+      <c r="I38" t="b">
+        <v>1</v>
+      </c>
       <c r="P38" s="6"/>
       <c r="Q38" s="11">
-        <f>C38+D38+E38+F38+G38+H38+I38+J38+K38+L38+M38+N38+O38+P38</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
@@ -1856,31 +1547,24 @@
         <v>38</v>
       </c>
       <c r="C39" s="5"/>
-      <c r="D39" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E39" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F39" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G39" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H39" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I39" s="13"/>
-      <c r="J39" s="13"/>
-      <c r="K39" s="13"/>
-      <c r="L39" s="13"/>
-      <c r="M39" s="13"/>
-      <c r="N39" s="13"/>
-      <c r="O39" s="13"/>
+      <c r="D39" t="b">
+        <v>1</v>
+      </c>
+      <c r="E39" t="b">
+        <v>1</v>
+      </c>
+      <c r="F39" t="b">
+        <v>1</v>
+      </c>
+      <c r="G39" t="b">
+        <v>1</v>
+      </c>
+      <c r="H39" t="b">
+        <v>1</v>
+      </c>
       <c r="P39" s="6"/>
       <c r="Q39" s="11">
-        <f>C39+D39+E39+F39+G39+H39+I39+J39+K39+L39+M39+N39+O39+P39</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -1889,29 +1573,21 @@
         <v>41</v>
       </c>
       <c r="C40" s="5"/>
-      <c r="D40" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E40" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F40" s="13"/>
-      <c r="G40" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H40" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I40" s="13"/>
-      <c r="J40" s="13"/>
-      <c r="K40" s="13"/>
-      <c r="L40" s="13"/>
-      <c r="M40" s="13"/>
-      <c r="N40" s="13"/>
-      <c r="O40" s="13"/>
+      <c r="D40" t="b">
+        <v>1</v>
+      </c>
+      <c r="E40" t="b">
+        <v>1</v>
+      </c>
+      <c r="G40" t="b">
+        <v>1</v>
+      </c>
+      <c r="H40" t="b">
+        <v>1</v>
+      </c>
       <c r="P40" s="6"/>
       <c r="Q40" s="11">
-        <f>C40+D40+E40+F40+G40+H40+I40+J40+K40+L40+M40+N40+O40+P40</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -1920,28 +1596,17 @@
         <v>50</v>
       </c>
       <c r="C41" s="5"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F41" s="13"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="13"/>
-      <c r="I41" s="13"/>
-      <c r="J41" s="13"/>
-      <c r="K41" s="13"/>
-      <c r="L41" s="13"/>
-      <c r="M41" s="13"/>
-      <c r="N41" s="13"/>
-      <c r="O41" s="13"/>
+      <c r="E41" t="b">
+        <v>1</v>
+      </c>
       <c r="P41" s="6"/>
       <c r="Q41" s="11">
-        <f>C41+D41+E41+F41+G41+H41+I41+J41+K41+L41+M41+N41+O41+P41</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B42" s="14" t="s">
+      <c r="B42" s="13" t="s">
         <v>37</v>
       </c>
       <c r="C42" s="7"/>
@@ -1961,7 +1626,7 @@
       <c r="O42" s="8"/>
       <c r="P42" s="9"/>
       <c r="Q42" s="11">
-        <f>C42+D42+E42+F42+G42+H42+I42+J42+K42+L42+M42+N42+O42+P42</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Laborator 27.04.2023 - problemele de la partial
</commit_message>
<xml_diff>
--- a/Prezenta.xlsx
+++ b/Prezenta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\AlgoritmiFundamentali_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{226D3BAD-DE3B-4C05-B2F2-332B509AB17F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D83D0C0-5901-49AC-89D1-5A87ECE6BCB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>Nume Prenume</t>
   </si>
@@ -193,6 +193,9 @@
   </si>
   <si>
     <t>Bucsa Andrei</t>
+  </si>
+  <si>
+    <t>Rotund Vasile</t>
   </si>
 </sst>
 </file>
@@ -408,7 +411,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -697,10 +700,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:Q42"/>
+  <dimension ref="B2:Q43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -792,7 +795,7 @@
       <c r="O3" s="3"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="11">
-        <f t="shared" ref="Q3:Q42" si="0">C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
+        <f>C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
         <v>7</v>
       </c>
     </row>
@@ -801,15 +804,25 @@
         <v>55</v>
       </c>
       <c r="C4" s="5"/>
-      <c r="I4" t="b">
-        <v>1</v>
-      </c>
-      <c r="J4" t="b">
-        <v>1</v>
-      </c>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
       <c r="P4" s="6"/>
       <c r="Q4" s="11">
-        <f t="shared" si="0"/>
+        <f>C4+D4+E4+F4+G4+H4+I4+J4+K4+L4+M4+N4+O4+P4</f>
         <v>2</v>
       </c>
     </row>
@@ -818,15 +831,25 @@
         <v>53</v>
       </c>
       <c r="C5" s="5"/>
-      <c r="I5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J5" t="b">
-        <v>1</v>
-      </c>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
       <c r="P5" s="6"/>
       <c r="Q5" s="11">
-        <f t="shared" si="0"/>
+        <f>C5+D5+E5+F5+G5+H5+I5+J5+K5+L5+M5+N5+O5+P5</f>
         <v>2</v>
       </c>
     </row>
@@ -835,12 +858,23 @@
         <v>35</v>
       </c>
       <c r="C6" s="5"/>
-      <c r="D6" t="b">
-        <v>1</v>
-      </c>
+      <c r="D6" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
       <c r="P6" s="6"/>
       <c r="Q6" s="11">
-        <f t="shared" si="0"/>
+        <f>C6+D6+E6+F6+G6+H6+I6+J6+K6+L6+M6+N6+O6+P6</f>
         <v>1</v>
       </c>
     </row>
@@ -849,27 +883,33 @@
         <v>51</v>
       </c>
       <c r="C7" s="5"/>
-      <c r="E7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G7" t="b">
-        <v>1</v>
-      </c>
-      <c r="H7" t="b">
-        <v>1</v>
-      </c>
-      <c r="I7" t="b">
-        <v>1</v>
-      </c>
-      <c r="J7" t="b">
-        <v>1</v>
-      </c>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I7" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="J7" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
       <c r="P7" s="6"/>
       <c r="Q7" s="11">
-        <f t="shared" si="0"/>
+        <f>C7+D7+E7+F7+G7+H7+I7+J7+K7+L7+M7+N7+O7+P7</f>
         <v>6</v>
       </c>
     </row>
@@ -878,12 +918,23 @@
         <v>46</v>
       </c>
       <c r="C8" s="5"/>
-      <c r="D8" t="b">
-        <v>1</v>
-      </c>
+      <c r="D8" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
       <c r="P8" s="6"/>
       <c r="Q8" s="11">
-        <f t="shared" si="0"/>
+        <f>C8+D8+E8+F8+G8+H8+I8+J8+K8+L8+M8+N8+O8+P8</f>
         <v>1</v>
       </c>
     </row>
@@ -892,24 +943,31 @@
         <v>36</v>
       </c>
       <c r="C9" s="5"/>
-      <c r="D9" t="b">
-        <v>1</v>
-      </c>
-      <c r="E9" t="b">
-        <v>1</v>
-      </c>
-      <c r="F9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G9" t="b">
-        <v>1</v>
-      </c>
-      <c r="I9" t="b">
-        <v>1</v>
-      </c>
+      <c r="D9" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
       <c r="P9" s="6"/>
       <c r="Q9" s="11">
-        <f t="shared" si="0"/>
+        <f>C9+D9+E9+F9+G9+H9+I9+J9+K9+L9+M9+N9+O9+P9</f>
         <v>5</v>
       </c>
     </row>
@@ -918,12 +976,23 @@
         <v>40</v>
       </c>
       <c r="C10" s="5"/>
-      <c r="D10" t="b">
-        <v>1</v>
-      </c>
+      <c r="D10" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
       <c r="P10" s="6"/>
       <c r="Q10" s="11">
-        <f t="shared" si="0"/>
+        <f>C10+D10+E10+F10+G10+H10+I10+J10+K10+L10+M10+N10+O10+P10</f>
         <v>1</v>
       </c>
     </row>
@@ -932,15 +1001,25 @@
         <v>44</v>
       </c>
       <c r="C11" s="5"/>
-      <c r="D11" t="b">
-        <v>1</v>
-      </c>
-      <c r="J11" t="b">
-        <v>1</v>
-      </c>
+      <c r="D11" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
       <c r="P11" s="6"/>
       <c r="Q11" s="11">
-        <f t="shared" si="0"/>
+        <f>C11+D11+E11+F11+G11+H11+I11+J11+K11+L11+M11+N11+O11+P11</f>
         <v>2</v>
       </c>
     </row>
@@ -949,24 +1028,31 @@
         <v>43</v>
       </c>
       <c r="C12" s="5"/>
-      <c r="D12" t="b">
-        <v>1</v>
-      </c>
-      <c r="E12" t="b">
-        <v>1</v>
-      </c>
-      <c r="F12" t="b">
-        <v>1</v>
-      </c>
-      <c r="H12" t="b">
-        <v>1</v>
-      </c>
-      <c r="I12" t="b">
-        <v>1</v>
-      </c>
+      <c r="D12" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E12" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F12" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I12" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
       <c r="P12" s="6"/>
       <c r="Q12" s="11">
-        <f t="shared" si="0"/>
+        <f>C12+D12+E12+F12+G12+H12+I12+J12+K12+L12+M12+N12+O12+P12</f>
         <v>5</v>
       </c>
     </row>
@@ -977,24 +1063,31 @@
       <c r="C13" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G13" t="b">
-        <v>1</v>
-      </c>
-      <c r="J13" t="b">
-        <v>1</v>
-      </c>
+      <c r="D13" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
       <c r="P13" s="6"/>
       <c r="Q13" s="11">
-        <f t="shared" si="0"/>
+        <f>C13+D13+E13+F13+G13+H13+I13+J13+K13+L13+M13+N13+O13+P13</f>
         <v>6</v>
       </c>
     </row>
@@ -1005,24 +1098,31 @@
       <c r="C14" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D14" t="b">
-        <v>1</v>
-      </c>
-      <c r="E14" t="b">
-        <v>1</v>
-      </c>
-      <c r="F14" t="b">
-        <v>1</v>
-      </c>
-      <c r="I14" t="b">
-        <v>1</v>
-      </c>
-      <c r="J14" t="b">
-        <v>1</v>
-      </c>
+      <c r="D14" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F14" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="J14" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
       <c r="P14" s="6"/>
       <c r="Q14" s="11">
-        <f t="shared" si="0"/>
+        <f>C14+D14+E14+F14+G14+H14+I14+J14+K14+L14+M14+N14+O14+P14</f>
         <v>6</v>
       </c>
     </row>
@@ -1033,21 +1133,29 @@
       <c r="C15" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D15" t="b">
-        <v>1</v>
-      </c>
-      <c r="F15" t="b">
-        <v>1</v>
-      </c>
-      <c r="H15" t="b">
-        <v>1</v>
-      </c>
-      <c r="J15" t="b">
-        <v>1</v>
-      </c>
+      <c r="D15" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
       <c r="P15" s="6"/>
       <c r="Q15" s="11">
-        <f t="shared" si="0"/>
+        <f>C15+D15+E15+F15+G15+H15+I15+J15+K15+L15+M15+N15+O15+P15</f>
         <v>5</v>
       </c>
     </row>
@@ -1058,24 +1166,31 @@
       <c r="C16" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D16" t="b">
-        <v>1</v>
-      </c>
-      <c r="E16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F16" t="b">
-        <v>1</v>
-      </c>
-      <c r="G16" t="b">
-        <v>1</v>
-      </c>
-      <c r="H16" t="b">
-        <v>1</v>
-      </c>
+      <c r="D16" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E16" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F16" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G16" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
+      <c r="O16" s="13"/>
       <c r="P16" s="6"/>
       <c r="Q16" s="11">
-        <f t="shared" si="0"/>
+        <f>C16+D16+E16+F16+G16+H16+I16+J16+K16+L16+M16+N16+O16+P16</f>
         <v>6</v>
       </c>
     </row>
@@ -1086,30 +1201,35 @@
       <c r="C17" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D17" t="b">
-        <v>1</v>
-      </c>
-      <c r="E17" t="b">
-        <v>1</v>
-      </c>
-      <c r="F17" t="b">
-        <v>1</v>
-      </c>
-      <c r="G17" t="b">
-        <v>1</v>
-      </c>
-      <c r="H17" t="b">
-        <v>1</v>
-      </c>
-      <c r="I17" t="b">
-        <v>1</v>
-      </c>
-      <c r="J17" t="b">
-        <v>1</v>
-      </c>
+      <c r="D17" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F17" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G17" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H17" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I17" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="J17" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="13"/>
       <c r="P17" s="6"/>
       <c r="Q17" s="11">
-        <f t="shared" si="0"/>
+        <f>C17+D17+E17+F17+G17+H17+I17+J17+K17+L17+M17+N17+O17+P17</f>
         <v>8</v>
       </c>
     </row>
@@ -1120,22 +1240,32 @@
       <c r="C18" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D18" t="b">
-        <v>1</v>
-      </c>
-      <c r="E18" t="b">
-        <v>1</v>
-      </c>
-      <c r="F18" t="b">
-        <v>1</v>
-      </c>
-      <c r="G18" t="b">
-        <v>1</v>
-      </c>
+      <c r="D18" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E18" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F18" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G18" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="13"/>
+      <c r="O18" s="13"/>
       <c r="P18" s="6"/>
       <c r="Q18" s="11">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f>C18+D18+E18+F18+G18+H18+I18+J18+K18+L18+M18+N18+O18+P18</f>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.3">
@@ -1145,15 +1275,25 @@
       <c r="C19" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="F19" t="b">
-        <v>1</v>
-      </c>
-      <c r="H19" t="b">
-        <v>1</v>
-      </c>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="13"/>
       <c r="P19" s="6"/>
       <c r="Q19" s="11">
-        <f t="shared" si="0"/>
+        <f>C19+D19+E19+F19+G19+H19+I19+J19+K19+L19+M19+N19+O19+P19</f>
         <v>3</v>
       </c>
     </row>
@@ -1164,27 +1304,33 @@
       <c r="C20" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D20" t="b">
-        <v>1</v>
-      </c>
-      <c r="E20" t="b">
-        <v>1</v>
-      </c>
-      <c r="F20" t="b">
-        <v>1</v>
-      </c>
-      <c r="G20" t="b">
-        <v>1</v>
-      </c>
-      <c r="H20" t="b">
-        <v>1</v>
-      </c>
-      <c r="J20" t="b">
-        <v>1</v>
-      </c>
+      <c r="D20" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E20" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F20" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G20" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
       <c r="P20" s="6"/>
       <c r="Q20" s="11">
-        <f t="shared" si="0"/>
+        <f>C20+D20+E20+F20+G20+H20+I20+J20+K20+L20+M20+N20+O20+P20</f>
         <v>7</v>
       </c>
     </row>
@@ -1195,18 +1341,27 @@
       <c r="C21" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D21" t="b">
-        <v>1</v>
-      </c>
-      <c r="F21" t="b">
-        <v>1</v>
-      </c>
-      <c r="J21" t="b">
-        <v>1</v>
-      </c>
+      <c r="D21" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13"/>
       <c r="P21" s="6"/>
       <c r="Q21" s="11">
-        <f t="shared" si="0"/>
+        <f>C21+D21+E21+F21+G21+H21+I21+J21+K21+L21+M21+N21+O21+P21</f>
         <v>4</v>
       </c>
     </row>
@@ -1217,12 +1372,23 @@
       <c r="C22" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="J22" t="b">
-        <v>1</v>
-      </c>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="13"/>
       <c r="P22" s="6"/>
       <c r="Q22" s="11">
-        <f t="shared" si="0"/>
+        <f>C22+D22+E22+F22+G22+H22+I22+J22+K22+L22+M22+N22+O22+P22</f>
         <v>2</v>
       </c>
     </row>
@@ -1233,30 +1399,35 @@
       <c r="C23" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E23" t="b">
-        <v>1</v>
-      </c>
-      <c r="F23" t="b">
-        <v>1</v>
-      </c>
-      <c r="G23" t="b">
-        <v>1</v>
-      </c>
-      <c r="H23" t="b">
-        <v>1</v>
-      </c>
-      <c r="I23" t="b">
-        <v>1</v>
-      </c>
-      <c r="J23" t="b">
-        <v>1</v>
-      </c>
+      <c r="D23" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E23" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F23" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G23" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H23" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I23" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="J23" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="13"/>
       <c r="P23" s="6"/>
       <c r="Q23" s="11">
-        <f t="shared" si="0"/>
+        <f>C23+D23+E23+F23+G23+H23+I23+J23+K23+L23+M23+N23+O23+P23</f>
         <v>8</v>
       </c>
     </row>
@@ -1265,15 +1436,25 @@
         <v>33</v>
       </c>
       <c r="C24" s="5"/>
-      <c r="D24" t="b">
-        <v>1</v>
-      </c>
-      <c r="J24" t="b">
-        <v>1</v>
-      </c>
+      <c r="D24" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="13"/>
+      <c r="N24" s="13"/>
+      <c r="O24" s="13"/>
       <c r="P24" s="6"/>
       <c r="Q24" s="11">
-        <f t="shared" si="0"/>
+        <f>C24+D24+E24+F24+G24+H24+I24+J24+K24+L24+M24+N24+O24+P24</f>
         <v>2</v>
       </c>
     </row>
@@ -1282,15 +1463,25 @@
         <v>52</v>
       </c>
       <c r="C25" s="5"/>
-      <c r="F25" t="b">
-        <v>1</v>
-      </c>
-      <c r="G25" t="b">
-        <v>1</v>
-      </c>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G25" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="13"/>
+      <c r="N25" s="13"/>
+      <c r="O25" s="13"/>
       <c r="P25" s="6"/>
       <c r="Q25" s="11">
-        <f t="shared" si="0"/>
+        <f>C25+D25+E25+F25+G25+H25+I25+J25+K25+L25+M25+N25+O25+P25</f>
         <v>2</v>
       </c>
     </row>
@@ -1301,30 +1492,35 @@
       <c r="C26" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D26" t="b">
-        <v>1</v>
-      </c>
-      <c r="E26" t="b">
-        <v>1</v>
-      </c>
-      <c r="F26" t="b">
-        <v>1</v>
-      </c>
-      <c r="G26" t="b">
-        <v>1</v>
-      </c>
-      <c r="H26" t="b">
-        <v>1</v>
-      </c>
-      <c r="I26" t="b">
-        <v>1</v>
-      </c>
-      <c r="J26" t="b">
-        <v>1</v>
-      </c>
+      <c r="D26" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E26" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F26" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G26" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H26" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I26" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="J26" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="13"/>
+      <c r="N26" s="13"/>
+      <c r="O26" s="13"/>
       <c r="P26" s="6"/>
       <c r="Q26" s="11">
-        <f t="shared" si="0"/>
+        <f>C26+D26+E26+F26+G26+H26+I26+J26+K26+L26+M26+N26+O26+P26</f>
         <v>8</v>
       </c>
     </row>
@@ -1335,12 +1531,23 @@
       <c r="C27" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="J27" t="b">
-        <v>1</v>
-      </c>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="13"/>
+      <c r="O27" s="13"/>
       <c r="P27" s="6"/>
       <c r="Q27" s="11">
-        <f t="shared" si="0"/>
+        <f>C27+D27+E27+F27+G27+H27+I27+J27+K27+L27+M27+N27+O27+P27</f>
         <v>2</v>
       </c>
     </row>
@@ -1351,24 +1558,31 @@
       <c r="C28" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D28" t="b">
-        <v>1</v>
-      </c>
-      <c r="E28" t="b">
-        <v>1</v>
-      </c>
-      <c r="G28" t="b">
-        <v>1</v>
-      </c>
-      <c r="H28" t="b">
-        <v>1</v>
-      </c>
-      <c r="J28" t="b">
-        <v>1</v>
-      </c>
+      <c r="D28" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E28" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H28" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="13"/>
+      <c r="N28" s="13"/>
+      <c r="O28" s="13"/>
       <c r="P28" s="6"/>
       <c r="Q28" s="11">
-        <f t="shared" si="0"/>
+        <f>C28+D28+E28+F28+G28+H28+I28+J28+K28+L28+M28+N28+O28+P28</f>
         <v>6</v>
       </c>
     </row>
@@ -1379,330 +1593,459 @@
       <c r="C29" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D29" t="b">
-        <v>1</v>
-      </c>
-      <c r="E29" t="b">
-        <v>1</v>
-      </c>
-      <c r="F29" t="b">
-        <v>1</v>
-      </c>
-      <c r="G29" t="b">
-        <v>1</v>
-      </c>
-      <c r="H29" t="b">
-        <v>1</v>
-      </c>
-      <c r="J29" t="b">
-        <v>1</v>
-      </c>
+      <c r="D29" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E29" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F29" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G29" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H29" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13"/>
+      <c r="M29" s="13"/>
+      <c r="N29" s="13"/>
+      <c r="O29" s="13"/>
       <c r="P29" s="6"/>
       <c r="Q29" s="11">
-        <f t="shared" si="0"/>
+        <f>C29+D29+E29+F29+G29+H29+I29+J29+K29+L29+M29+N29+O29+P29</f>
         <v>7</v>
       </c>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B30" s="10" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="C30" s="5"/>
-      <c r="D30" t="b">
-        <v>1</v>
-      </c>
-      <c r="E30" t="b">
-        <v>1</v>
-      </c>
-      <c r="G30" t="b">
-        <v>1</v>
-      </c>
-      <c r="H30" t="b">
-        <v>1</v>
-      </c>
-      <c r="I30" t="b">
-        <v>1</v>
-      </c>
-      <c r="J30" t="b">
-        <v>1</v>
-      </c>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13"/>
+      <c r="M30" s="13"/>
+      <c r="N30" s="13"/>
+      <c r="O30" s="13"/>
       <c r="P30" s="6"/>
       <c r="Q30" s="11">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f>C30+D30+E30+F30+G30+H30+I30+J30+K30+L30+M30+N30+O30+P30</f>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B31" s="10" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="C31" s="5"/>
-      <c r="D31" t="b">
-        <v>1</v>
-      </c>
-      <c r="E31" t="b">
-        <v>1</v>
-      </c>
-      <c r="F31" t="b">
-        <v>1</v>
-      </c>
-      <c r="H31" t="b">
-        <v>1</v>
-      </c>
-      <c r="I31" t="b">
-        <v>1</v>
-      </c>
+      <c r="D31" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E31" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H31" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I31" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="J31" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
+      <c r="M31" s="13"/>
+      <c r="N31" s="13"/>
+      <c r="O31" s="13"/>
       <c r="P31" s="6"/>
       <c r="Q31" s="11">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f>C31+D31+E31+F31+G31+H31+I31+J31+K31+L31+M31+N31+O31+P31</f>
+        <v>6</v>
       </c>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B32" s="10" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="C32" s="5"/>
-      <c r="D32" t="b">
-        <v>1</v>
-      </c>
-      <c r="G32" t="b">
-        <v>1</v>
-      </c>
-      <c r="H32" t="b">
-        <v>1</v>
-      </c>
-      <c r="J32" t="b">
-        <v>1</v>
-      </c>
+      <c r="D32" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E32" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F32" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I32" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="J32" s="13"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="13"/>
+      <c r="N32" s="13"/>
+      <c r="O32" s="13"/>
       <c r="P32" s="6"/>
       <c r="Q32" s="11">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f>C32+D32+E32+F32+G32+H32+I32+J32+K32+L32+M32+N32+O32+P32</f>
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B33" s="10" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="C33" s="5"/>
-      <c r="D33" t="b">
-        <v>1</v>
-      </c>
-      <c r="E33" t="b">
-        <v>1</v>
-      </c>
-      <c r="G33" t="b">
-        <v>1</v>
-      </c>
+      <c r="D33" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H33" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I33" s="13"/>
+      <c r="J33" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K33" s="13"/>
+      <c r="L33" s="13"/>
+      <c r="M33" s="13"/>
+      <c r="N33" s="13"/>
+      <c r="O33" s="13"/>
       <c r="P33" s="6"/>
       <c r="Q33" s="11">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>C33+D33+E33+F33+G33+H33+I33+J33+K33+L33+M33+N33+O33+P33</f>
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B34" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C34" s="5"/>
-      <c r="D34" t="b">
-        <v>1</v>
-      </c>
+      <c r="D34" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E34" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="13"/>
+      <c r="M34" s="13"/>
+      <c r="N34" s="13"/>
+      <c r="O34" s="13"/>
       <c r="P34" s="6"/>
       <c r="Q34" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>C34+D34+E34+F34+G34+H34+I34+J34+K34+L34+M34+N34+O34+P34</f>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B35" s="10" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="C35" s="5"/>
-      <c r="D35" t="b">
-        <v>1</v>
-      </c>
+      <c r="D35" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="13"/>
+      <c r="K35" s="13"/>
+      <c r="L35" s="13"/>
+      <c r="M35" s="13"/>
+      <c r="N35" s="13"/>
+      <c r="O35" s="13"/>
       <c r="P35" s="6"/>
       <c r="Q35" s="11">
-        <f t="shared" si="0"/>
+        <f>C35+D35+E35+F35+G35+H35+I35+J35+K35+L35+M35+N35+O35+P35</f>
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B36" s="10" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C36" s="5"/>
-      <c r="D36" t="b">
-        <v>1</v>
-      </c>
+      <c r="D36" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="13"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
+      <c r="M36" s="13"/>
+      <c r="N36" s="13"/>
+      <c r="O36" s="13"/>
       <c r="P36" s="6"/>
       <c r="Q36" s="11">
-        <f t="shared" si="0"/>
+        <f>C36+D36+E36+F36+G36+H36+I36+J36+K36+L36+M36+N36+O36+P36</f>
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B37" s="10" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C37" s="5"/>
-      <c r="D37" t="b">
-        <v>1</v>
-      </c>
-      <c r="E37" t="b">
-        <v>1</v>
-      </c>
-      <c r="F37" t="b">
-        <v>1</v>
-      </c>
-      <c r="G37" t="b">
-        <v>1</v>
-      </c>
-      <c r="H37" t="b">
-        <v>1</v>
-      </c>
-      <c r="I37" t="b">
-        <v>1</v>
-      </c>
-      <c r="J37" t="b">
-        <v>1</v>
-      </c>
+      <c r="D37" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13"/>
+      <c r="K37" s="13"/>
+      <c r="L37" s="13"/>
+      <c r="M37" s="13"/>
+      <c r="N37" s="13"/>
+      <c r="O37" s="13"/>
       <c r="P37" s="6"/>
       <c r="Q37" s="11">
-        <f t="shared" si="0"/>
-        <v>7</v>
+        <f>C37+D37+E37+F37+G37+H37+I37+J37+K37+L37+M37+N37+O37+P37</f>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B38" s="10" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C38" s="5"/>
-      <c r="D38" t="b">
-        <v>1</v>
-      </c>
-      <c r="E38" t="b">
-        <v>1</v>
-      </c>
-      <c r="F38" t="b">
-        <v>1</v>
-      </c>
-      <c r="G38" t="b">
-        <v>1</v>
-      </c>
-      <c r="H38" t="b">
-        <v>1</v>
-      </c>
-      <c r="I38" t="b">
-        <v>1</v>
-      </c>
-      <c r="J38" t="b">
-        <v>1</v>
-      </c>
+      <c r="D38" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E38" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F38" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G38" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H38" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I38" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="J38" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K38" s="13"/>
+      <c r="L38" s="13"/>
+      <c r="M38" s="13"/>
+      <c r="N38" s="13"/>
+      <c r="O38" s="13"/>
       <c r="P38" s="6"/>
       <c r="Q38" s="11">
-        <f t="shared" si="0"/>
+        <f>C38+D38+E38+F38+G38+H38+I38+J38+K38+L38+M38+N38+O38+P38</f>
         <v>7</v>
       </c>
     </row>
     <row r="39" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B39" s="10" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C39" s="5"/>
-      <c r="D39" t="b">
-        <v>1</v>
-      </c>
-      <c r="E39" t="b">
-        <v>1</v>
-      </c>
-      <c r="F39" t="b">
-        <v>1</v>
-      </c>
-      <c r="G39" t="b">
-        <v>1</v>
-      </c>
-      <c r="H39" t="b">
-        <v>1</v>
-      </c>
+      <c r="D39" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E39" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F39" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G39" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H39" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I39" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="J39" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K39" s="13"/>
+      <c r="L39" s="13"/>
+      <c r="M39" s="13"/>
+      <c r="N39" s="13"/>
+      <c r="O39" s="13"/>
       <c r="P39" s="6"/>
       <c r="Q39" s="11">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f>C39+D39+E39+F39+G39+H39+I39+J39+K39+L39+M39+N39+O39+P39</f>
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B40" s="10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C40" s="5"/>
-      <c r="D40" t="b">
-        <v>1</v>
-      </c>
-      <c r="E40" t="b">
-        <v>1</v>
-      </c>
-      <c r="G40" t="b">
-        <v>1</v>
-      </c>
-      <c r="H40" t="b">
-        <v>1</v>
-      </c>
-      <c r="J40" t="b">
-        <v>1</v>
-      </c>
+      <c r="D40" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E40" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F40" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G40" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H40" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I40" s="13"/>
+      <c r="J40" s="13"/>
+      <c r="K40" s="13"/>
+      <c r="L40" s="13"/>
+      <c r="M40" s="13"/>
+      <c r="N40" s="13"/>
+      <c r="O40" s="13"/>
       <c r="P40" s="6"/>
       <c r="Q40" s="11">
-        <f t="shared" si="0"/>
+        <f>C40+D40+E40+F40+G40+H40+I40+J40+K40+L40+M40+N40+O40+P40</f>
         <v>5</v>
       </c>
     </row>
     <row r="41" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B41" s="10" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C41" s="5"/>
-      <c r="E41" t="b">
-        <v>1</v>
-      </c>
+      <c r="D41" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E41" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H41" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I41" s="13"/>
+      <c r="J41" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K41" s="13"/>
+      <c r="L41" s="13"/>
+      <c r="M41" s="13"/>
+      <c r="N41" s="13"/>
+      <c r="O41" s="13"/>
       <c r="P41" s="6"/>
       <c r="Q41" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>C41+D41+E41+F41+G41+H41+I41+J41+K41+L41+M41+N41+O41+P41</f>
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B42" s="13" t="s">
+      <c r="B42" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C42" s="5"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F42" s="13"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
+      <c r="I42" s="13"/>
+      <c r="J42" s="13"/>
+      <c r="K42" s="13"/>
+      <c r="L42" s="13"/>
+      <c r="M42" s="13"/>
+      <c r="N42" s="13"/>
+      <c r="O42" s="13"/>
+      <c r="P42" s="6"/>
+      <c r="Q42" s="11">
+        <f>C42+D42+E42+F42+G42+H42+I42+J42+K42+L42+M42+N42+O42+P42</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B43" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C42" s="7"/>
-      <c r="D42" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="E42" s="8"/>
-      <c r="F42" s="8"/>
-      <c r="G42" s="8"/>
-      <c r="H42" s="8"/>
-      <c r="I42" s="8"/>
-      <c r="J42" s="8"/>
-      <c r="K42" s="8"/>
-      <c r="L42" s="8"/>
-      <c r="M42" s="8"/>
-      <c r="N42" s="8"/>
-      <c r="O42" s="8"/>
-      <c r="P42" s="9"/>
-      <c r="Q42" s="11">
-        <f t="shared" si="0"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
+      <c r="J43" s="8"/>
+      <c r="K43" s="8"/>
+      <c r="L43" s="8"/>
+      <c r="M43" s="8"/>
+      <c r="N43" s="8"/>
+      <c r="O43" s="8"/>
+      <c r="P43" s="9"/>
+      <c r="Q43" s="11">
+        <f>C43+D43+E43+F43+G43+H43+I43+J43+K43+L43+M43+N43+O43+P43</f>
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:Q42">
-    <sortCondition ref="B3:B42"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:Q43">
+    <sortCondition ref="B43"/>
   </sortState>
-  <conditionalFormatting sqref="Q3:Q42">
+  <conditionalFormatting sqref="Q3:Q43">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
       <formula>4</formula>
     </cfRule>

</xml_diff>

<commit_message>
am adaugat navigare intre pagini
</commit_message>
<xml_diff>
--- a/Prezenta.xlsx
+++ b/Prezenta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\AlgoritmiFundamentali_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D83D0C0-5901-49AC-89D1-5A87ECE6BCB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CFFA125-E15C-4DBC-A64E-B8F04E986D07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -391,7 +391,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -411,7 +411,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -703,7 +702,7 @@
   <dimension ref="B2:Q43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -788,15 +787,17 @@
       <c r="J3" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="K3" s="3"/>
+      <c r="K3" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="11">
-        <f>C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
-        <v>7</v>
+        <f t="shared" ref="Q3:Q43" si="0">C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.3">
@@ -804,26 +805,19 @@
         <v>55</v>
       </c>
       <c r="C4" s="5"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="J4" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
+      <c r="I4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" t="b">
+        <v>1</v>
+      </c>
+      <c r="K4" t="b">
+        <v>1</v>
+      </c>
       <c r="P4" s="6"/>
       <c r="Q4" s="11">
-        <f>C4+D4+E4+F4+G4+H4+I4+J4+K4+L4+M4+N4+O4+P4</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.3">
@@ -831,26 +825,19 @@
         <v>53</v>
       </c>
       <c r="C5" s="5"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="J5" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
+      <c r="I5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K5" t="b">
+        <v>1</v>
+      </c>
       <c r="P5" s="6"/>
       <c r="Q5" s="11">
-        <f>C5+D5+E5+F5+G5+H5+I5+J5+K5+L5+M5+N5+O5+P5</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.3">
@@ -858,23 +845,12 @@
         <v>35</v>
       </c>
       <c r="C6" s="5"/>
-      <c r="D6" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
       <c r="P6" s="6"/>
       <c r="Q6" s="11">
-        <f>C6+D6+E6+F6+G6+H6+I6+J6+K6+L6+M6+N6+O6+P6</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -883,33 +859,27 @@
         <v>51</v>
       </c>
       <c r="C7" s="5"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F7" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G7" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H7" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I7" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="J7" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" t="b">
+        <v>1</v>
+      </c>
+      <c r="I7" t="b">
+        <v>1</v>
+      </c>
+      <c r="J7" t="b">
+        <v>1</v>
+      </c>
       <c r="P7" s="6"/>
       <c r="Q7" s="11">
-        <f>C7+D7+E7+F7+G7+H7+I7+J7+K7+L7+M7+N7+O7+P7</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
@@ -918,23 +888,12 @@
         <v>46</v>
       </c>
       <c r="C8" s="5"/>
-      <c r="D8" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13"/>
+      <c r="D8" t="b">
+        <v>1</v>
+      </c>
       <c r="P8" s="6"/>
       <c r="Q8" s="11">
-        <f>C8+D8+E8+F8+G8+H8+I8+J8+K8+L8+M8+N8+O8+P8</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -943,31 +902,24 @@
         <v>36</v>
       </c>
       <c r="C9" s="5"/>
-      <c r="D9" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E9" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F9" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G9" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="13"/>
+      <c r="D9" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9" t="b">
+        <v>1</v>
+      </c>
+      <c r="I9" t="b">
+        <v>1</v>
+      </c>
       <c r="P9" s="6"/>
       <c r="Q9" s="11">
-        <f>C9+D9+E9+F9+G9+H9+I9+J9+K9+L9+M9+N9+O9+P9</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -976,23 +928,12 @@
         <v>40</v>
       </c>
       <c r="C10" s="5"/>
-      <c r="D10" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13"/>
+      <c r="D10" t="b">
+        <v>1</v>
+      </c>
       <c r="P10" s="6"/>
       <c r="Q10" s="11">
-        <f>C10+D10+E10+F10+G10+H10+I10+J10+K10+L10+M10+N10+O10+P10</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1001,25 +942,15 @@
         <v>44</v>
       </c>
       <c r="C11" s="5"/>
-      <c r="D11" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="13"/>
+      <c r="D11" t="b">
+        <v>1</v>
+      </c>
+      <c r="J11" t="b">
+        <v>1</v>
+      </c>
       <c r="P11" s="6"/>
       <c r="Q11" s="11">
-        <f>C11+D11+E11+F11+G11+H11+I11+J11+K11+L11+M11+N11+O11+P11</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -1028,32 +959,28 @@
         <v>43</v>
       </c>
       <c r="C12" s="5"/>
-      <c r="D12" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E12" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F12" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I12" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
-      <c r="N12" s="13"/>
-      <c r="O12" s="13"/>
+      <c r="D12" t="b">
+        <v>1</v>
+      </c>
+      <c r="E12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I12" t="b">
+        <v>1</v>
+      </c>
+      <c r="K12" t="b">
+        <v>1</v>
+      </c>
       <c r="P12" s="6"/>
       <c r="Q12" s="11">
-        <f>C12+D12+E12+F12+G12+H12+I12+J12+K12+L12+M12+N12+O12+P12</f>
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.3">
@@ -1063,31 +990,24 @@
       <c r="C13" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D13" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E13" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F13" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G13" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
-      <c r="O13" s="13"/>
+      <c r="D13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13" t="b">
+        <v>1</v>
+      </c>
+      <c r="J13" t="b">
+        <v>1</v>
+      </c>
       <c r="P13" s="6"/>
       <c r="Q13" s="11">
-        <f>C13+D13+E13+F13+G13+H13+I13+J13+K13+L13+M13+N13+O13+P13</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
@@ -1098,32 +1018,28 @@
       <c r="C14" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D14" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E14" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F14" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="J14" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
-      <c r="N14" s="13"/>
-      <c r="O14" s="13"/>
+      <c r="D14" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14" t="b">
+        <v>1</v>
+      </c>
+      <c r="F14" t="b">
+        <v>1</v>
+      </c>
+      <c r="I14" t="b">
+        <v>1</v>
+      </c>
+      <c r="J14" t="b">
+        <v>1</v>
+      </c>
+      <c r="K14" t="b">
+        <v>1</v>
+      </c>
       <c r="P14" s="6"/>
       <c r="Q14" s="11">
-        <f>C14+D14+E14+F14+G14+H14+I14+J14+K14+L14+M14+N14+O14+P14</f>
-        <v>6</v>
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.3">
@@ -1133,30 +1049,25 @@
       <c r="C15" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D15" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="13"/>
-      <c r="O15" s="13"/>
+      <c r="D15" t="b">
+        <v>1</v>
+      </c>
+      <c r="F15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H15" t="b">
+        <v>1</v>
+      </c>
+      <c r="J15" t="b">
+        <v>1</v>
+      </c>
+      <c r="K15" t="b">
+        <v>1</v>
+      </c>
       <c r="P15" s="6"/>
       <c r="Q15" s="11">
-        <f>C15+D15+E15+F15+G15+H15+I15+J15+K15+L15+M15+N15+O15+P15</f>
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.3">
@@ -1166,31 +1077,24 @@
       <c r="C16" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D16" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E16" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F16" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G16" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H16" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="13"/>
-      <c r="N16" s="13"/>
-      <c r="O16" s="13"/>
+      <c r="D16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16" t="b">
+        <v>1</v>
+      </c>
       <c r="P16" s="6"/>
       <c r="Q16" s="11">
-        <f>C16+D16+E16+F16+G16+H16+I16+J16+K16+L16+M16+N16+O16+P16</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
@@ -1201,36 +1105,34 @@
       <c r="C17" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D17" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E17" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F17" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G17" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H17" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I17" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="J17" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="13"/>
-      <c r="O17" s="13"/>
+      <c r="D17" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17" t="b">
+        <v>1</v>
+      </c>
+      <c r="F17" t="b">
+        <v>1</v>
+      </c>
+      <c r="G17" t="b">
+        <v>1</v>
+      </c>
+      <c r="H17" t="b">
+        <v>1</v>
+      </c>
+      <c r="I17" t="b">
+        <v>1</v>
+      </c>
+      <c r="J17" t="b">
+        <v>1</v>
+      </c>
+      <c r="K17" t="b">
+        <v>1</v>
+      </c>
       <c r="P17" s="6"/>
       <c r="Q17" s="11">
-        <f>C17+D17+E17+F17+G17+H17+I17+J17+K17+L17+M17+N17+O17+P17</f>
-        <v>8</v>
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.3">
@@ -1240,31 +1142,24 @@
       <c r="C18" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D18" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E18" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F18" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G18" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
-      <c r="N18" s="13"/>
-      <c r="O18" s="13"/>
+      <c r="D18" t="b">
+        <v>1</v>
+      </c>
+      <c r="E18" t="b">
+        <v>1</v>
+      </c>
+      <c r="F18" t="b">
+        <v>1</v>
+      </c>
+      <c r="G18" t="b">
+        <v>1</v>
+      </c>
+      <c r="J18" t="b">
+        <v>1</v>
+      </c>
       <c r="P18" s="6"/>
       <c r="Q18" s="11">
-        <f>C18+D18+E18+F18+G18+H18+I18+J18+K18+L18+M18+N18+O18+P18</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
@@ -1275,26 +1170,19 @@
       <c r="C19" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
-      <c r="N19" s="13"/>
-      <c r="O19" s="13"/>
+      <c r="F19" t="b">
+        <v>1</v>
+      </c>
+      <c r="H19" t="b">
+        <v>1</v>
+      </c>
+      <c r="K19" t="b">
+        <v>1</v>
+      </c>
       <c r="P19" s="6"/>
       <c r="Q19" s="11">
-        <f>C19+D19+E19+F19+G19+H19+I19+J19+K19+L19+M19+N19+O19+P19</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.3">
@@ -1304,33 +1192,27 @@
       <c r="C20" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D20" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E20" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F20" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G20" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H20" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="13"/>
-      <c r="O20" s="13"/>
+      <c r="D20" t="b">
+        <v>1</v>
+      </c>
+      <c r="E20" t="b">
+        <v>1</v>
+      </c>
+      <c r="F20" t="b">
+        <v>1</v>
+      </c>
+      <c r="G20" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20" t="b">
+        <v>1</v>
+      </c>
+      <c r="J20" t="b">
+        <v>1</v>
+      </c>
       <c r="P20" s="6"/>
       <c r="Q20" s="11">
-        <f>C20+D20+E20+F20+G20+H20+I20+J20+K20+L20+M20+N20+O20+P20</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
@@ -1341,27 +1223,18 @@
       <c r="C21" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D21" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
-      <c r="N21" s="13"/>
-      <c r="O21" s="13"/>
+      <c r="D21" t="b">
+        <v>1</v>
+      </c>
+      <c r="F21" t="b">
+        <v>1</v>
+      </c>
+      <c r="J21" t="b">
+        <v>1</v>
+      </c>
       <c r="P21" s="6"/>
       <c r="Q21" s="11">
-        <f>C21+D21+E21+F21+G21+H21+I21+J21+K21+L21+M21+N21+O21+P21</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -1372,23 +1245,12 @@
       <c r="C22" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
-      <c r="O22" s="13"/>
+      <c r="J22" t="b">
+        <v>1</v>
+      </c>
       <c r="P22" s="6"/>
       <c r="Q22" s="11">
-        <f>C22+D22+E22+F22+G22+H22+I22+J22+K22+L22+M22+N22+O22+P22</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -1399,36 +1261,34 @@
       <c r="C23" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D23" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E23" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F23" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G23" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H23" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I23" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="J23" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
-      <c r="O23" s="13"/>
+      <c r="D23" t="b">
+        <v>1</v>
+      </c>
+      <c r="E23" t="b">
+        <v>1</v>
+      </c>
+      <c r="F23" t="b">
+        <v>1</v>
+      </c>
+      <c r="G23" t="b">
+        <v>1</v>
+      </c>
+      <c r="H23" t="b">
+        <v>1</v>
+      </c>
+      <c r="I23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J23" t="b">
+        <v>1</v>
+      </c>
+      <c r="K23" t="b">
+        <v>1</v>
+      </c>
       <c r="P23" s="6"/>
       <c r="Q23" s="11">
-        <f>C23+D23+E23+F23+G23+H23+I23+J23+K23+L23+M23+N23+O23+P23</f>
-        <v>8</v>
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.3">
@@ -1436,26 +1296,19 @@
         <v>33</v>
       </c>
       <c r="C24" s="5"/>
-      <c r="D24" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="K24" s="13"/>
-      <c r="L24" s="13"/>
-      <c r="M24" s="13"/>
-      <c r="N24" s="13"/>
-      <c r="O24" s="13"/>
+      <c r="D24" t="b">
+        <v>1</v>
+      </c>
+      <c r="J24" t="b">
+        <v>1</v>
+      </c>
+      <c r="K24" t="b">
+        <v>1</v>
+      </c>
       <c r="P24" s="6"/>
       <c r="Q24" s="11">
-        <f>C24+D24+E24+F24+G24+H24+I24+J24+K24+L24+M24+N24+O24+P24</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.3">
@@ -1463,25 +1316,15 @@
         <v>52</v>
       </c>
       <c r="C25" s="5"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G25" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="13"/>
-      <c r="N25" s="13"/>
-      <c r="O25" s="13"/>
+      <c r="F25" t="b">
+        <v>1</v>
+      </c>
+      <c r="G25" t="b">
+        <v>1</v>
+      </c>
       <c r="P25" s="6"/>
       <c r="Q25" s="11">
-        <f>C25+D25+E25+F25+G25+H25+I25+J25+K25+L25+M25+N25+O25+P25</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -1492,35 +1335,30 @@
       <c r="C26" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D26" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E26" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F26" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G26" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H26" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I26" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="J26" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="K26" s="13"/>
-      <c r="L26" s="13"/>
-      <c r="M26" s="13"/>
-      <c r="N26" s="13"/>
-      <c r="O26" s="13"/>
+      <c r="D26" t="b">
+        <v>1</v>
+      </c>
+      <c r="E26" t="b">
+        <v>1</v>
+      </c>
+      <c r="F26" t="b">
+        <v>1</v>
+      </c>
+      <c r="G26" t="b">
+        <v>1</v>
+      </c>
+      <c r="H26" t="b">
+        <v>1</v>
+      </c>
+      <c r="I26" t="b">
+        <v>1</v>
+      </c>
+      <c r="J26" t="b">
+        <v>1</v>
+      </c>
       <c r="P26" s="6"/>
       <c r="Q26" s="11">
-        <f>C26+D26+E26+F26+G26+H26+I26+J26+K26+L26+M26+N26+O26+P26</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
@@ -1531,24 +1369,16 @@
       <c r="C27" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="K27" s="13"/>
-      <c r="L27" s="13"/>
-      <c r="M27" s="13"/>
-      <c r="N27" s="13"/>
-      <c r="O27" s="13"/>
+      <c r="J27" t="b">
+        <v>1</v>
+      </c>
+      <c r="K27" t="b">
+        <v>1</v>
+      </c>
       <c r="P27" s="6"/>
       <c r="Q27" s="11">
-        <f>C27+D27+E27+F27+G27+H27+I27+J27+K27+L27+M27+N27+O27+P27</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.3">
@@ -1558,31 +1388,24 @@
       <c r="C28" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D28" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E28" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H28" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I28" s="13"/>
-      <c r="J28" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="K28" s="13"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="13"/>
-      <c r="N28" s="13"/>
-      <c r="O28" s="13"/>
+      <c r="D28" t="b">
+        <v>1</v>
+      </c>
+      <c r="E28" t="b">
+        <v>1</v>
+      </c>
+      <c r="G28" t="b">
+        <v>1</v>
+      </c>
+      <c r="H28" t="b">
+        <v>1</v>
+      </c>
+      <c r="J28" t="b">
+        <v>1</v>
+      </c>
       <c r="P28" s="6"/>
       <c r="Q28" s="11">
-        <f>C28+D28+E28+F28+G28+H28+I28+J28+K28+L28+M28+N28+O28+P28</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
@@ -1593,33 +1416,27 @@
       <c r="C29" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D29" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E29" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F29" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G29" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H29" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I29" s="13"/>
-      <c r="J29" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="K29" s="13"/>
-      <c r="L29" s="13"/>
-      <c r="M29" s="13"/>
-      <c r="N29" s="13"/>
-      <c r="O29" s="13"/>
+      <c r="D29" t="b">
+        <v>1</v>
+      </c>
+      <c r="E29" t="b">
+        <v>1</v>
+      </c>
+      <c r="F29" t="b">
+        <v>1</v>
+      </c>
+      <c r="G29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H29" t="b">
+        <v>1</v>
+      </c>
+      <c r="J29" t="b">
+        <v>1</v>
+      </c>
       <c r="P29" s="6"/>
       <c r="Q29" s="11">
-        <f>C29+D29+E29+F29+G29+H29+I29+J29+K29+L29+M29+N29+O29+P29</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
@@ -1628,23 +1445,12 @@
         <v>56</v>
       </c>
       <c r="C30" s="5"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="13"/>
-      <c r="J30" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="K30" s="13"/>
-      <c r="L30" s="13"/>
-      <c r="M30" s="13"/>
-      <c r="N30" s="13"/>
-      <c r="O30" s="13"/>
+      <c r="J30" t="b">
+        <v>1</v>
+      </c>
       <c r="P30" s="6"/>
       <c r="Q30" s="11">
-        <f>C30+D30+E30+F30+G30+H30+I30+J30+K30+L30+M30+N30+O30+P30</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1653,34 +1459,31 @@
         <v>34</v>
       </c>
       <c r="C31" s="5"/>
-      <c r="D31" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E31" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H31" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I31" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="J31" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="K31" s="13"/>
-      <c r="L31" s="13"/>
-      <c r="M31" s="13"/>
-      <c r="N31" s="13"/>
-      <c r="O31" s="13"/>
+      <c r="D31" t="b">
+        <v>1</v>
+      </c>
+      <c r="E31" t="b">
+        <v>1</v>
+      </c>
+      <c r="G31" t="b">
+        <v>1</v>
+      </c>
+      <c r="H31" t="b">
+        <v>1</v>
+      </c>
+      <c r="I31" t="b">
+        <v>1</v>
+      </c>
+      <c r="J31" t="b">
+        <v>1</v>
+      </c>
+      <c r="K31" t="b">
+        <v>1</v>
+      </c>
       <c r="P31" s="6"/>
       <c r="Q31" s="11">
-        <f>C31+D31+E31+F31+G31+H31+I31+J31+K31+L31+M31+N31+O31+P31</f>
-        <v>6</v>
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.3">
@@ -1688,32 +1491,28 @@
         <v>54</v>
       </c>
       <c r="C32" s="5"/>
-      <c r="D32" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E32" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F32" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I32" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="J32" s="13"/>
-      <c r="K32" s="13"/>
-      <c r="L32" s="13"/>
-      <c r="M32" s="13"/>
-      <c r="N32" s="13"/>
-      <c r="O32" s="13"/>
+      <c r="D32" t="b">
+        <v>1</v>
+      </c>
+      <c r="E32" t="b">
+        <v>1</v>
+      </c>
+      <c r="F32" t="b">
+        <v>1</v>
+      </c>
+      <c r="H32" t="b">
+        <v>1</v>
+      </c>
+      <c r="I32" t="b">
+        <v>1</v>
+      </c>
+      <c r="K32" t="b">
+        <v>1</v>
+      </c>
       <c r="P32" s="6"/>
       <c r="Q32" s="11">
-        <f>C32+D32+E32+F32+G32+H32+I32+J32+K32+L32+M32+N32+O32+P32</f>
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="2:17" x14ac:dyDescent="0.3">
@@ -1721,29 +1520,21 @@
         <v>42</v>
       </c>
       <c r="C33" s="5"/>
-      <c r="D33" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H33" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I33" s="13"/>
-      <c r="J33" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="K33" s="13"/>
-      <c r="L33" s="13"/>
-      <c r="M33" s="13"/>
-      <c r="N33" s="13"/>
-      <c r="O33" s="13"/>
+      <c r="D33" t="b">
+        <v>1</v>
+      </c>
+      <c r="G33" t="b">
+        <v>1</v>
+      </c>
+      <c r="H33" t="b">
+        <v>1</v>
+      </c>
+      <c r="J33" t="b">
+        <v>1</v>
+      </c>
       <c r="P33" s="6"/>
       <c r="Q33" s="11">
-        <f>C33+D33+E33+F33+G33+H33+I33+J33+K33+L33+M33+N33+O33+P33</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -1752,27 +1543,18 @@
         <v>31</v>
       </c>
       <c r="C34" s="5"/>
-      <c r="D34" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E34" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H34" s="13"/>
-      <c r="I34" s="13"/>
-      <c r="J34" s="13"/>
-      <c r="K34" s="13"/>
-      <c r="L34" s="13"/>
-      <c r="M34" s="13"/>
-      <c r="N34" s="13"/>
-      <c r="O34" s="13"/>
+      <c r="D34" t="b">
+        <v>1</v>
+      </c>
+      <c r="E34" t="b">
+        <v>1</v>
+      </c>
+      <c r="G34" t="b">
+        <v>1</v>
+      </c>
       <c r="P34" s="6"/>
       <c r="Q34" s="11">
-        <f>C34+D34+E34+F34+G34+H34+I34+J34+K34+L34+M34+N34+O34+P34</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -1781,23 +1563,12 @@
         <v>32</v>
       </c>
       <c r="C35" s="5"/>
-      <c r="D35" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="13"/>
-      <c r="J35" s="13"/>
-      <c r="K35" s="13"/>
-      <c r="L35" s="13"/>
-      <c r="M35" s="13"/>
-      <c r="N35" s="13"/>
-      <c r="O35" s="13"/>
+      <c r="D35" t="b">
+        <v>1</v>
+      </c>
       <c r="P35" s="6"/>
       <c r="Q35" s="11">
-        <f>C35+D35+E35+F35+G35+H35+I35+J35+K35+L35+M35+N35+O35+P35</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1806,23 +1577,12 @@
         <v>47</v>
       </c>
       <c r="C36" s="5"/>
-      <c r="D36" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="13"/>
-      <c r="I36" s="13"/>
-      <c r="J36" s="13"/>
-      <c r="K36" s="13"/>
-      <c r="L36" s="13"/>
-      <c r="M36" s="13"/>
-      <c r="N36" s="13"/>
-      <c r="O36" s="13"/>
+      <c r="D36" t="b">
+        <v>1</v>
+      </c>
       <c r="P36" s="6"/>
       <c r="Q36" s="11">
-        <f>C36+D36+E36+F36+G36+H36+I36+J36+K36+L36+M36+N36+O36+P36</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1831,23 +1591,12 @@
         <v>45</v>
       </c>
       <c r="C37" s="5"/>
-      <c r="D37" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="13"/>
-      <c r="I37" s="13"/>
-      <c r="J37" s="13"/>
-      <c r="K37" s="13"/>
-      <c r="L37" s="13"/>
-      <c r="M37" s="13"/>
-      <c r="N37" s="13"/>
-      <c r="O37" s="13"/>
+      <c r="D37" t="b">
+        <v>1</v>
+      </c>
       <c r="P37" s="6"/>
       <c r="Q37" s="11">
-        <f>C37+D37+E37+F37+G37+H37+I37+J37+K37+L37+M37+N37+O37+P37</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1856,36 +1605,34 @@
         <v>39</v>
       </c>
       <c r="C38" s="5"/>
-      <c r="D38" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E38" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F38" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G38" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H38" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I38" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="J38" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="K38" s="13"/>
-      <c r="L38" s="13"/>
-      <c r="M38" s="13"/>
-      <c r="N38" s="13"/>
-      <c r="O38" s="13"/>
+      <c r="D38" t="b">
+        <v>1</v>
+      </c>
+      <c r="E38" t="b">
+        <v>1</v>
+      </c>
+      <c r="F38" t="b">
+        <v>1</v>
+      </c>
+      <c r="G38" t="b">
+        <v>1</v>
+      </c>
+      <c r="H38" t="b">
+        <v>1</v>
+      </c>
+      <c r="I38" t="b">
+        <v>1</v>
+      </c>
+      <c r="J38" t="b">
+        <v>1</v>
+      </c>
+      <c r="K38" t="b">
+        <v>1</v>
+      </c>
       <c r="P38" s="6"/>
       <c r="Q38" s="11">
-        <f>C38+D38+E38+F38+G38+H38+I38+J38+K38+L38+M38+N38+O38+P38</f>
-        <v>7</v>
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
     </row>
     <row r="39" spans="2:17" x14ac:dyDescent="0.3">
@@ -1893,35 +1640,30 @@
         <v>30</v>
       </c>
       <c r="C39" s="5"/>
-      <c r="D39" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E39" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F39" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G39" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H39" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I39" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="J39" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="K39" s="13"/>
-      <c r="L39" s="13"/>
-      <c r="M39" s="13"/>
-      <c r="N39" s="13"/>
-      <c r="O39" s="13"/>
+      <c r="D39" t="b">
+        <v>1</v>
+      </c>
+      <c r="E39" t="b">
+        <v>1</v>
+      </c>
+      <c r="F39" t="b">
+        <v>1</v>
+      </c>
+      <c r="G39" t="b">
+        <v>1</v>
+      </c>
+      <c r="H39" t="b">
+        <v>1</v>
+      </c>
+      <c r="I39" t="b">
+        <v>1</v>
+      </c>
+      <c r="J39" t="b">
+        <v>1</v>
+      </c>
       <c r="P39" s="6"/>
       <c r="Q39" s="11">
-        <f>C39+D39+E39+F39+G39+H39+I39+J39+K39+L39+M39+N39+O39+P39</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
@@ -1930,31 +1672,24 @@
         <v>38</v>
       </c>
       <c r="C40" s="5"/>
-      <c r="D40" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E40" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F40" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G40" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H40" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I40" s="13"/>
-      <c r="J40" s="13"/>
-      <c r="K40" s="13"/>
-      <c r="L40" s="13"/>
-      <c r="M40" s="13"/>
-      <c r="N40" s="13"/>
-      <c r="O40" s="13"/>
+      <c r="D40" t="b">
+        <v>1</v>
+      </c>
+      <c r="E40" t="b">
+        <v>1</v>
+      </c>
+      <c r="F40" t="b">
+        <v>1</v>
+      </c>
+      <c r="G40" t="b">
+        <v>1</v>
+      </c>
+      <c r="H40" t="b">
+        <v>1</v>
+      </c>
       <c r="P40" s="6"/>
       <c r="Q40" s="11">
-        <f>C40+D40+E40+F40+G40+H40+I40+J40+K40+L40+M40+N40+O40+P40</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -1963,31 +1698,24 @@
         <v>41</v>
       </c>
       <c r="C41" s="5"/>
-      <c r="D41" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E41" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F41" s="13"/>
-      <c r="G41" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H41" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I41" s="13"/>
-      <c r="J41" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="K41" s="13"/>
-      <c r="L41" s="13"/>
-      <c r="M41" s="13"/>
-      <c r="N41" s="13"/>
-      <c r="O41" s="13"/>
+      <c r="D41" t="b">
+        <v>1</v>
+      </c>
+      <c r="E41" t="b">
+        <v>1</v>
+      </c>
+      <c r="G41" t="b">
+        <v>1</v>
+      </c>
+      <c r="H41" t="b">
+        <v>1</v>
+      </c>
+      <c r="J41" t="b">
+        <v>1</v>
+      </c>
       <c r="P41" s="6"/>
       <c r="Q41" s="11">
-        <f>C41+D41+E41+F41+G41+H41+I41+J41+K41+L41+M41+N41+O41+P41</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -1996,24 +1724,16 @@
         <v>50</v>
       </c>
       <c r="C42" s="5"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="13"/>
-      <c r="I42" s="13"/>
-      <c r="J42" s="13"/>
-      <c r="K42" s="13"/>
-      <c r="L42" s="13"/>
-      <c r="M42" s="13"/>
-      <c r="N42" s="13"/>
-      <c r="O42" s="13"/>
+      <c r="E42" t="b">
+        <v>1</v>
+      </c>
+      <c r="K42" t="b">
+        <v>1</v>
+      </c>
       <c r="P42" s="6"/>
       <c r="Q42" s="11">
-        <f>C42+D42+E42+F42+G42+H42+I42+J42+K42+L42+M42+N42+O42+P42</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="2:17" x14ac:dyDescent="0.3">
@@ -2037,7 +1757,7 @@
       <c r="O43" s="8"/>
       <c r="P43" s="9"/>
       <c r="Q43" s="11">
-        <f>C43+D43+E43+F43+G43+H43+I43+J43+K43+L43+M43+N43+O43+P43</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Laborator 02.05.2023 - navigare intre pagini si un card model pentru retete
</commit_message>
<xml_diff>
--- a/Prezenta.xlsx
+++ b/Prezenta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\AlgoritmiFundamentali_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CFFA125-E15C-4DBC-A64E-B8F04E986D07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB4AF357-E8A2-4685-A71E-C5CFDAD1A3C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -701,8 +701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1322,10 +1322,13 @@
       <c r="G25" t="b">
         <v>1</v>
       </c>
+      <c r="K25" t="b">
+        <v>1</v>
+      </c>
       <c r="P25" s="6"/>
       <c r="Q25" s="11">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.3">
@@ -1713,10 +1716,13 @@
       <c r="J41" t="b">
         <v>1</v>
       </c>
+      <c r="K41" t="b">
+        <v>1</v>
+      </c>
       <c r="P41" s="6"/>
       <c r="Q41" s="11">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="42" spans="2:17" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Laborator 04.05.2023 - Afisatul punctelor in 3D folosind o formula de proiectare la 2D
</commit_message>
<xml_diff>
--- a/Prezenta.xlsx
+++ b/Prezenta.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\AlgoritmiFundamentali_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB4AF357-E8A2-4685-A71E-C5CFDAD1A3C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A9E251C-595B-4967-ACC5-0A10EB082C89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,6 +19,17 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -701,8 +712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M34" sqref="M34"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K44" sqref="K44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1005,10 +1016,13 @@
       <c r="J13" t="b">
         <v>1</v>
       </c>
+      <c r="K13" t="b">
+        <v>1</v>
+      </c>
       <c r="P13" s="6"/>
       <c r="Q13" s="11">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.3">
@@ -1157,10 +1171,13 @@
       <c r="J18" t="b">
         <v>1</v>
       </c>
+      <c r="K18" t="b">
+        <v>1</v>
+      </c>
       <c r="P18" s="6"/>
       <c r="Q18" s="11">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.3">
@@ -1733,13 +1750,16 @@
       <c r="E42" t="b">
         <v>1</v>
       </c>
+      <c r="J42" t="b">
+        <v>1</v>
+      </c>
       <c r="K42" t="b">
         <v>1</v>
       </c>
       <c r="P42" s="6"/>
       <c r="Q42" s="11">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="2:17" x14ac:dyDescent="0.3">
@@ -1756,7 +1776,9 @@
       <c r="H43" s="8"/>
       <c r="I43" s="8"/>
       <c r="J43" s="8"/>
-      <c r="K43" s="8"/>
+      <c r="K43" s="8" t="b">
+        <v>1</v>
+      </c>
       <c r="L43" s="8"/>
       <c r="M43" s="8"/>
       <c r="N43" s="8"/>
@@ -1764,7 +1786,7 @@
       <c r="P43" s="9"/>
       <c r="Q43" s="11">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Laborator 18.05.2023 - algoritmul lui Lee pus in practica
</commit_message>
<xml_diff>
--- a/Prezenta.xlsx
+++ b/Prezenta.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\AlgoritmiFundamentali_2023\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC9EC0C3-A656-410F-B3FE-32D01B0A9F30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="22368" windowHeight="9275"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
   <si>
     <t>Nume Prenume</t>
   </si>
@@ -188,19 +194,43 @@
   </si>
   <si>
     <t>Tecsi-Murgui Renata</t>
+  </si>
+  <si>
+    <t>Proiect</t>
+  </si>
+  <si>
+    <t>Osu!</t>
+  </si>
+  <si>
+    <t>Nota</t>
+  </si>
+  <si>
+    <t>Platformer</t>
+  </si>
+  <si>
+    <t>Site Cosmetice</t>
+  </si>
+  <si>
+    <t>Site Bio</t>
+  </si>
+  <si>
+    <t>Site Pizza</t>
+  </si>
+  <si>
+    <t>Site Studenti</t>
+  </si>
+  <si>
+    <t>Twitter</t>
+  </si>
+  <si>
+    <t>FlappyBird</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="22">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -216,159 +246,8 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="36">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -377,210 +256,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.39994506668294322"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.39994506668294322"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -722,253 +415,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -988,57 +439,27 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -1053,6 +474,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1310,25 +734,26 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="B2:Q44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:S44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V20" sqref="V20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="2.66666666666667" customWidth="1"/>
-    <col min="2" max="2" width="20.8888888888889" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" customWidth="1"/>
+    <col min="18" max="18" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17">
+    <row r="2" spans="2:19">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1377,8 +802,14 @@
       <c r="Q2" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="2:17">
+      <c r="R2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="2:19">
       <c r="B3" s="3" t="s">
         <v>16</v>
       </c>
@@ -1410,16 +841,20 @@
       <c r="L3" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="M3" s="5"/>
+      <c r="M3" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
       <c r="P3" s="9"/>
       <c r="Q3" s="12">
-        <f t="shared" ref="Q3:Q43" si="0">C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="2:17">
+        <f t="shared" ref="Q3:Q44" si="0">C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
+        <v>10</v>
+      </c>
+      <c r="R3" s="13"/>
+      <c r="S3" s="14"/>
+    </row>
+    <row r="4" spans="2:19">
       <c r="B4" s="3" t="s">
         <v>17</v>
       </c>
@@ -1436,13 +871,20 @@
       <c r="L4" t="b">
         <v>1</v>
       </c>
+      <c r="M4" t="b">
+        <v>1</v>
+      </c>
       <c r="P4" s="10"/>
       <c r="Q4" s="12">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="2:17">
+        <v>5</v>
+      </c>
+      <c r="R4" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="S4" s="16"/>
+    </row>
+    <row r="5" spans="2:19">
       <c r="B5" s="3" t="s">
         <v>18</v>
       </c>
@@ -1459,13 +901,20 @@
       <c r="L5" t="b">
         <v>1</v>
       </c>
+      <c r="M5" t="b">
+        <v>1</v>
+      </c>
       <c r="P5" s="10"/>
       <c r="Q5" s="12">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="2:17">
+        <v>5</v>
+      </c>
+      <c r="R5" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="S5" s="16"/>
+    </row>
+    <row r="6" spans="2:19">
       <c r="B6" s="3" t="s">
         <v>19</v>
       </c>
@@ -1478,8 +927,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="2:17">
+      <c r="R6" s="15"/>
+      <c r="S6" s="16"/>
+    </row>
+    <row r="7" spans="2:19">
       <c r="B7" s="3" t="s">
         <v>20</v>
       </c>
@@ -1510,8 +961,10 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="2:17">
+      <c r="R7" s="15"/>
+      <c r="S7" s="16"/>
+    </row>
+    <row r="8" spans="2:19">
       <c r="B8" s="3" t="s">
         <v>21</v>
       </c>
@@ -1524,8 +977,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="2:17">
+      <c r="R8" s="15"/>
+      <c r="S8" s="16"/>
+    </row>
+    <row r="9" spans="2:19">
       <c r="B9" s="3" t="s">
         <v>22</v>
       </c>
@@ -1550,8 +1005,10 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="2:17">
+      <c r="R9" s="15"/>
+      <c r="S9" s="16"/>
+    </row>
+    <row r="10" spans="2:19">
       <c r="B10" s="3" t="s">
         <v>23</v>
       </c>
@@ -1564,8 +1021,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="2:17">
+      <c r="R10" s="15"/>
+      <c r="S10" s="16"/>
+    </row>
+    <row r="11" spans="2:19">
       <c r="B11" s="3" t="s">
         <v>24</v>
       </c>
@@ -1581,8 +1040,10 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="2:17">
+      <c r="R11" s="15"/>
+      <c r="S11" s="16"/>
+    </row>
+    <row r="12" spans="2:19">
       <c r="B12" s="3" t="s">
         <v>25</v>
       </c>
@@ -1613,8 +1074,10 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="2:17">
+      <c r="R12" s="15"/>
+      <c r="S12" s="16"/>
+    </row>
+    <row r="13" spans="2:19">
       <c r="B13" s="3" t="s">
         <v>26</v>
       </c>
@@ -1647,8 +1110,10 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="2:17">
+      <c r="R13" s="15"/>
+      <c r="S13" s="16"/>
+    </row>
+    <row r="14" spans="2:19">
       <c r="B14" s="3" t="s">
         <v>27</v>
       </c>
@@ -1676,13 +1141,20 @@
       <c r="L14" t="b">
         <v>1</v>
       </c>
+      <c r="M14" t="b">
+        <v>1</v>
+      </c>
       <c r="P14" s="10"/>
       <c r="Q14" s="12">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="2:17">
+        <v>9</v>
+      </c>
+      <c r="R14" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="S14" s="16"/>
+    </row>
+    <row r="15" spans="2:19">
       <c r="B15" s="3" t="s">
         <v>28</v>
       </c>
@@ -1709,8 +1181,10 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="2:17">
+      <c r="R15" s="15"/>
+      <c r="S15" s="16"/>
+    </row>
+    <row r="16" spans="2:19">
       <c r="B16" s="3" t="s">
         <v>29</v>
       </c>
@@ -1735,13 +1209,22 @@
       <c r="L16" t="b">
         <v>1</v>
       </c>
+      <c r="M16" t="b">
+        <v>1</v>
+      </c>
       <c r="P16" s="10"/>
       <c r="Q16" s="12">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="2:17">
+        <v>8</v>
+      </c>
+      <c r="R16" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="S16" s="16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="2:19">
       <c r="B17" s="3" t="s">
         <v>30</v>
       </c>
@@ -1780,8 +1263,10 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="2:17">
+      <c r="R17" s="15"/>
+      <c r="S17" s="16"/>
+    </row>
+    <row r="18" spans="2:19">
       <c r="B18" s="3" t="s">
         <v>31</v>
       </c>
@@ -1809,13 +1294,18 @@
       <c r="L18" t="b">
         <v>1</v>
       </c>
+      <c r="M18" t="b">
+        <v>1</v>
+      </c>
       <c r="P18" s="10"/>
       <c r="Q18" s="12">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="2:17">
+        <v>9</v>
+      </c>
+      <c r="R18" s="15"/>
+      <c r="S18" s="16"/>
+    </row>
+    <row r="19" spans="2:19">
       <c r="B19" s="3" t="s">
         <v>32</v>
       </c>
@@ -1836,8 +1326,10 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="2:17">
+      <c r="R19" s="15"/>
+      <c r="S19" s="16"/>
+    </row>
+    <row r="20" spans="2:19">
       <c r="B20" s="3" t="s">
         <v>33</v>
       </c>
@@ -1865,13 +1357,22 @@
       <c r="L20" t="b">
         <v>1</v>
       </c>
+      <c r="M20" t="b">
+        <v>1</v>
+      </c>
       <c r="P20" s="10"/>
       <c r="Q20" s="12">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="2:17">
+        <v>9</v>
+      </c>
+      <c r="R20" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="S20" s="16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="2:19">
       <c r="B21" s="3" t="s">
         <v>34</v>
       </c>
@@ -1892,8 +1393,10 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="2:17">
+      <c r="R21" s="15"/>
+      <c r="S21" s="16"/>
+    </row>
+    <row r="22" spans="2:19">
       <c r="B22" s="3" t="s">
         <v>35</v>
       </c>
@@ -1911,8 +1414,10 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="2:17">
+      <c r="R22" s="15"/>
+      <c r="S22" s="16"/>
+    </row>
+    <row r="23" spans="2:19">
       <c r="B23" s="3" t="s">
         <v>36</v>
       </c>
@@ -1951,8 +1456,10 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="2:17">
+      <c r="R23" s="15"/>
+      <c r="S23" s="16"/>
+    </row>
+    <row r="24" spans="2:19">
       <c r="B24" s="3" t="s">
         <v>37</v>
       </c>
@@ -1974,8 +1481,10 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="25" spans="2:17">
+      <c r="R24" s="15"/>
+      <c r="S24" s="16"/>
+    </row>
+    <row r="25" spans="2:19">
       <c r="B25" s="3" t="s">
         <v>38</v>
       </c>
@@ -1994,8 +1503,10 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="26" spans="2:17">
+      <c r="R25" s="15"/>
+      <c r="S25" s="16"/>
+    </row>
+    <row r="26" spans="2:19">
       <c r="B26" s="3" t="s">
         <v>39</v>
       </c>
@@ -2026,13 +1537,20 @@
       <c r="L26" t="b">
         <v>1</v>
       </c>
+      <c r="M26" t="b">
+        <v>1</v>
+      </c>
       <c r="P26" s="10"/>
       <c r="Q26" s="12">
         <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="2:17">
+        <v>10</v>
+      </c>
+      <c r="R26" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="S26" s="16"/>
+    </row>
+    <row r="27" spans="2:19">
       <c r="B27" s="3" t="s">
         <v>40</v>
       </c>
@@ -2053,8 +1571,10 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="2:17">
+      <c r="R27" s="15"/>
+      <c r="S27" s="16"/>
+    </row>
+    <row r="28" spans="2:19">
       <c r="B28" s="3" t="s">
         <v>41</v>
       </c>
@@ -2081,8 +1601,10 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="29" spans="2:17">
+      <c r="R28" s="15"/>
+      <c r="S28" s="16"/>
+    </row>
+    <row r="29" spans="2:19">
       <c r="B29" s="3" t="s">
         <v>42</v>
       </c>
@@ -2115,8 +1637,10 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="30" spans="2:17">
+      <c r="R29" s="15"/>
+      <c r="S29" s="16"/>
+    </row>
+    <row r="30" spans="2:19">
       <c r="B30" s="3" t="s">
         <v>43</v>
       </c>
@@ -2129,8 +1653,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="2:17">
+      <c r="R30" s="15"/>
+      <c r="S30" s="16"/>
+    </row>
+    <row r="31" spans="2:19">
       <c r="B31" s="3" t="s">
         <v>44</v>
       </c>
@@ -2164,8 +1690,10 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="32" spans="2:17">
+      <c r="R31" s="15"/>
+      <c r="S31" s="16"/>
+    </row>
+    <row r="32" spans="2:19">
       <c r="B32" s="3" t="s">
         <v>45</v>
       </c>
@@ -2196,8 +1724,10 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="33" spans="2:17">
+      <c r="R32" s="15"/>
+      <c r="S32" s="16"/>
+    </row>
+    <row r="33" spans="2:19">
       <c r="B33" s="3" t="s">
         <v>46</v>
       </c>
@@ -2219,8 +1749,10 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="34" spans="2:17">
+      <c r="R33" s="15"/>
+      <c r="S33" s="16"/>
+    </row>
+    <row r="34" spans="2:19">
       <c r="B34" s="3" t="s">
         <v>47</v>
       </c>
@@ -2239,8 +1771,10 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="35" spans="2:17">
+      <c r="R34" s="15"/>
+      <c r="S34" s="16"/>
+    </row>
+    <row r="35" spans="2:19">
       <c r="B35" s="3" t="s">
         <v>48</v>
       </c>
@@ -2253,24 +1787,31 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="2:17">
+      <c r="R35" s="15"/>
+      <c r="S35" s="16"/>
+    </row>
+    <row r="36" spans="2:19">
       <c r="B36" s="3" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="C36" s="6"/>
-      <c r="D36" t="b">
+      <c r="L36" t="b">
+        <v>1</v>
+      </c>
+      <c r="M36" t="b">
         <v>1</v>
       </c>
       <c r="P36" s="10"/>
       <c r="Q36" s="12">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="2:17">
+        <v>2</v>
+      </c>
+      <c r="R36" s="15"/>
+      <c r="S36" s="16"/>
+    </row>
+    <row r="37" spans="2:19">
       <c r="B37" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C37" s="6"/>
       <c r="D37" t="b">
@@ -2281,48 +1822,28 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="2:17">
+      <c r="R37" s="15"/>
+      <c r="S37" s="16"/>
+    </row>
+    <row r="38" spans="2:19">
       <c r="B38" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C38" s="6"/>
       <c r="D38" t="b">
         <v>1</v>
       </c>
-      <c r="E38" t="b">
-        <v>1</v>
-      </c>
-      <c r="F38" t="b">
-        <v>1</v>
-      </c>
-      <c r="G38" t="b">
-        <v>1</v>
-      </c>
-      <c r="H38" t="b">
-        <v>1</v>
-      </c>
-      <c r="I38" t="b">
-        <v>1</v>
-      </c>
-      <c r="J38" t="b">
-        <v>1</v>
-      </c>
-      <c r="K38" t="b">
-        <v>1</v>
-      </c>
-      <c r="L38" t="b">
-        <v>1</v>
-      </c>
       <c r="P38" s="10"/>
       <c r="Q38" s="12">
         <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="39" spans="2:17">
+        <v>1</v>
+      </c>
+      <c r="R38" s="15"/>
+      <c r="S38" s="16"/>
+    </row>
+    <row r="39" spans="2:19">
       <c r="B39" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C39" s="6"/>
       <c r="D39" t="b">
@@ -2346,15 +1867,28 @@
       <c r="J39" t="b">
         <v>1</v>
       </c>
+      <c r="K39" t="b">
+        <v>1</v>
+      </c>
+      <c r="L39" t="b">
+        <v>1</v>
+      </c>
+      <c r="M39" t="b">
+        <v>1</v>
+      </c>
       <c r="P39" s="10"/>
       <c r="Q39" s="12">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40" spans="2:17">
+        <v>10</v>
+      </c>
+      <c r="R39" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="S39" s="16"/>
+    </row>
+    <row r="40" spans="2:19">
       <c r="B40" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C40" s="6"/>
       <c r="D40" t="b">
@@ -2372,15 +1906,23 @@
       <c r="H40" t="b">
         <v>1</v>
       </c>
+      <c r="I40" t="b">
+        <v>1</v>
+      </c>
+      <c r="J40" t="b">
+        <v>1</v>
+      </c>
       <c r="P40" s="10"/>
       <c r="Q40" s="12">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="41" spans="2:17">
+        <v>7</v>
+      </c>
+      <c r="R40" s="15"/>
+      <c r="S40" s="16"/>
+    </row>
+    <row r="41" spans="2:19">
       <c r="B41" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C41" s="6"/>
       <c r="D41" t="b">
@@ -2389,89 +1931,116 @@
       <c r="E41" t="b">
         <v>1</v>
       </c>
+      <c r="F41" t="b">
+        <v>1</v>
+      </c>
       <c r="G41" t="b">
         <v>1</v>
       </c>
       <c r="H41" t="b">
-        <v>1</v>
-      </c>
-      <c r="J41" t="b">
-        <v>1</v>
-      </c>
-      <c r="K41" t="b">
-        <v>1</v>
-      </c>
-      <c r="L41" t="b">
         <v>1</v>
       </c>
       <c r="P41" s="10"/>
       <c r="Q41" s="12">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="42" spans="2:17">
+        <v>5</v>
+      </c>
+      <c r="R41" s="15"/>
+      <c r="S41" s="16"/>
+    </row>
+    <row r="42" spans="2:19">
       <c r="B42" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C42" s="6"/>
+      <c r="D42" t="b">
+        <v>1</v>
+      </c>
       <c r="E42" t="b">
         <v>1</v>
       </c>
+      <c r="G42" t="b">
+        <v>1</v>
+      </c>
+      <c r="H42" t="b">
+        <v>1</v>
+      </c>
       <c r="J42" t="b">
         <v>1</v>
       </c>
       <c r="K42" t="b">
+        <v>1</v>
+      </c>
+      <c r="L42" t="b">
         <v>1</v>
       </c>
       <c r="P42" s="10"/>
       <c r="Q42" s="12">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="43" spans="2:17">
+        <v>7</v>
+      </c>
+      <c r="R42" s="15"/>
+      <c r="S42" s="16"/>
+    </row>
+    <row r="43" spans="2:19">
       <c r="B43" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C43" s="6"/>
+      <c r="E43" t="b">
+        <v>1</v>
+      </c>
+      <c r="J43" t="b">
+        <v>1</v>
+      </c>
+      <c r="K43" t="b">
+        <v>1</v>
+      </c>
+      <c r="M43" t="b">
+        <v>1</v>
+      </c>
+      <c r="P43" s="10"/>
+      <c r="Q43" s="12">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="R43" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="S43" s="16"/>
+    </row>
+    <row r="44" spans="2:19">
+      <c r="B44" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C43" s="7"/>
-      <c r="D43" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="E43" s="8"/>
-      <c r="F43" s="8"/>
-      <c r="G43" s="8"/>
-      <c r="H43" s="8"/>
-      <c r="I43" s="8"/>
-      <c r="J43" s="8"/>
-      <c r="K43" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="L43" s="8"/>
-      <c r="M43" s="8"/>
-      <c r="N43" s="8"/>
-      <c r="O43" s="8"/>
-      <c r="P43" s="11"/>
-      <c r="Q43" s="12">
+      <c r="C44" s="7"/>
+      <c r="D44" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="8"/>
+      <c r="J44" s="8"/>
+      <c r="K44" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="L44" s="8"/>
+      <c r="M44" s="8"/>
+      <c r="N44" s="8"/>
+      <c r="O44" s="8"/>
+      <c r="P44" s="11"/>
+      <c r="Q44" s="12">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="2:17">
-      <c r="B44" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="L44" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q44" s="12">
-        <f>C44+D44+E44+F44+G44+H44+I44+J44+K44+L44+M44+N44+O44+P44</f>
-        <v>1</v>
-      </c>
+      <c r="R44" s="17"/>
+      <c r="S44" s="18"/>
     </row>
   </sheetData>
-  <sortState ref="B3:Q43">
-    <sortCondition ref="B43"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:S44">
+    <sortCondition ref="B44"/>
   </sortState>
   <conditionalFormatting sqref="Q3:Q44">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
@@ -2479,6 +2048,5 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>